<commit_message>
Added changes from the rabbit and Yannick to the initial commits from Genevieve.
</commit_message>
<xml_diff>
--- a/localisation/references/questionnaireLocalisation.xlsx
+++ b/localisation/references/questionnaireLocalisation.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="185">
   <si>
     <t xml:space="preserve">questionName</t>
   </si>
@@ -184,6 +184,9 @@
     <t xml:space="preserve">&gt;=</t>
   </si>
   <si>
+    <t xml:space="preserve">iden</t>
+  </si>
+  <si>
     <t xml:space="preserve">abbreviation</t>
   </si>
   <si>
@@ -322,7 +325,7 @@
     <t xml:space="preserve">Cette personne s'identifie comme:</t>
   </si>
   <si>
-    <t xml:space="preserve">This person identifies  as:</t>
+    <t xml:space="preserve">This person identifies as:</t>
   </si>
   <si>
     <t xml:space="preserve">householdIncomeChoices</t>
@@ -446,9 +449,6 @@
   </si>
   <si>
     <t xml:space="preserve">refusal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I prefer not to respond</t>
   </si>
   <si>
     <t xml:space="preserve">inputRangeName</t>
@@ -596,9 +596,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -748,7 +749,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -777,6 +778,10 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -785,36 +790,40 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1134,15 +1143,18 @@
   </sheetPr>
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
+      <selection pane="bottomLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="10.91"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1219,14 +1231,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="165.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="6" t="b">
+      <c r="C2" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1259,7 +1271,7 @@
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
-      <c r="T2" s="6" t="b">
+      <c r="T2" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1267,16 +1279,16 @@
       <c r="V2" s="6"/>
       <c r="W2" s="6"/>
       <c r="X2" s="6"/>
-      <c r="Y2" s="7"/>
-    </row>
-    <row r="3" customFormat="false" ht="127.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y2" s="8"/>
+    </row>
+    <row r="3" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="6" t="b">
+      <c r="C3" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1309,7 +1321,7 @@
       <c r="Q3" s="6"/>
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
-      <c r="T3" s="6" t="b">
+      <c r="T3" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1317,16 +1329,16 @@
       <c r="V3" s="6"/>
       <c r="W3" s="6"/>
       <c r="X3" s="6"/>
-      <c r="Y3" s="7"/>
-    </row>
-    <row r="4" customFormat="false" ht="165.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y3" s="8"/>
+    </row>
+    <row r="4" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="6" t="b">
+      <c r="C4" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1359,7 +1371,7 @@
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
-      <c r="T4" s="6" t="b">
+      <c r="T4" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1367,7 +1379,7 @@
       <c r="V4" s="6"/>
       <c r="W4" s="6"/>
       <c r="X4" s="6"/>
-      <c r="Y4" s="7"/>
+      <c r="Y4" s="8"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C4">
@@ -1399,52 +1411,57 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="27.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="15.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="9" width="20.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="8" width="19.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="8" width="12.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="8" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="27.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="15.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="20.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="9" width="19.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="9" width="12.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="9" width="8.59"/>
   </cols>
   <sheetData>
-    <row r="1" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+    <row r="1" s="13" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
+    <row r="2" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="13" t="n">
+      <c r="E2" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="13"/>
+      <c r="F2" s="14"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1527,66 +1544,66 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="10.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="13" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="13" width="12.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="13" width="10.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="13" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="13" width="15.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="13" width="10.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="14" width="10.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="14" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="14" width="12.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="14" width="10.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="14" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="14" width="15.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="14" width="10.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="15" t="s">
+      <c r="B1" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="D1" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="E1" s="16" t="s">
         <v>53</v>
       </c>
+      <c r="F1" s="16" t="s">
+        <v>54</v>
+      </c>
       <c r="G1" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="H1" s="15" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
+      <c r="H1" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="8" t="b">
+      <c r="D2" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="18" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F2" s="8" t="b">
+      <c r="F2" s="18" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G2" s="8" t="b">
+      <c r="G2" s="18" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1619,603 +1636,603 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="17" width="21.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="15.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="17" width="23.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="17" width="19.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="17" width="24.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="17" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="19" width="21.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="19" width="15.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="19" width="23.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="19" width="19.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="19" width="24.29"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="19" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="18" t="s">
+      <c r="A1" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="H1" s="18" t="s">
+      <c r="G1" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="17" t="s">
-        <v>61</v>
+      <c r="I1" s="19" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="20" t="s">
+      <c r="A2" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="B2" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
+      <c r="D2" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="20" t="s">
+      <c r="A3" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="B3" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
+      <c r="D3" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="20" t="s">
+      <c r="A4" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="B4" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
+      <c r="D4" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="20" t="s">
+      <c r="A5" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="B5" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
+      <c r="D5" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="20" t="s">
+      <c r="A6" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="B6" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
+      <c r="D6" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="22"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" s="22"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="H10" s="22"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="22"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="H12" s="22"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="22"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" s="22"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="H17" s="22"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="H21" s="22"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="D30" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="C33" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="D33" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" s="20" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="C36" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20" t="s">
+      <c r="D36" s="19" t="s">
         <v>80</v>
-      </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="H8" s="20"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="H9" s="20"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="H10" s="20"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="H11" s="20"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="H12" s="20"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="H13" s="20"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="H14" s="20"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="H17" s="20"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="H21" s="20"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="D24" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="D25" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="D26" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B27" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="C27" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="D27" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B28" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="C28" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="D28" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B29" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="C29" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="D29" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B30" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="C30" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="D30" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B31" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="C31" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="D31" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B32" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="C32" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="D32" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B33" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="C33" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="D33" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="1048485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2332,207 +2349,207 @@
       <selection pane="topLeft" activeCell="M19" activeCellId="0" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="23" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="23" width="12.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="23" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="23" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="23" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="23" width="11.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="23" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="23" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="25" width="18.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="13.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="25" width="12.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="25" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="25" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="25" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="25" width="11.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="25" width="13.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="25" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="24" t="s">
+    <row r="1" s="27" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="27" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="28" t="s">
         <v>152</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="28" t="s">
         <v>153</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="28" t="s">
         <v>154</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="28" t="s">
         <v>156</v>
       </c>
-      <c r="H2" s="26" t="n">
+      <c r="H2" s="28" t="n">
         <v>-10</v>
       </c>
-      <c r="I2" s="26" t="n">
+      <c r="I2" s="28" t="n">
         <v>100</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="L2" s="26" t="s">
+      <c r="L2" s="28" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="28" t="s">
         <v>159</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="28" t="s">
         <v>165</v>
       </c>
-      <c r="H3" s="26" t="n">
+      <c r="H3" s="28" t="n">
         <v>-10</v>
       </c>
-      <c r="I3" s="26" t="n">
+      <c r="I3" s="28" t="n">
         <v>100</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J3" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="K3" s="26" t="s">
+      <c r="K3" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="L3" s="26" t="s">
+      <c r="L3" s="28" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="28" t="s">
         <v>169</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="28" t="s">
         <v>172</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="28" t="s">
         <v>173</v>
       </c>
-      <c r="H4" s="26" t="n">
+      <c r="H4" s="28" t="n">
         <v>-10</v>
       </c>
-      <c r="I4" s="26" t="n">
+      <c r="I4" s="28" t="n">
         <v>100</v>
       </c>
-      <c r="J4" s="26" t="s">
+      <c r="J4" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="K4" s="26" t="s">
+      <c r="K4" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="L4" s="26" t="s">
+      <c r="L4" s="28" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="28" t="s">
         <v>163</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="H5" s="26" t="n">
+      <c r="H5" s="28" t="n">
         <v>-10</v>
       </c>
-      <c r="I5" s="26" t="n">
+      <c r="I5" s="28" t="n">
         <v>100</v>
       </c>
-      <c r="J5" s="26" t="s">
+      <c r="J5" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="K5" s="26" t="s">
+      <c r="K5" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="L5" s="26" t="s">
+      <c r="L5" s="28" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2557,21 +2574,21 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="16.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="23" width="33.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="23" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="25" width="16.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="25" width="33.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="25" width="16.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
+    <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="25" t="s">
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -2588,10 +2605,10 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="25" t="s">
         <v>179</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -2603,17 +2620,17 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
+    <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="14" t="s">
         <v>184</v>
       </c>
       <c r="E3" s="3"/>

</xml_diff>

<commit_message>
Add address info section
Re-arranges the sections that were already made, and adds a section to input info for the two addresses we want to compare, including the location and living costs of each.
</commit_message>
<xml_diff>
--- a/localisation/references/questionnaireLocalisation.xlsx
+++ b/localisation/references/questionnaireLocalisation.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="314">
   <si>
     <t xml:space="preserve">questionName</t>
   </si>
@@ -127,19 +127,22 @@
     <t xml:space="preserve">householdSizeValidation</t>
   </si>
   <si>
-    <t xml:space="preserve">home_income</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number</t>
+    <t xml:space="preserve">household_income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select</t>
   </si>
   <si>
     <t xml:space="preserve">household.income</t>
   </si>
   <si>
-    <t xml:space="preserve">**Revenu du ménage** avant impôts (brut), en dollars Canadiens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**Household income** before taxes (gross income), in Canadian dollars</t>
+    <t xml:space="preserve">**Tranche de revenu** avant impôts (brut) **du ménage**, en 2024?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What was your **household's income range** before taxes (gross income), in 2024?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">householdIncomeChoices</t>
   </si>
   <si>
     <t xml:space="preserve">household_carNumber</t>
@@ -154,109 +157,196 @@
   </si>
   <si>
     <t xml:space="preserve">min=0
-max=5
+max=3
 overMaxAllowed</t>
   </si>
   <si>
     <t xml:space="preserve">carNumberValidation</t>
   </si>
   <si>
-    <t xml:space="preserve">home_ownership</t>
+    <t xml:space="preserve">home_save</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NextButton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enregistrer et continuer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Save and continue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addressesInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Custom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addresses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addressName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nom ou adresse de la maison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name or address of the home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optionalValidation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addressGeography</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geography</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Veuillez positionner la maison sur la carte
+__Naviguez, zoomez, et cliquez sur la carte pour localiser le lieu. Une fois localisé, vous pourrez déplacer le point pour davantage de précision. Vous pouvez également chercher le lieu en utilisant le nom ou l'adresse avec le bouton ci-dessous.__</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please locate the home on the map
+__Pan, zoom and click on map. Once a pin icon has been dropped, you will be able to drag the icon to specify a more precise location. You can also search for a place using its name or address with the button below.__</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Custom because of the map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addressOwnership</t>
   </si>
   <si>
     <t xml:space="preserve">Radio</t>
   </si>
   <si>
-    <t xml:space="preserve">**Louez-vous ou possédez-vous** cette maison?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**Do you own or rent** this home?</t>
+    <t xml:space="preserve">ownership</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comptez-vous **acheter ou louer** cette maison?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you plan to **buy or rent** this home?</t>
   </si>
   <si>
     <t xml:space="preserve">householdOwnershipChoices</t>
   </si>
   <si>
-    <t xml:space="preserve">home_address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**Adresse**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**Address**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">home_city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**Ville** ou **municipalité**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**City** or **municipality**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">home_region</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**Province**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">home_country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**Pays**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**Country**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hiddenWithCanadaAsDefaultValueCustomConditional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">home_postalCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**Code postal**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**Postal Code**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">formatter=canadianPostalCodeFormatter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalCodeValidation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">home_geography</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Custom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**Positionnement de votre domicile**
-Recherchez votre domicile en utilisant son code postal ou son adresse en cliquant sur le bouton ci-dessous, ou veuillez positionner le lieu sur la carte en naviguant, zoomant et cliquant. Une fois le lieu localisé, vous pouvez déplacer le point pour plus de précision.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**Positioning your home**
-Search for your home using its postal code or address by clicking the button below, or please position the location on the map by navigating, zooming, and clicking. Once the location is found, you can move the point for greater precision.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">home_save</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NextButton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enregistrer et continuer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Save and continue</t>
+    <t xml:space="preserve">addressRent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Prix du loyer par mois**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Monthly cost of rent**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifOwnershipTypeIsRentCustomConditional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addressAreUtilitiesIncluded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">areUtilitiesIncluded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Le prix des services publics** (électricité, gaz, ...) **est-il inclus dans le loyer?**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Is the cost of utilities** (electricity, gas, ...) **included in the rent?**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yesNo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addressMortgage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mortgage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Montant du prêt hypothécaire**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Mortgage amount**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifOwnershipTypeIsBuyCustomConditional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addressInterestRate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interestRate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Taux d'intérêt du prêt hypothécaire**, en %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Mortgage interest rate**, in %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interestRateCustomValidation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We need a custom widget to input decimal numbers, which is important for an interest rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addressAmortizationPeriod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amortizationPeriod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Période d'amortissement du prêt hypothécaire**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Amortization period of the mortgage**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amortizationYearsCustomChoices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We add custom choices so we don’t have to write 30 choices for each year in the excel document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addressTaxes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taxes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Montant annuel des taxes municipales et scolaires**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Annual cost of municipal and school taxes**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addressUtilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">utilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Montant mensuel des services publics** (électricité, gaz, ...)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Monthly cost of utilities** (electricity, gas, ...)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">askForUtilitiesCustomConditional</t>
   </si>
   <si>
     <t xml:space="preserve">householdMembers</t>
@@ -331,9 +421,6 @@
     <t xml:space="preserve">carCategoryChoices</t>
   </si>
   <si>
-    <t xml:space="preserve">The car categories choices  are taken from: https://carcosts.caa.ca/</t>
-  </si>
-  <si>
     <t xml:space="preserve">carEngineType</t>
   </si>
   <si>
@@ -365,48 +452,12 @@
     <t xml:space="preserve">parentheses</t>
   </si>
   <si>
-    <t xml:space="preserve">hasHouseholdBicycleConditional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">household.bicycleNumber</t>
+    <t xml:space="preserve">${currentPerson}.age</t>
   </si>
   <si>
     <t xml:space="preserve">&gt;=</t>
   </si>
   <si>
-    <t xml:space="preserve">hasHouseholdSizeBeenAnswered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">household.size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">!==</t>
-  </si>
-  <si>
-    <t xml:space="preserve">null</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${currentPerson}.age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifOwnershipTypeIsRent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">home.ownership</t>
-  </si>
-  <si>
-    <t xml:space="preserve">===</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifOwnershipTypeIsOwn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">own</t>
-  </si>
-  <si>
     <t xml:space="preserve">abbreviation</t>
   </si>
   <si>
@@ -437,6 +488,15 @@
     <t xml:space="preserve">Home</t>
   </si>
   <si>
+    <t xml:space="preserve">ad_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adresses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Addresses</t>
+  </si>
+  <si>
     <t xml:space="preserve">hh_</t>
   </si>
   <si>
@@ -518,9 +578,6 @@
     <t xml:space="preserve">I prefer not to answer</t>
   </si>
   <si>
-    <t xml:space="preserve">yesNo</t>
-  </si>
-  <si>
     <t xml:space="preserve">yesNoPreferNotToAnswer</t>
   </si>
   <si>
@@ -563,9 +620,6 @@
     <t xml:space="preserve">This person identifies as:</t>
   </si>
   <si>
-    <t xml:space="preserve">householdIncomeChoices</t>
-  </si>
-  <si>
     <t xml:space="preserve">000000_009999</t>
   </si>
   <si>
@@ -683,19 +737,34 @@
     <t xml:space="preserve">$200,000 and more</t>
   </si>
   <si>
+    <t xml:space="preserve">Je ne sais pas (notez que la précision des résultats pourrait être affectée)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I don't know (note that the accuracy of the results may be affected)</t>
+  </si>
+  <si>
     <t xml:space="preserve">refusal</t>
   </si>
   <si>
+    <t xml:space="preserve">Je préfère ne pas répondre (notez que la précision des résultats pourrait être affectée)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I prefer not to answer (note that the accuracy of the results may be affected)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Louer</t>
   </si>
   <si>
     <t xml:space="preserve">Rent</t>
   </si>
   <si>
-    <t xml:space="preserve">Posséder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Own</t>
+    <t xml:space="preserve">buy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acheter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buy</t>
   </si>
   <si>
     <t xml:space="preserve">passengerCar</t>
@@ -918,12 +987,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
-    <numFmt numFmtId="166" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="&quot;VRAI&quot;;&quot;VRAI&quot;;&quot;FAUX&quot;"/>
+    <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="168" formatCode="@"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -970,13 +1041,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -997,6 +1061,20 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1121,7 +1199,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1166,11 +1244,15 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1178,47 +1260,35 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1226,23 +1296,43 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1250,19 +1340,15 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1270,7 +1356,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1278,23 +1364,19 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1653,14 +1735,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:XFD19"/>
+  <dimension ref="A1:XFD30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
-      <selection pane="bottomRight" activeCell="O19" activeCellId="0" sqref="O19"/>
+      <selection pane="bottomLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="bottomRight" activeCell="L8" activeCellId="0" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1832,7 +1914,9 @@
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
+      <c r="O3" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
@@ -1849,7 +1933,7 @@
     </row>
     <row r="4" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>26</v>
@@ -1867,20 +1951,20 @@
         <v>household.carNumber</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
@@ -1897,169 +1981,143 @@
       <c r="X4" s="7"/>
       <c r="Y4" s="9"/>
     </row>
-    <row r="5" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="7" t="s">
+    <row r="5" s="15" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="8" t="n">
+      <c r="B5" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7" t="str">
+      <c r="E5" s="13"/>
+      <c r="F5" s="14" t="str">
         <f aca="false">REPLACE(A5, FIND("_", A5), 1, ".")</f>
-        <v>home.ownership</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" s="7" t="s">
+        <v>home.save</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="10" t="s">
+      <c r="H5" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7" t="n">
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="9"/>
-    </row>
-    <row r="6" s="9" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
+      <c r="U5" s="13"/>
+      <c r="V5" s="13"/>
+      <c r="W5" s="13"/>
+      <c r="X5" s="13"/>
+      <c r="XEE5" s="1"/>
+      <c r="XEF5" s="1"/>
+      <c r="XEG5" s="1"/>
+      <c r="XEH5" s="1"/>
+      <c r="XEI5" s="1"/>
+      <c r="XEJ5" s="1"/>
+      <c r="XEK5" s="1"/>
+      <c r="XEL5" s="1"/>
+      <c r="XEM5" s="1"/>
+      <c r="XEN5" s="1"/>
+      <c r="XEO5" s="1"/>
+      <c r="XEP5" s="1"/>
+      <c r="XEQ5" s="1"/>
+      <c r="XER5" s="1"/>
+      <c r="XES5" s="1"/>
+      <c r="XET5" s="1"/>
+      <c r="XEU5" s="1"/>
+      <c r="XEV5" s="1"/>
+      <c r="XEW5" s="1"/>
+      <c r="XEX5" s="1"/>
+      <c r="XEY5" s="1"/>
+      <c r="XEZ5" s="1"/>
+      <c r="XFA5" s="1"/>
+      <c r="XFB5" s="1"/>
+      <c r="XFC5" s="1"/>
+      <c r="XFD5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="16" t="s">
         <v>48</v>
       </c>
       <c r="C6" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7" t="str">
-        <f aca="false">REPLACE(A6, FIND("_", A6), 1, ".")</f>
-        <v>home.address</v>
-      </c>
-      <c r="G6" s="7" t="s">
+      <c r="D6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
       <c r="T6" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
-      <c r="XEE6" s="1"/>
-      <c r="XEF6" s="1"/>
-      <c r="XEG6" s="1"/>
-      <c r="XEH6" s="1"/>
-      <c r="XEI6" s="1"/>
-      <c r="XEJ6" s="1"/>
-      <c r="XEK6" s="1"/>
-      <c r="XEL6" s="1"/>
-      <c r="XEM6" s="1"/>
-      <c r="XEN6" s="1"/>
-      <c r="XEO6" s="1"/>
-      <c r="XEP6" s="1"/>
-      <c r="XEQ6" s="1"/>
-      <c r="XER6" s="1"/>
-      <c r="XES6" s="1"/>
-      <c r="XET6" s="1"/>
-      <c r="XEU6" s="1"/>
-      <c r="XEV6" s="1"/>
-      <c r="XEW6" s="1"/>
-      <c r="XEX6" s="1"/>
-      <c r="XEY6" s="1"/>
-      <c r="XEZ6" s="1"/>
-      <c r="XFA6" s="1"/>
-      <c r="XFB6" s="1"/>
-      <c r="XFC6" s="1"/>
-      <c r="XFD6" s="1"/>
-    </row>
-    <row r="7" s="9" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
+    </row>
+    <row r="7" s="9" customFormat="true" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="8" t="b">
+      <c r="C7" s="19" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7" t="str">
-        <f aca="false">REPLACE(A7, FIND("_", A7), 1, ".")</f>
-        <v>home.city</v>
+        <v>49</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="8" t="b">
+        <v>54</v>
+      </c>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="7" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
+      <c r="U7" s="20"/>
+      <c r="V7" s="20"/>
+      <c r="W7" s="20"/>
+      <c r="X7" s="20"/>
       <c r="XEE7" s="1"/>
       <c r="XEF7" s="1"/>
       <c r="XEG7" s="1"/>
@@ -2087,50 +2145,54 @@
       <c r="XFC7" s="1"/>
       <c r="XFD7" s="1"/>
     </row>
-    <row r="8" s="9" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="7" t="s">
+    <row r="8" s="9" customFormat="true" ht="96.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="8" t="b">
+      <c r="C8" s="19" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7" t="str">
-        <f aca="false">REPLACE(A8, FIND("_", A8), 1, ".")</f>
-        <v>home.region</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="8" t="b">
+        <v>49</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
-      <c r="X8" s="7"/>
+      <c r="U8" s="20"/>
+      <c r="V8" s="20"/>
+      <c r="W8" s="20"/>
+      <c r="X8" s="20"/>
+      <c r="Y8" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="XEE8" s="1"/>
       <c r="XEF8" s="1"/>
       <c r="XEG8" s="1"/>
@@ -2158,40 +2220,41 @@
       <c r="XFC8" s="1"/>
       <c r="XFD8" s="1"/>
     </row>
-    <row r="9" s="9" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="C9" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7" t="str">
-        <f aca="false">REPLACE(A9, FIND("_", A9), 1, ".")</f>
-        <v>home.country</v>
+        <v>49</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
-      <c r="M9" s="7" t="s">
-        <v>59</v>
-      </c>
+      <c r="M9" s="10"/>
       <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
+      <c r="O9" s="10" t="s">
+        <v>66</v>
+      </c>
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
@@ -2202,580 +2265,308 @@
       </c>
       <c r="U9" s="7"/>
       <c r="V9" s="7"/>
-      <c r="W9" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="W9" s="7"/>
       <c r="X9" s="7"/>
-      <c r="XEE9" s="1"/>
-      <c r="XEF9" s="1"/>
-      <c r="XEG9" s="1"/>
-      <c r="XEH9" s="1"/>
-      <c r="XEI9" s="1"/>
-      <c r="XEJ9" s="1"/>
-      <c r="XEK9" s="1"/>
-      <c r="XEL9" s="1"/>
-      <c r="XEM9" s="1"/>
-      <c r="XEN9" s="1"/>
-      <c r="XEO9" s="1"/>
-      <c r="XEP9" s="1"/>
-      <c r="XEQ9" s="1"/>
-      <c r="XER9" s="1"/>
-      <c r="XES9" s="1"/>
-      <c r="XET9" s="1"/>
-      <c r="XEU9" s="1"/>
-      <c r="XEV9" s="1"/>
-      <c r="XEW9" s="1"/>
-      <c r="XEX9" s="1"/>
-      <c r="XEY9" s="1"/>
-      <c r="XEZ9" s="1"/>
-      <c r="XFA9" s="1"/>
-      <c r="XFB9" s="1"/>
-      <c r="XFC9" s="1"/>
-      <c r="XFD9" s="1"/>
-    </row>
-    <row r="10" s="9" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>48</v>
+      <c r="Y9" s="9"/>
+    </row>
+    <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>68</v>
       </c>
       <c r="C10" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7" t="str">
-        <f aca="false">REPLACE(A10, FIND("_", A10), 1, ".")</f>
-        <v>home.postalCode</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="8" t="b">
+        <v>49</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="M10" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="O10" s="21"/>
+      <c r="T10" s="24" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
-      <c r="W10" s="7"/>
-      <c r="X10" s="7"/>
-      <c r="XEE10" s="1"/>
-      <c r="XEF10" s="1"/>
-      <c r="XEG10" s="1"/>
-      <c r="XEH10" s="1"/>
-      <c r="XEI10" s="1"/>
-      <c r="XEJ10" s="1"/>
-      <c r="XEK10" s="1"/>
-      <c r="XEL10" s="1"/>
-      <c r="XEM10" s="1"/>
-      <c r="XEN10" s="1"/>
-      <c r="XEO10" s="1"/>
-      <c r="XEP10" s="1"/>
-      <c r="XEQ10" s="1"/>
-      <c r="XER10" s="1"/>
-      <c r="XES10" s="1"/>
-      <c r="XET10" s="1"/>
-      <c r="XEU10" s="1"/>
-      <c r="XEV10" s="1"/>
-      <c r="XEW10" s="1"/>
-      <c r="XEX10" s="1"/>
-      <c r="XEY10" s="1"/>
-      <c r="XEZ10" s="1"/>
-      <c r="XFA10" s="1"/>
-      <c r="XFB10" s="1"/>
-      <c r="XFC10" s="1"/>
-      <c r="XFD10" s="1"/>
-    </row>
-    <row r="11" s="9" customFormat="true" ht="117.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>67</v>
+    </row>
+    <row r="11" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>62</v>
       </c>
       <c r="C11" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7" t="str">
-        <f aca="false">REPLACE(A11, FIND("_", A11), 1, ".")</f>
-        <v>home.geography</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7" t="b">
+        <v>49</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="M11" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="O11" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="T11" s="24" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U11" s="7"/>
-      <c r="V11" s="7"/>
-      <c r="W11" s="7"/>
-      <c r="X11" s="7"/>
-      <c r="XEE11" s="1"/>
-      <c r="XEF11" s="1"/>
-      <c r="XEG11" s="1"/>
-      <c r="XEH11" s="1"/>
-      <c r="XEI11" s="1"/>
-      <c r="XEJ11" s="1"/>
-      <c r="XEK11" s="1"/>
-      <c r="XEL11" s="1"/>
-      <c r="XEM11" s="1"/>
-      <c r="XEN11" s="1"/>
-      <c r="XEO11" s="1"/>
-      <c r="XEP11" s="1"/>
-      <c r="XEQ11" s="1"/>
-      <c r="XER11" s="1"/>
-      <c r="XES11" s="1"/>
-      <c r="XET11" s="1"/>
-      <c r="XEU11" s="1"/>
-      <c r="XEV11" s="1"/>
-      <c r="XEW11" s="1"/>
-      <c r="XEX11" s="1"/>
-      <c r="XEY11" s="1"/>
-      <c r="XEZ11" s="1"/>
-      <c r="XFA11" s="1"/>
-      <c r="XFB11" s="1"/>
-      <c r="XFC11" s="1"/>
-      <c r="XFD11" s="1"/>
-    </row>
-    <row r="12" s="16" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="13" t="b">
+    </row>
+    <row r="12" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D12" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15" t="str">
-        <f aca="false">REPLACE(A12, FIND("_", A12), 1, ".")</f>
-        <v>home.save</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="13" t="b">
+      <c r="D12" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="M12" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="O12" s="25"/>
+      <c r="T12" s="24" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U12" s="14"/>
-      <c r="V12" s="14"/>
-      <c r="W12" s="14"/>
-      <c r="X12" s="14"/>
-      <c r="XEE12" s="1"/>
-      <c r="XEF12" s="1"/>
-      <c r="XEG12" s="1"/>
-      <c r="XEH12" s="1"/>
-      <c r="XEI12" s="1"/>
-      <c r="XEJ12" s="1"/>
-      <c r="XEK12" s="1"/>
-      <c r="XEL12" s="1"/>
-      <c r="XEM12" s="1"/>
-      <c r="XEN12" s="1"/>
-      <c r="XEO12" s="1"/>
-      <c r="XEP12" s="1"/>
-      <c r="XEQ12" s="1"/>
-      <c r="XER12" s="1"/>
-      <c r="XES12" s="1"/>
-      <c r="XET12" s="1"/>
-      <c r="XEU12" s="1"/>
-      <c r="XEV12" s="1"/>
-      <c r="XEW12" s="1"/>
-      <c r="XEX12" s="1"/>
-      <c r="XEY12" s="1"/>
-      <c r="XEZ12" s="1"/>
-      <c r="XFA12" s="1"/>
-      <c r="XFB12" s="1"/>
-      <c r="XFC12" s="1"/>
-      <c r="XFD12" s="1"/>
-    </row>
-    <row r="13" s="9" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="19" t="b">
+    </row>
+    <row r="13" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D13" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="21"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="21"/>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="21"/>
-      <c r="S13" s="21"/>
-      <c r="T13" s="22" t="b">
+      <c r="D13" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="M13" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="O13" s="25"/>
+      <c r="T13" s="24" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U13" s="21"/>
-      <c r="V13" s="21"/>
-      <c r="W13" s="21"/>
-      <c r="X13" s="21"/>
-      <c r="XEE13" s="1"/>
-      <c r="XEF13" s="1"/>
-      <c r="XEG13" s="1"/>
-      <c r="XEH13" s="1"/>
-      <c r="XEI13" s="1"/>
-      <c r="XEJ13" s="1"/>
-      <c r="XEK13" s="1"/>
-      <c r="XEL13" s="1"/>
-      <c r="XEM13" s="1"/>
-      <c r="XEN13" s="1"/>
-      <c r="XEO13" s="1"/>
-      <c r="XEP13" s="1"/>
-      <c r="XEQ13" s="1"/>
-      <c r="XER13" s="1"/>
-      <c r="XES13" s="1"/>
-      <c r="XET13" s="1"/>
-      <c r="XEU13" s="1"/>
-      <c r="XEV13" s="1"/>
-      <c r="XEW13" s="1"/>
-      <c r="XEX13" s="1"/>
-      <c r="XEY13" s="1"/>
-      <c r="XEZ13" s="1"/>
-      <c r="XFA13" s="1"/>
-      <c r="XFB13" s="1"/>
-      <c r="XFC13" s="1"/>
-      <c r="XFD13" s="1"/>
-    </row>
-    <row r="14" s="9" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" s="20" t="s">
+      <c r="Y13" s="23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="22" t="b">
+      <c r="C14" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D14" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="H14" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="I14" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="J14" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="K14" s="20"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23" t="s">
+      <c r="D14" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="H14" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="K14" s="7"/>
+      <c r="M14" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="O14" s="23"/>
-      <c r="P14" s="23"/>
-      <c r="Q14" s="23"/>
-      <c r="R14" s="23"/>
-      <c r="S14" s="23"/>
-      <c r="T14" s="22" t="b">
+      <c r="O14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="T14" s="24" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U14" s="23"/>
-      <c r="V14" s="23"/>
-      <c r="W14" s="23"/>
-      <c r="X14" s="23"/>
-      <c r="XEE14" s="1"/>
-      <c r="XEF14" s="1"/>
-      <c r="XEG14" s="1"/>
-      <c r="XEH14" s="1"/>
-      <c r="XEI14" s="1"/>
-      <c r="XEJ14" s="1"/>
-      <c r="XEK14" s="1"/>
-      <c r="XEL14" s="1"/>
-      <c r="XEM14" s="1"/>
-      <c r="XEN14" s="1"/>
-      <c r="XEO14" s="1"/>
-      <c r="XEP14" s="1"/>
-      <c r="XEQ14" s="1"/>
-      <c r="XER14" s="1"/>
-      <c r="XES14" s="1"/>
-      <c r="XET14" s="1"/>
-      <c r="XEU14" s="1"/>
-      <c r="XEV14" s="1"/>
-      <c r="XEW14" s="1"/>
-      <c r="XEX14" s="1"/>
-      <c r="XEY14" s="1"/>
-      <c r="XEZ14" s="1"/>
-      <c r="XFA14" s="1"/>
-      <c r="XFB14" s="1"/>
-      <c r="XFC14" s="1"/>
-      <c r="XFD14" s="1"/>
-    </row>
-    <row r="15" s="9" customFormat="true" ht="128.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="22" t="b">
+      <c r="W14" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="Y14" s="23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D15" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="H15" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="23"/>
-      <c r="S15" s="23"/>
-      <c r="T15" s="22" t="b">
+      <c r="D15" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="H15" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K15" s="7"/>
+      <c r="M15" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="T15" s="24" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U15" s="23"/>
-      <c r="V15" s="23"/>
-      <c r="W15" s="23"/>
-      <c r="X15" s="23"/>
-      <c r="XEE15" s="1"/>
-      <c r="XEF15" s="1"/>
-      <c r="XEG15" s="1"/>
-      <c r="XEH15" s="1"/>
-      <c r="XEI15" s="1"/>
-      <c r="XEJ15" s="1"/>
-      <c r="XEK15" s="1"/>
-      <c r="XEL15" s="1"/>
-      <c r="XEM15" s="1"/>
-      <c r="XEN15" s="1"/>
-      <c r="XEO15" s="1"/>
-      <c r="XEP15" s="1"/>
-      <c r="XEQ15" s="1"/>
-      <c r="XER15" s="1"/>
-      <c r="XES15" s="1"/>
-      <c r="XET15" s="1"/>
-      <c r="XEU15" s="1"/>
-      <c r="XEV15" s="1"/>
-      <c r="XEW15" s="1"/>
-      <c r="XEX15" s="1"/>
-      <c r="XEY15" s="1"/>
-      <c r="XEZ15" s="1"/>
-      <c r="XFA15" s="1"/>
-      <c r="XFB15" s="1"/>
-      <c r="XFC15" s="1"/>
-      <c r="XFD15" s="1"/>
-    </row>
-    <row r="16" s="16" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="C16" s="13" t="b">
+    </row>
+    <row r="16" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D16" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="15" t="str">
-        <f aca="false">REPLACE(A16, FIND("_", A16), 1, ".")</f>
-        <v>household.save</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="13" t="b">
+      <c r="D16" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="M16" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="T16" s="24" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U16" s="14"/>
-      <c r="V16" s="14"/>
-      <c r="W16" s="14"/>
-      <c r="X16" s="14"/>
-      <c r="XEE16" s="1"/>
-      <c r="XEF16" s="1"/>
-      <c r="XEG16" s="1"/>
-      <c r="XEH16" s="1"/>
-      <c r="XEI16" s="1"/>
-      <c r="XEJ16" s="1"/>
-      <c r="XEK16" s="1"/>
-      <c r="XEL16" s="1"/>
-      <c r="XEM16" s="1"/>
-      <c r="XEN16" s="1"/>
-      <c r="XEO16" s="1"/>
-      <c r="XEP16" s="1"/>
-      <c r="XEQ16" s="1"/>
-      <c r="XER16" s="1"/>
-      <c r="XES16" s="1"/>
-      <c r="XET16" s="1"/>
-      <c r="XEU16" s="1"/>
-      <c r="XEV16" s="1"/>
-      <c r="XEW16" s="1"/>
-      <c r="XEX16" s="1"/>
-      <c r="XEY16" s="1"/>
-      <c r="XEZ16" s="1"/>
-      <c r="XFA16" s="1"/>
-      <c r="XFB16" s="1"/>
-      <c r="XFC16" s="1"/>
-      <c r="XFD16" s="1"/>
-    </row>
-    <row r="17" s="9" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" s="19" t="b">
+    </row>
+    <row r="17" s="9" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="24" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="27"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
+      <c r="Q17" s="27"/>
+      <c r="R17" s="27"/>
+      <c r="S17" s="27"/>
+      <c r="T17" s="24" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D17" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E17" s="24"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="21"/>
-      <c r="N17" s="21"/>
-      <c r="O17" s="21"/>
-      <c r="P17" s="21"/>
-      <c r="Q17" s="21"/>
-      <c r="R17" s="21"/>
-      <c r="S17" s="21"/>
-      <c r="T17" s="22" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U17" s="21"/>
-      <c r="V17" s="21"/>
-      <c r="W17" s="21"/>
-      <c r="X17" s="21"/>
+      <c r="U17" s="27"/>
+      <c r="V17" s="27"/>
+      <c r="W17" s="27"/>
+      <c r="X17" s="27"/>
       <c r="XEE17" s="1"/>
       <c r="XEF17" s="1"/>
       <c r="XEG17" s="1"/>
@@ -2804,55 +2595,56 @@
       <c r="XFD17" s="1"/>
     </row>
     <row r="18" s="9" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="22" t="b">
+      <c r="A18" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="24" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="I18" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="J18" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="K18" s="22"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="28"/>
+      <c r="R18" s="28"/>
+      <c r="S18" s="28"/>
+      <c r="T18" s="24" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D18" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="F18" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="G18" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="H18" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23"/>
-      <c r="O18" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="23"/>
-      <c r="R18" s="23"/>
-      <c r="S18" s="23"/>
-      <c r="T18" s="22" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U18" s="23"/>
-      <c r="V18" s="23"/>
-      <c r="W18" s="23"/>
-      <c r="X18" s="23"/>
-      <c r="Y18" s="9" t="s">
-        <v>97</v>
-      </c>
+      <c r="U18" s="28"/>
+      <c r="V18" s="28"/>
+      <c r="W18" s="28"/>
+      <c r="X18" s="28"/>
       <c r="XEE18" s="1"/>
       <c r="XEF18" s="1"/>
       <c r="XEG18" s="1"/>
@@ -2880,43 +2672,335 @@
       <c r="XFC18" s="1"/>
       <c r="XFD18" s="1"/>
     </row>
-    <row r="19" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="22" t="b">
+    <row r="19" s="9" customFormat="true" ht="128.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="24" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="N19" s="28"/>
+      <c r="O19" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="P19" s="28"/>
+      <c r="Q19" s="28"/>
+      <c r="R19" s="28"/>
+      <c r="S19" s="28"/>
+      <c r="T19" s="24" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D19" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="F19" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="H19" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="M19" s="26"/>
-      <c r="O19" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="T19" s="22" t="b">
+      <c r="U19" s="28"/>
+      <c r="V19" s="28"/>
+      <c r="W19" s="28"/>
+      <c r="X19" s="28"/>
+      <c r="XEE19" s="1"/>
+      <c r="XEF19" s="1"/>
+      <c r="XEG19" s="1"/>
+      <c r="XEH19" s="1"/>
+      <c r="XEI19" s="1"/>
+      <c r="XEJ19" s="1"/>
+      <c r="XEK19" s="1"/>
+      <c r="XEL19" s="1"/>
+      <c r="XEM19" s="1"/>
+      <c r="XEN19" s="1"/>
+      <c r="XEO19" s="1"/>
+      <c r="XEP19" s="1"/>
+      <c r="XEQ19" s="1"/>
+      <c r="XER19" s="1"/>
+      <c r="XES19" s="1"/>
+      <c r="XET19" s="1"/>
+      <c r="XEU19" s="1"/>
+      <c r="XEV19" s="1"/>
+      <c r="XEW19" s="1"/>
+      <c r="XEX19" s="1"/>
+      <c r="XEY19" s="1"/>
+      <c r="XEZ19" s="1"/>
+      <c r="XFA19" s="1"/>
+      <c r="XFB19" s="1"/>
+      <c r="XFC19" s="1"/>
+      <c r="XFD19" s="1"/>
+    </row>
+    <row r="20" s="15" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="24" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" s="13"/>
+      <c r="F20" s="14" t="str">
+        <f aca="false">REPLACE(A20, FIND("_", A20), 1, ".")</f>
+        <v>household.save</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
+      <c r="S20" s="13"/>
+      <c r="T20" s="11" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-    </row>
+      <c r="U20" s="13"/>
+      <c r="V20" s="13"/>
+      <c r="W20" s="13"/>
+      <c r="X20" s="13"/>
+      <c r="XEE20" s="1"/>
+      <c r="XEF20" s="1"/>
+      <c r="XEG20" s="1"/>
+      <c r="XEH20" s="1"/>
+      <c r="XEI20" s="1"/>
+      <c r="XEJ20" s="1"/>
+      <c r="XEK20" s="1"/>
+      <c r="XEL20" s="1"/>
+      <c r="XEM20" s="1"/>
+      <c r="XEN20" s="1"/>
+      <c r="XEO20" s="1"/>
+      <c r="XEP20" s="1"/>
+      <c r="XEQ20" s="1"/>
+      <c r="XER20" s="1"/>
+      <c r="XES20" s="1"/>
+      <c r="XET20" s="1"/>
+      <c r="XEU20" s="1"/>
+      <c r="XEV20" s="1"/>
+      <c r="XEW20" s="1"/>
+      <c r="XEX20" s="1"/>
+      <c r="XEY20" s="1"/>
+      <c r="XEZ20" s="1"/>
+      <c r="XFA20" s="1"/>
+      <c r="XFB20" s="1"/>
+      <c r="XFC20" s="1"/>
+      <c r="XFD20" s="1"/>
+    </row>
+    <row r="21" s="9" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="24" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="E21" s="29"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="27"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="27"/>
+      <c r="Q21" s="27"/>
+      <c r="R21" s="27"/>
+      <c r="S21" s="27"/>
+      <c r="T21" s="24" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U21" s="27"/>
+      <c r="V21" s="27"/>
+      <c r="W21" s="27"/>
+      <c r="X21" s="27"/>
+      <c r="XEE21" s="1"/>
+      <c r="XEF21" s="1"/>
+      <c r="XEG21" s="1"/>
+      <c r="XEH21" s="1"/>
+      <c r="XEI21" s="1"/>
+      <c r="XEJ21" s="1"/>
+      <c r="XEK21" s="1"/>
+      <c r="XEL21" s="1"/>
+      <c r="XEM21" s="1"/>
+      <c r="XEN21" s="1"/>
+      <c r="XEO21" s="1"/>
+      <c r="XEP21" s="1"/>
+      <c r="XEQ21" s="1"/>
+      <c r="XER21" s="1"/>
+      <c r="XES21" s="1"/>
+      <c r="XET21" s="1"/>
+      <c r="XEU21" s="1"/>
+      <c r="XEV21" s="1"/>
+      <c r="XEW21" s="1"/>
+      <c r="XEX21" s="1"/>
+      <c r="XEY21" s="1"/>
+      <c r="XEZ21" s="1"/>
+      <c r="XFA21" s="1"/>
+      <c r="XFB21" s="1"/>
+      <c r="XFC21" s="1"/>
+      <c r="XFD21" s="1"/>
+    </row>
+    <row r="22" s="9" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="24" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="H22" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="28"/>
+      <c r="N22" s="28"/>
+      <c r="O22" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="P22" s="28"/>
+      <c r="Q22" s="28"/>
+      <c r="R22" s="28"/>
+      <c r="S22" s="28"/>
+      <c r="T22" s="24" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U22" s="28"/>
+      <c r="V22" s="28"/>
+      <c r="W22" s="28"/>
+      <c r="X22" s="28"/>
+      <c r="XEE22" s="1"/>
+      <c r="XEF22" s="1"/>
+      <c r="XEG22" s="1"/>
+      <c r="XEH22" s="1"/>
+      <c r="XEI22" s="1"/>
+      <c r="XEJ22" s="1"/>
+      <c r="XEK22" s="1"/>
+      <c r="XEL22" s="1"/>
+      <c r="XEM22" s="1"/>
+      <c r="XEN22" s="1"/>
+      <c r="XEO22" s="1"/>
+      <c r="XEP22" s="1"/>
+      <c r="XEQ22" s="1"/>
+      <c r="XER22" s="1"/>
+      <c r="XES22" s="1"/>
+      <c r="XET22" s="1"/>
+      <c r="XEU22" s="1"/>
+      <c r="XEV22" s="1"/>
+      <c r="XEW22" s="1"/>
+      <c r="XEX22" s="1"/>
+      <c r="XEY22" s="1"/>
+      <c r="XEZ22" s="1"/>
+      <c r="XFA22" s="1"/>
+      <c r="XFB22" s="1"/>
+      <c r="XFC22" s="1"/>
+      <c r="XFD22" s="1"/>
+    </row>
+    <row r="23" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="24" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="G23" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H23" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="M23" s="17"/>
+      <c r="O23" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="T23" s="24" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <conditionalFormatting sqref="C1:C2 C4:C5">
+  <conditionalFormatting sqref="C1:C2 C8 C4 C6">
     <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("FALSE",C1)))</formula>
     </cfRule>
@@ -2924,57 +3008,38 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3">
-    <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="0">
-      <formula>NOT(ISERROR(SEARCH("FALSE",C3)))</formula>
+  <conditionalFormatting sqref="C17:C23">
+    <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="2">
+      <formula>NOT(ISERROR(SEARCH("FALSE",C17)))</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C17:C19">
-    <cfRule type="containsText" priority="6" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="2">
-      <formula>NOT(ISERROR(SEARCH("FALSE",C17)))</formula>
+  <conditionalFormatting sqref="C3 C9:C16">
+    <cfRule type="containsText" priority="6" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="0">
+      <formula>NOT(ISERROR(SEARCH("FALSE",C3)))</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:C11">
-    <cfRule type="containsText" priority="8" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="0">
-      <formula>NOT(ISERROR(SEARCH("FALSE",C7)))</formula>
+  <conditionalFormatting sqref="C5">
+    <cfRule type="containsText" priority="8" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="4">
+      <formula>NOT(ISERROR(SEARCH("FALSE",C5)))</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C12 C16">
-    <cfRule type="containsText" priority="10" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="4">
-      <formula>NOT(ISERROR(SEARCH("FALSE",C12)))</formula>
+  <conditionalFormatting sqref="C7:C8">
+    <cfRule type="containsText" priority="10" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="6">
+      <formula>NOT(ISERROR(SEARCH("FALSE",C7)))</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="11" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" priority="11" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13:C15">
-    <cfRule type="containsText" priority="12" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="2">
-      <formula>NOT(ISERROR(SEARCH("FALSE",C13)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="13" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C6:C11">
-    <cfRule type="containsText" priority="14" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="6">
-      <formula>NOT(ISERROR(SEARCH("FALSE",C6)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="Y18" r:id="rId1" display="The car categories choices  are taken from: https://carcosts.caa.ca/"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2993,110 +3058,76 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="38.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="26" width="15.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="28" width="20.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="26" width="19.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="26" width="12.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="26" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="17" width="38.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="15.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="17" width="31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="31" width="20.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="17" width="19.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="17" width="12.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="17" width="8.59"/>
   </cols>
   <sheetData>
-    <row r="1" s="31" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="C1" s="29" t="s">
+    <row r="1" s="34" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>107</v>
+      <c r="D1" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>110</v>
-      </c>
-      <c r="E2" s="26" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="D4" s="32" t="s">
-        <v>110</v>
-      </c>
-      <c r="E4" s="26" t="n">
+      <c r="A2" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" s="17" t="n">
         <v>16</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="C5" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>121</v>
-      </c>
-    </row>
+    <row r="1048386" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048387" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048388" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048389" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048390" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048391" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048392" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048393" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048394" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048395" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048396" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048397" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048398" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048399" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048400" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048401" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048402" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048403" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048404" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048405" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048406" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048407" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048408" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048409" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048410" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3285,125 +3316,171 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="10.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="26" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="12.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="26" width="10.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="26" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="26" width="15.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="26" width="10.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="17" width="10.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="17" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="17" width="12.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="17" width="10.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="17" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="17" width="15.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="17" width="10.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="35" t="s">
-        <v>122</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="E1" s="34" t="s">
-        <v>125</v>
-      </c>
-      <c r="F1" s="34" t="s">
-        <v>126</v>
+      <c r="B1" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>143</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>128</v>
+        <v>144</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>129</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>130</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="E2" s="36" t="b">
+      <c r="B2" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2" s="38" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F2" s="36" t="b">
+      <c r="F2" s="38" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G2" s="36" t="b">
+      <c r="G2" s="38" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="E3" s="36" t="b">
+    <row r="3" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="E3" s="38" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F3" s="36" t="b">
+      <c r="F3" s="38" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G3" s="36" t="b">
+      <c r="G3" s="38" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>137</v>
-      </c>
-      <c r="E4" s="36" t="b">
+      <c r="A4" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="E4" s="38" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F4" s="36" t="b">
+      <c r="F4" s="38" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G4" s="36" t="b">
+      <c r="G4" s="38" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="E5" s="38" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="38" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="38" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1048428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3551,743 +3628,757 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="29.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="19.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="27" width="30.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="27" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="27" width="24.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="27" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="29.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="19.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="30" width="30.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="30" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="30" width="24.29"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="30" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="B1" s="37" t="s">
-        <v>106</v>
-      </c>
-      <c r="C1" s="37" t="s">
+      <c r="A1" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="37" t="s">
-        <v>139</v>
-      </c>
-      <c r="H1" s="37" t="s">
+      <c r="G1" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="H1" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="27" t="s">
-        <v>140</v>
+      <c r="I1" s="30" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="39" t="s">
-        <v>141</v>
-      </c>
-      <c r="B2" s="39" t="s">
-        <v>141</v>
-      </c>
-      <c r="C2" s="39" t="s">
-        <v>142</v>
-      </c>
-      <c r="D2" s="39" t="s">
-        <v>143</v>
-      </c>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
+      <c r="A2" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="s">
-        <v>144</v>
-      </c>
-      <c r="B3" s="39" t="s">
-        <v>144</v>
-      </c>
-      <c r="C3" s="39" t="s">
-        <v>145</v>
-      </c>
-      <c r="D3" s="39" t="s">
-        <v>146</v>
-      </c>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+      <c r="A3" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39" t="s">
-        <v>147</v>
-      </c>
-      <c r="B4" s="39" t="s">
-        <v>147</v>
-      </c>
-      <c r="C4" s="39" t="s">
-        <v>148</v>
-      </c>
-      <c r="D4" s="39" t="s">
-        <v>149</v>
-      </c>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
+      <c r="A4" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="39" t="s">
-        <v>150</v>
-      </c>
-      <c r="B5" s="39" t="s">
-        <v>147</v>
-      </c>
-      <c r="C5" s="39" t="s">
-        <v>151</v>
-      </c>
-      <c r="D5" s="39" t="s">
-        <v>152</v>
-      </c>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+      <c r="A5" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="B6" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="C6" s="39" t="s">
-        <v>154</v>
-      </c>
-      <c r="D6" s="39" t="s">
-        <v>155</v>
-      </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
+      <c r="A6" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="B7" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="C7" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="D7" s="39" t="s">
-        <v>158</v>
-      </c>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
+      <c r="A7" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39" t="s">
-        <v>141</v>
-      </c>
-      <c r="H8" s="39"/>
+      <c r="A8" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="H8" s="25"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39" t="s">
-        <v>144</v>
-      </c>
-      <c r="H9" s="39"/>
+      <c r="A9" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="H9" s="25"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="H10" s="39"/>
+      <c r="A10" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" s="25"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="H11" s="39"/>
+      <c r="A11" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="H11" s="25"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39" t="s">
-        <v>141</v>
-      </c>
-      <c r="H12" s="39"/>
+      <c r="A12" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="H12" s="25"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39" t="s">
-        <v>144</v>
-      </c>
-      <c r="H13" s="39"/>
+      <c r="A13" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="H13" s="25"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="H14" s="39"/>
+      <c r="A14" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="H14" s="25"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="40" t="s">
-        <v>161</v>
-      </c>
-      <c r="B15" s="39" t="s">
-        <v>162</v>
-      </c>
-      <c r="C15" s="39" t="s">
-        <v>163</v>
-      </c>
-      <c r="D15" s="39" t="s">
-        <v>164</v>
-      </c>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
+      <c r="A15" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="40" t="s">
-        <v>161</v>
-      </c>
-      <c r="B16" s="39" t="s">
-        <v>165</v>
-      </c>
-      <c r="C16" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="D16" s="39" t="s">
-        <v>167</v>
-      </c>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
+      <c r="A16" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="40" t="s">
-        <v>161</v>
-      </c>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="H17" s="39"/>
+      <c r="A17" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="H17" s="25"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="40" t="s">
-        <v>168</v>
-      </c>
-      <c r="B18" s="39" t="s">
-        <v>162</v>
-      </c>
-      <c r="C18" s="39" t="s">
-        <v>163</v>
-      </c>
-      <c r="D18" s="39" t="s">
-        <v>169</v>
-      </c>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
+      <c r="A18" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="40" t="s">
-        <v>168</v>
-      </c>
-      <c r="B19" s="39" t="s">
-        <v>165</v>
-      </c>
-      <c r="C19" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="D19" s="39" t="s">
+      <c r="A19" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="H21" s="25"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>205</v>
+      </c>
+      <c r="C26" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>209</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="C28" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>218</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>225</v>
+      </c>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>226</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>227</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="C34" s="30" t="s">
+        <v>230</v>
+      </c>
+      <c r="D34" s="30" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="C35" s="30" t="s">
+        <v>232</v>
+      </c>
+      <c r="D35" s="30" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="30" t="s">
+        <v>234</v>
+      </c>
+      <c r="C36" s="30" t="s">
+        <v>235</v>
+      </c>
+      <c r="D36" s="30" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="30" t="s">
+        <v>237</v>
+      </c>
+      <c r="D37" s="30" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" s="30" t="s">
+        <v>239</v>
+      </c>
+      <c r="C38" s="30" t="s">
+        <v>240</v>
+      </c>
+      <c r="D38" s="30" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="B39" s="30" t="s">
+        <v>242</v>
+      </c>
+      <c r="C39" s="30" t="s">
+        <v>243</v>
+      </c>
+      <c r="D39" s="30" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="B40" s="30" t="s">
+        <v>245</v>
+      </c>
+      <c r="C40" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="D40" s="30" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="B41" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="C41" s="30" t="s">
+        <v>249</v>
+      </c>
+      <c r="D41" s="30" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="G42" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="40" t="s">
-        <v>168</v>
-      </c>
-      <c r="B20" s="39" t="s">
-        <v>171</v>
-      </c>
-      <c r="C20" s="39" t="s">
-        <v>172</v>
-      </c>
-      <c r="D20" s="39" t="s">
-        <v>173</v>
-      </c>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="40" t="s">
-        <v>168</v>
-      </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="H21" s="39"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="B22" s="27" t="s">
-        <v>175</v>
-      </c>
-      <c r="C22" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="D22" s="27" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="B23" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="C23" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="D23" s="25" t="s">
-        <v>180</v>
-      </c>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="C24" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>183</v>
-      </c>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="B25" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>186</v>
-      </c>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>189</v>
-      </c>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="B27" s="25" t="s">
-        <v>190</v>
-      </c>
-      <c r="C27" s="25" t="s">
-        <v>191</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>192</v>
-      </c>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="B28" s="25" t="s">
-        <v>193</v>
-      </c>
-      <c r="C28" s="25" t="s">
-        <v>194</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>195</v>
-      </c>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="B29" s="25" t="s">
-        <v>196</v>
-      </c>
-      <c r="C29" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="D29" s="25" t="s">
-        <v>198</v>
-      </c>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="B30" s="25" t="s">
-        <v>199</v>
-      </c>
-      <c r="C30" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="D30" s="25" t="s">
-        <v>201</v>
-      </c>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="B31" s="25" t="s">
-        <v>202</v>
-      </c>
-      <c r="C31" s="25" t="s">
-        <v>203</v>
-      </c>
-      <c r="D31" s="25" t="s">
-        <v>204</v>
-      </c>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="B32" s="25" t="s">
-        <v>205</v>
-      </c>
-      <c r="C32" s="25" t="s">
-        <v>206</v>
-      </c>
-      <c r="D32" s="25" t="s">
-        <v>207</v>
-      </c>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="B33" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="C33" s="25" t="s">
-        <v>209</v>
-      </c>
-      <c r="D33" s="25" t="s">
-        <v>210</v>
-      </c>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="B34" s="27" t="s">
-        <v>211</v>
-      </c>
-      <c r="C34" s="27" t="s">
-        <v>212</v>
-      </c>
-      <c r="D34" s="27" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="B35" s="27" t="s">
-        <v>153</v>
-      </c>
-      <c r="C35" s="27" t="s">
-        <v>154</v>
-      </c>
-      <c r="D35" s="27" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="B36" s="27" t="s">
-        <v>214</v>
-      </c>
-      <c r="C36" s="27" t="s">
-        <v>157</v>
-      </c>
-      <c r="D36" s="27" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="B37" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="C37" s="27" t="s">
-        <v>215</v>
-      </c>
-      <c r="D37" s="27" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="B38" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="C38" s="27" t="s">
-        <v>217</v>
-      </c>
-      <c r="D38" s="27" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="B39" s="27" t="s">
-        <v>219</v>
-      </c>
-      <c r="C39" s="27" t="s">
-        <v>220</v>
-      </c>
-      <c r="D39" s="27" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="B40" s="27" t="s">
-        <v>222</v>
-      </c>
-      <c r="C40" s="27" t="s">
-        <v>223</v>
-      </c>
-      <c r="D40" s="27" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="B41" s="27" t="s">
-        <v>225</v>
-      </c>
-      <c r="C41" s="27" t="s">
-        <v>226</v>
-      </c>
-      <c r="D41" s="27" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="G42" s="39" t="s">
-        <v>150</v>
-      </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="B43" s="27" t="s">
-        <v>228</v>
-      </c>
-      <c r="C43" s="27" t="s">
-        <v>229</v>
-      </c>
-      <c r="D43" s="27" t="s">
-        <v>230</v>
-      </c>
-      <c r="H43" s="26"/>
+      <c r="A43" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" s="30" t="s">
+        <v>251</v>
+      </c>
+      <c r="C43" s="30" t="s">
+        <v>252</v>
+      </c>
+      <c r="D43" s="30" t="s">
+        <v>253</v>
+      </c>
+      <c r="H43" s="17"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="B44" s="27" t="s">
-        <v>231</v>
-      </c>
-      <c r="C44" s="27" t="s">
-        <v>232</v>
-      </c>
-      <c r="D44" s="27" t="s">
-        <v>233</v>
-      </c>
-      <c r="H44" s="26"/>
+      <c r="A44" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="B44" s="30" t="s">
+        <v>254</v>
+      </c>
+      <c r="C44" s="30" t="s">
+        <v>255</v>
+      </c>
+      <c r="D44" s="30" t="s">
+        <v>256</v>
+      </c>
+      <c r="H44" s="17"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="B45" s="27" t="s">
-        <v>234</v>
-      </c>
-      <c r="C45" s="27" t="s">
-        <v>235</v>
-      </c>
-      <c r="D45" s="27" t="s">
-        <v>236</v>
-      </c>
-      <c r="H45" s="26"/>
+      <c r="A45" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="B45" s="30" t="s">
+        <v>257</v>
+      </c>
+      <c r="C45" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="D45" s="30" t="s">
+        <v>259</v>
+      </c>
+      <c r="H45" s="17"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="B46" s="27" t="s">
-        <v>237</v>
-      </c>
-      <c r="C46" s="27" t="s">
-        <v>238</v>
-      </c>
-      <c r="D46" s="27" t="s">
-        <v>239</v>
-      </c>
-      <c r="H46" s="26"/>
-    </row>
+      <c r="A46" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="B46" s="30" t="s">
+        <v>260</v>
+      </c>
+      <c r="C46" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="D46" s="30" t="s">
+        <v>262</v>
+      </c>
+      <c r="H46" s="17"/>
+    </row>
+    <row r="1048398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4472,7 +4563,7 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4489,65 +4580,65 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="24.39"/>
   </cols>
   <sheetData>
-    <row r="1" s="42" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="41" t="s">
-        <v>240</v>
-      </c>
-      <c r="B1" s="41" t="s">
-        <v>241</v>
-      </c>
-      <c r="C1" s="41" t="s">
-        <v>242</v>
-      </c>
-      <c r="D1" s="41" t="s">
-        <v>243</v>
-      </c>
-      <c r="E1" s="41" t="s">
-        <v>244</v>
-      </c>
-      <c r="F1" s="41" t="s">
-        <v>245</v>
-      </c>
-      <c r="G1" s="41" t="s">
-        <v>246</v>
-      </c>
-      <c r="H1" s="41" t="s">
-        <v>247</v>
-      </c>
-      <c r="I1" s="41" t="s">
-        <v>248</v>
-      </c>
-      <c r="J1" s="41" t="s">
-        <v>249</v>
-      </c>
-      <c r="K1" s="41" t="s">
-        <v>250</v>
-      </c>
-      <c r="L1" s="42" t="s">
-        <v>251</v>
+    <row r="1" s="43" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="42" t="s">
+        <v>263</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>264</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>266</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>267</v>
+      </c>
+      <c r="F1" s="42" t="s">
+        <v>268</v>
+      </c>
+      <c r="G1" s="42" t="s">
+        <v>269</v>
+      </c>
+      <c r="H1" s="42" t="s">
+        <v>270</v>
+      </c>
+      <c r="I1" s="42" t="s">
+        <v>271</v>
+      </c>
+      <c r="J1" s="42" t="s">
+        <v>272</v>
+      </c>
+      <c r="K1" s="42" t="s">
+        <v>273</v>
+      </c>
+      <c r="L1" s="43" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>252</v>
+        <v>275</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>253</v>
+        <v>276</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>254</v>
+        <v>277</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>255</v>
+        <v>278</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>256</v>
+        <v>279</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>257</v>
+        <v>280</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>258</v>
+        <v>281</v>
       </c>
       <c r="H2" s="10" t="n">
         <v>-10</v>
@@ -4556,36 +4647,36 @@
         <v>100</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>259</v>
+        <v>282</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>259</v>
+        <v>282</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>260</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>261</v>
+        <v>284</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>262</v>
+        <v>285</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>263</v>
-      </c>
-      <c r="D3" s="43" t="s">
-        <v>264</v>
-      </c>
-      <c r="E3" s="43" t="s">
-        <v>265</v>
-      </c>
-      <c r="F3" s="43" t="s">
-        <v>266</v>
+        <v>286</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>287</v>
+      </c>
+      <c r="E3" s="44" t="s">
+        <v>288</v>
+      </c>
+      <c r="F3" s="44" t="s">
+        <v>289</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>267</v>
+        <v>290</v>
       </c>
       <c r="H3" s="10" t="n">
         <v>-10</v>
@@ -4594,36 +4685,36 @@
         <v>100</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>259</v>
+        <v>282</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>259</v>
+        <v>282</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>268</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>269</v>
+        <v>292</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>270</v>
+        <v>293</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>271</v>
+        <v>294</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>272</v>
+        <v>295</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>273</v>
+        <v>296</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>274</v>
+        <v>297</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>275</v>
+        <v>298</v>
       </c>
       <c r="H4" s="10" t="n">
         <v>-10</v>
@@ -4632,36 +4723,36 @@
         <v>100</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>259</v>
+        <v>282</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>259</v>
+        <v>282</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>260</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>276</v>
+        <v>299</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>262</v>
+        <v>285</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>277</v>
+        <v>300</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>278</v>
+        <v>301</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>265</v>
+        <v>288</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>279</v>
+        <v>302</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>280</v>
+        <v>303</v>
       </c>
       <c r="H5" s="10" t="n">
         <v>-10</v>
@@ -4670,15 +4761,43 @@
         <v>100</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>259</v>
+        <v>282</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>259</v>
+        <v>282</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>260</v>
-      </c>
-    </row>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="1048465" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048466" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048467" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048468" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048469" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048470" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048471" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048472" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048473" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048474" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048475" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048476" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048477" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048478" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048479" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048480" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048481" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048482" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048483" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048484" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048485" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048486" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048487" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048488" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048489" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048490" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048491" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048492" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048493" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048494" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048495" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4782,7 +4901,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4814,60 +4933,77 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>281</v>
+        <v>304</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>282</v>
+        <v>305</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>283</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>285</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>286</v>
+        <v>307</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>308</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>281</v>
+        <v>304</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>287</v>
+        <v>310</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>288</v>
+        <v>311</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>289</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>290</v>
-      </c>
-    </row>
+        <v>307</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>312</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="1048378" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048379" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048380" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048381" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048382" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048383" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048384" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048385" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048386" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048387" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048388" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048389" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048390" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048391" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048392" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048393" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048394" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048395" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048396" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048397" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
questionnaire: add group for results by address
Add a group for each address in the results section. In this group, add
widgets to display some information coming from the server. For now,
only the monthly housing cost is displayed.
</commit_message>
<xml_diff>
--- a/localisation/references/questionnaireLocalisation.xlsx
+++ b/localisation/references/questionnaireLocalisation.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="364">
   <si>
     <t xml:space="preserve">questionName</t>
   </si>
@@ -533,6 +533,26 @@
     <t xml:space="preserve">Accessibility comparison</t>
   </si>
   <si>
+    <t xml:space="preserve">resultsByAddress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">monthlyCost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">monthlyCost.housingCostMonthly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coût mensuel total du logement
+**{{housingCostMonthly}}** $</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Housing Monthly Cost
+$**{{housingCostMonthly}}**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Custom because of the label with placeholder</t>
+  </si>
+  <si>
     <t xml:space="preserve">conditional_name</t>
   </si>
   <si>
@@ -1110,6 +1130,15 @@
   </si>
   <si>
     <t xml:space="preserve">Delete this destination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addressGroupName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Option B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Option A</t>
   </si>
 </sst>
 </file>
@@ -1121,7 +1150,7 @@
     <numFmt numFmtId="165" formatCode="&quot;VRAI&quot;;&quot;VRAI&quot;;&quot;FAUX&quot;"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1210,6 +1239,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1301,6 +1336,13 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="thin"/>
       <top style="thin"/>
@@ -1310,13 +1352,6 @@
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right/>
       <top style="thin"/>
       <bottom/>
       <diagonal/>
@@ -1347,7 +1382,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1448,23 +1483,23 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1504,15 +1539,19 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1520,11 +1559,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1532,7 +1571,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1544,16 +1583,20 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1855,14 +1898,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:XFD33"/>
+  <dimension ref="A1:XFD35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
-      <selection pane="bottomRight" activeCell="C29" activeCellId="0" sqref="C29"/>
+      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="G28" activeCellId="0" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2597,7 +2640,7 @@
       <c r="XFA11" s="1"/>
       <c r="XFB11" s="1"/>
       <c r="XFC11" s="1"/>
-      <c r="XFD11" s="1"/>
+      <c r="XFD11" s="0"/>
     </row>
     <row r="12" s="9" customFormat="true" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="17" t="s">
@@ -2671,7 +2714,7 @@
       <c r="XFA12" s="1"/>
       <c r="XFB12" s="1"/>
       <c r="XFC12" s="1"/>
-      <c r="XFD12" s="1"/>
+      <c r="XFD12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
@@ -2707,6 +2750,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="XFD13" s="25"/>
     </row>
     <row r="14" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
@@ -2738,31 +2782,32 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" s="29" customFormat="true" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="25" t="s">
+      <c r="XFD14" s="1"/>
+    </row>
+    <row r="15" s="30" customFormat="true" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="27" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D15" s="28" t="s">
+      <c r="C15" s="28" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D15" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="O15" s="28"/>
-      <c r="T15" s="27" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="XFD15" s="30"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="M15" s="29"/>
+      <c r="O15" s="29"/>
+      <c r="T15" s="28" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="XFD15" s="1"/>
     </row>
     <row r="16" s="9" customFormat="true" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="23" t="s">
@@ -2836,7 +2881,7 @@
       <c r="XFA16" s="1"/>
       <c r="XFB16" s="1"/>
       <c r="XFC16" s="1"/>
-      <c r="XFD16" s="1"/>
+      <c r="XFD16" s="0"/>
     </row>
     <row r="17" s="9" customFormat="true" ht="96.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="23" t="s">
@@ -2911,7 +2956,7 @@
       <c r="XFA17" s="1"/>
       <c r="XFB17" s="1"/>
       <c r="XFC17" s="1"/>
-      <c r="XFD17" s="1"/>
+      <c r="XFD17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="51.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
@@ -3188,6 +3233,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="XFD24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="33.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
@@ -3312,6 +3358,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="XFD27" s="1"/>
     </row>
     <row r="28" s="9" customFormat="true" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="23" t="s">
@@ -3385,7 +3432,7 @@
       <c r="XFA28" s="1"/>
       <c r="XFB28" s="1"/>
       <c r="XFC28" s="1"/>
-      <c r="XFD28" s="1"/>
+      <c r="XFD28" s="0"/>
     </row>
     <row r="29" s="9" customFormat="true" ht="96.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="23" t="s">
@@ -3566,7 +3613,7 @@
       <c r="XFA31" s="1"/>
       <c r="XFB31" s="1"/>
       <c r="XFC31" s="1"/>
-      <c r="XFD31" s="1"/>
+      <c r="XFD31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
@@ -3620,8 +3667,60 @@
         <v>161</v>
       </c>
     </row>
+    <row r="34" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="37" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" s="37" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="F35" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="G35" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="H35" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="T35" s="19" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="Y35" s="0" t="s">
+        <v>167</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C2 C17 C4 C15 C27 C6 C3 C18:C25 C7:C9">
+  <conditionalFormatting sqref="C17:C25 C1:C4 C15 C27 C6:C9">
     <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("FALSE",C1)))</formula>
     </cfRule>
@@ -3629,7 +3728,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10:C14 C26 C5 C31 C16:C17 C28:C30 C32:C33">
+  <conditionalFormatting sqref="C10:C14 C26 C5 C16:C17 C28:C35">
     <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="2">
       <formula>NOT(ISERROR(SEARCH("FALSE",C5)))</formula>
     </cfRule>
@@ -3663,30 +3762,30 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="38.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="23" width="15.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="39" width="20.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="40" width="20.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="23" width="19.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="23" width="12.14"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="23" width="8.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="B1" s="40" t="s">
-        <v>163</v>
-      </c>
-      <c r="C1" s="40" t="s">
+      <c r="A1" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="41" t="s">
-        <v>164</v>
-      </c>
-      <c r="E1" s="40" t="s">
-        <v>165</v>
-      </c>
-      <c r="F1" s="40" t="s">
-        <v>166</v>
+      <c r="D1" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>171</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3694,10 +3793,10 @@
         <v>63</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="D2" s="42" t="s">
-        <v>168</v>
+        <v>173</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>174</v>
       </c>
       <c r="E2" s="23" t="n">
         <v>16</v>
@@ -3708,10 +3807,10 @@
         <v>73</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="D3" s="42" t="s">
-        <v>168</v>
+        <v>175</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>174</v>
       </c>
       <c r="E3" s="23" t="n">
         <v>2</v>
@@ -3955,29 +4054,29 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="44" t="s">
-        <v>170</v>
-      </c>
-      <c r="C1" s="43" t="s">
-        <v>171</v>
-      </c>
-      <c r="D1" s="43" t="s">
-        <v>172</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>173</v>
-      </c>
-      <c r="F1" s="43" t="s">
-        <v>174</v>
+      <c r="B1" s="45" t="s">
+        <v>176</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>177</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="F1" s="44" t="s">
+        <v>180</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="H1" s="43" t="s">
-        <v>176</v>
+        <v>181</v>
+      </c>
+      <c r="H1" s="44" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3985,23 +4084,23 @@
         <v>27</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>179</v>
-      </c>
-      <c r="E2" s="45" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F2" s="45" t="b">
+        <v>185</v>
+      </c>
+      <c r="E2" s="46" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="46" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G2" s="45" t="b">
+      <c r="G2" s="46" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4011,23 +4110,23 @@
         <v>49</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="E3" s="45" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F3" s="45" t="b">
+        <v>188</v>
+      </c>
+      <c r="E3" s="46" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="46" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G3" s="45" t="b">
+      <c r="G3" s="46" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4037,23 +4136,23 @@
         <v>67</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="E4" s="45" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F4" s="45" t="b">
+        <v>191</v>
+      </c>
+      <c r="E4" s="46" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="46" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G4" s="45" t="b">
+      <c r="G4" s="46" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4064,23 +4163,23 @@
         <v>87</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="E5" s="45" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F5" s="45" t="b">
+        <v>194</v>
+      </c>
+      <c r="E5" s="46" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="46" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G5" s="45" t="b">
+      <c r="G5" s="46" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4090,23 +4189,23 @@
         <v>141</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>191</v>
-      </c>
-      <c r="E6" s="45" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F6" s="45" t="b">
+        <v>197</v>
+      </c>
+      <c r="E6" s="46" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="46" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G6" s="45" t="b">
+      <c r="G6" s="46" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4116,23 +4215,23 @@
         <v>156</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>194</v>
-      </c>
-      <c r="E7" s="45" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F7" s="45" t="b">
+        <v>200</v>
+      </c>
+      <c r="E7" s="46" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="46" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G7" s="45" t="b">
+      <c r="G7" s="46" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4339,46 +4438,46 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="B1" s="46" t="s">
-        <v>165</v>
-      </c>
-      <c r="C1" s="46" t="s">
+      <c r="A1" s="47" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="46" t="s">
-        <v>196</v>
-      </c>
-      <c r="H1" s="46" t="s">
+      <c r="G1" s="47" t="s">
+        <v>202</v>
+      </c>
+      <c r="H1" s="47" t="s">
         <v>12</v>
       </c>
       <c r="I1" s="24" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="35" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="E2" s="35"/>
       <c r="F2" s="35"/>
@@ -4387,16 +4486,16 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="35" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="E3" s="35"/>
       <c r="F3" s="35"/>
@@ -4405,16 +4504,16 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="35" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="E4" s="35"/>
       <c r="F4" s="35"/>
@@ -4423,16 +4522,16 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="35" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="E5" s="35"/>
       <c r="F5" s="35"/>
@@ -4441,16 +4540,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="35" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="E6" s="35"/>
       <c r="F6" s="35"/>
@@ -4459,16 +4558,16 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="35" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="E7" s="35"/>
       <c r="F7" s="35"/>
@@ -4485,7 +4584,7 @@
       <c r="E8" s="35"/>
       <c r="F8" s="35"/>
       <c r="G8" s="35" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="H8" s="35"/>
     </row>
@@ -4499,7 +4598,7 @@
       <c r="E9" s="35"/>
       <c r="F9" s="35"/>
       <c r="G9" s="35" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="H9" s="35"/>
     </row>
@@ -4527,13 +4626,13 @@
       <c r="E11" s="35"/>
       <c r="F11" s="35"/>
       <c r="G11" s="35" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="H11" s="35"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="35" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="B12" s="35"/>
       <c r="C12" s="35"/>
@@ -4541,13 +4640,13 @@
       <c r="E12" s="35"/>
       <c r="F12" s="35"/>
       <c r="G12" s="35" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="H12" s="35"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="35" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="B13" s="35"/>
       <c r="C13" s="35"/>
@@ -4555,13 +4654,13 @@
       <c r="E13" s="35"/>
       <c r="F13" s="35"/>
       <c r="G13" s="35" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="H13" s="35"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="35" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="B14" s="35"/>
       <c r="C14" s="35"/>
@@ -4569,22 +4668,22 @@
       <c r="E14" s="35"/>
       <c r="F14" s="35"/>
       <c r="G14" s="35" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="H14" s="35"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="48" t="s">
-        <v>217</v>
+      <c r="A15" s="49" t="s">
+        <v>223</v>
       </c>
       <c r="B15" s="35" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="E15" s="35"/>
       <c r="F15" s="35"/>
@@ -4592,17 +4691,17 @@
       <c r="H15" s="35"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="48" t="s">
-        <v>217</v>
+      <c r="A16" s="49" t="s">
+        <v>223</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C16" s="35" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="E16" s="35"/>
       <c r="F16" s="35"/>
@@ -4610,8 +4709,8 @@
       <c r="H16" s="35"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="48" t="s">
-        <v>217</v>
+      <c r="A17" s="49" t="s">
+        <v>223</v>
       </c>
       <c r="B17" s="35"/>
       <c r="C17" s="35"/>
@@ -4619,22 +4718,22 @@
       <c r="E17" s="35"/>
       <c r="F17" s="35"/>
       <c r="G17" s="35" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="H17" s="35"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="49" t="s">
+        <v>230</v>
+      </c>
+      <c r="B18" s="35" t="s">
         <v>224</v>
       </c>
-      <c r="B18" s="35" t="s">
-        <v>218</v>
-      </c>
       <c r="C18" s="35" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="E18" s="35"/>
       <c r="F18" s="35"/>
@@ -4642,17 +4741,17 @@
       <c r="H18" s="35"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="48" t="s">
-        <v>224</v>
+      <c r="A19" s="49" t="s">
+        <v>230</v>
       </c>
       <c r="B19" s="35" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C19" s="35" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="E19" s="35"/>
       <c r="F19" s="35"/>
@@ -4660,17 +4759,17 @@
       <c r="H19" s="35"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="48" t="s">
-        <v>224</v>
+      <c r="A20" s="49" t="s">
+        <v>230</v>
       </c>
       <c r="B20" s="35" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="C20" s="35" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="E20" s="35"/>
       <c r="F20" s="35"/>
@@ -4678,8 +4777,8 @@
       <c r="H20" s="35"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="48" t="s">
-        <v>224</v>
+      <c r="A21" s="49" t="s">
+        <v>230</v>
       </c>
       <c r="B21" s="35"/>
       <c r="C21" s="35"/>
@@ -4687,7 +4786,7 @@
       <c r="E21" s="35"/>
       <c r="F21" s="35"/>
       <c r="G21" s="35" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="H21" s="35"/>
     </row>
@@ -4696,13 +4795,13 @@
         <v>37</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4710,13 +4809,13 @@
         <v>37</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -4726,13 +4825,13 @@
         <v>37</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -4742,13 +4841,13 @@
         <v>37</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -4758,13 +4857,13 @@
         <v>37</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -4774,13 +4873,13 @@
         <v>37</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -4790,13 +4889,13 @@
         <v>37</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -4806,13 +4905,13 @@
         <v>37</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -4822,13 +4921,13 @@
         <v>37</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -4838,13 +4937,13 @@
         <v>37</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
@@ -4854,13 +4953,13 @@
         <v>37</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
@@ -4870,13 +4969,13 @@
         <v>37</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
@@ -4886,13 +4985,13 @@
         <v>37</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="D34" s="24" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4900,13 +4999,13 @@
         <v>37</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="D35" s="24" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4914,13 +5013,13 @@
         <v>37</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4931,10 +5030,10 @@
         <v>104</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="D37" s="24" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4942,13 +5041,13 @@
         <v>102</v>
       </c>
       <c r="B38" s="24" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4956,13 +5055,13 @@
         <v>78</v>
       </c>
       <c r="B39" s="24" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4970,13 +5069,13 @@
         <v>78</v>
       </c>
       <c r="B40" s="24" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4984,13 +5083,13 @@
         <v>78</v>
       </c>
       <c r="B41" s="24" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4998,7 +5097,7 @@
         <v>78</v>
       </c>
       <c r="G42" s="35" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5006,13 +5105,13 @@
         <v>83</v>
       </c>
       <c r="B43" s="24" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="H43" s="23"/>
     </row>
@@ -5021,13 +5120,13 @@
         <v>83</v>
       </c>
       <c r="B44" s="24" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="H44" s="23"/>
     </row>
@@ -5036,13 +5135,13 @@
         <v>83</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="H45" s="23"/>
     </row>
@@ -5051,13 +5150,13 @@
         <v>83</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="C46" s="24" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="H46" s="23"/>
     </row>
@@ -5277,64 +5376,64 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="49" t="s">
-        <v>300</v>
-      </c>
-      <c r="B1" s="49" t="s">
-        <v>301</v>
-      </c>
-      <c r="C1" s="49" t="s">
-        <v>302</v>
-      </c>
-      <c r="D1" s="49" t="s">
-        <v>303</v>
-      </c>
-      <c r="E1" s="49" t="s">
-        <v>304</v>
-      </c>
-      <c r="F1" s="49" t="s">
-        <v>305</v>
-      </c>
-      <c r="G1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>306</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>307</v>
       </c>
-      <c r="I1" s="49" t="s">
+      <c r="C1" s="50" t="s">
         <v>308</v>
       </c>
-      <c r="J1" s="49" t="s">
+      <c r="D1" s="50" t="s">
         <v>309</v>
       </c>
-      <c r="K1" s="49" t="s">
+      <c r="E1" s="50" t="s">
         <v>310</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="F1" s="50" t="s">
         <v>311</v>
+      </c>
+      <c r="G1" s="50" t="s">
+        <v>312</v>
+      </c>
+      <c r="H1" s="50" t="s">
+        <v>313</v>
+      </c>
+      <c r="I1" s="50" t="s">
+        <v>314</v>
+      </c>
+      <c r="J1" s="50" t="s">
+        <v>315</v>
+      </c>
+      <c r="K1" s="50" t="s">
+        <v>316</v>
+      </c>
+      <c r="L1" s="51" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="H2" s="10" t="n">
         <v>-10</v>
@@ -5343,36 +5442,36 @@
         <v>100</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>323</v>
-      </c>
-      <c r="D3" s="51" t="s">
-        <v>324</v>
-      </c>
-      <c r="E3" s="51" t="s">
-        <v>325</v>
-      </c>
-      <c r="F3" s="51" t="s">
-        <v>326</v>
+        <v>329</v>
+      </c>
+      <c r="D3" s="52" t="s">
+        <v>330</v>
+      </c>
+      <c r="E3" s="52" t="s">
+        <v>331</v>
+      </c>
+      <c r="F3" s="52" t="s">
+        <v>332</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="H3" s="10" t="n">
         <v>-10</v>
@@ -5381,36 +5480,36 @@
         <v>100</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="H4" s="10" t="n">
         <v>-10</v>
@@ -5419,36 +5518,36 @@
         <v>100</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="H5" s="10" t="n">
         <v>-10</v>
@@ -5457,13 +5556,13 @@
         <v>100</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
     </row>
     <row r="1048465" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -5597,7 +5696,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5632,13 +5731,13 @@
         <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5646,13 +5745,13 @@
         <v>49</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5660,13 +5759,13 @@
         <v>67</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5674,13 +5773,13 @@
         <v>67</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5688,13 +5787,13 @@
         <v>141</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5702,15 +5801,37 @@
         <v>141</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>354</v>
-      </c>
-    </row>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B8" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="1048376" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048377" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048378" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048379" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048380" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
results: add car cost and total monthly cost to the UI
</commit_message>
<xml_diff>
--- a/localisation/references/questionnaireLocalisation.xlsx
+++ b/localisation/references/questionnaireLocalisation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="423">
   <si>
     <t xml:space="preserve">questionName</t>
   </si>
@@ -585,7 +585,7 @@
     <t xml:space="preserve">resultsByAddress</t>
   </si>
   <si>
-    <t xml:space="preserve">monthlyCost</t>
+    <t xml:space="preserve">monthlyHousingCost</t>
   </si>
   <si>
     <t xml:space="preserve">monthlyCost.housingCostMonthly</t>
@@ -602,6 +602,34 @@
     <t xml:space="preserve">Custom because of the label with placeholder</t>
   </si>
   <si>
+    <t xml:space="preserve">monthlyCarCost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">monthlyCost.carCostMonthly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coût mensuel de la possession de véhicules (selon les données de CAA Québec)
+**{{carCostMonthly}}** $</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monthly cost of car possession (according to CAA Québec data)
+$**{{carCostMonthly}}**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">monthlyTotalCost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">monthlyCost.totalCostMonthly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coût mensuel total
+**{{monthlyCost}}** $</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Monthly Cost
+$**{{monthlyCost}}**</t>
+  </si>
+  <si>
     <t xml:space="preserve">destinationsRouting</t>
   </si>
   <si>
@@ -1287,6 +1315,17 @@
   </si>
   <si>
     <t xml:space="preserve">Transit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">monthlyCost.carCostMonthlyNull</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coût mensuel de la possession de véhicules (selon les données de CAA Québec)
+-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monthly cost of car possession (according to CAA Québec data)
+-</t>
   </si>
 </sst>
 </file>
@@ -1524,7 +1563,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1751,6 +1790,10 @@
     </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2052,14 +2095,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:XFD44"/>
+  <dimension ref="A1:XFD46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="O16" activeCellId="0" sqref="O16"/>
+      <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+      <selection pane="bottomRight" activeCell="F42" activeCellId="0" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4223,7 +4266,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="102.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
         <v>183</v>
       </c>
@@ -4240,17 +4283,19 @@
       <c r="E41" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="F41" s="30" t="s">
+      <c r="F41" s="43" t="s">
         <v>184</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="G41" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="H41" s="30" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="T41" s="26"/>
+      <c r="Y41" s="1"/>
+    </row>
+    <row r="42" customFormat="false" ht="59" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
         <v>187</v>
       </c>
@@ -4265,23 +4310,25 @@
         <v>171</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="F42" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F42" s="43" t="s">
         <v>188</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="G42" s="30" t="s">
         <v>189</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="H42" s="30" t="s">
         <v>190</v>
       </c>
+      <c r="T42" s="26"/>
+      <c r="Y42" s="1"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C43" s="38" t="n">
@@ -4292,9 +4339,9 @@
         <v>171</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="F43" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F43" s="30" t="s">
         <v>192</v>
       </c>
       <c r="G43" s="2" t="s">
@@ -4308,7 +4355,7 @@
       <c r="A44" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C44" s="38" t="n">
@@ -4319,7 +4366,7 @@
         <v>171</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>196</v>
@@ -4328,7 +4375,61 @@
         <v>197</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" s="38" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C46" s="38" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -4340,7 +4441,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C12:C18 C6:C7 C20:C21 C33:C44 C31 C2 C30">
+  <conditionalFormatting sqref="C12:C18 C6:C7 C20:C21 C31 C2 C30 C33:C46">
     <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="2">
       <formula>NOT(ISERROR(SEARCH("FALSE",C2)))</formula>
     </cfRule>
@@ -4382,22 +4483,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="45" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="C1" s="45" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="F1" s="45" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4405,10 +4506,10 @@
         <v>70</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="D2" s="47" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="E2" s="30" t="n">
         <v>16</v>
@@ -4419,10 +4520,10 @@
         <v>83</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="E3" s="30" t="n">
         <v>2</v>
@@ -4670,25 +4771,25 @@
         <v>3</v>
       </c>
       <c r="B1" s="49" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C1" s="48" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D1" s="48" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="E1" s="48" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="F1" s="48" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="H1" s="48" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4696,13 +4797,13 @@
         <v>27</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="E2" s="50" t="b">
         <f aca="false">TRUE()</f>
@@ -4722,13 +4823,13 @@
         <v>52</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="E3" s="50" t="b">
         <f aca="false">TRUE()</f>
@@ -4748,13 +4849,13 @@
         <v>74</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="E4" s="50" t="b">
         <f aca="false">TRUE()</f>
@@ -4775,13 +4876,13 @@
         <v>97</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="E5" s="50" t="b">
         <f aca="false">TRUE()</f>
@@ -4801,13 +4902,13 @@
         <v>154</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="E6" s="50" t="b">
         <f aca="false">TRUE()</f>
@@ -4827,13 +4928,13 @@
         <v>171</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="E7" s="50" t="b">
         <f aca="false">TRUE()</f>
@@ -5051,10 +5152,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="B1" s="51" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="C1" s="51" t="s">
         <v>6</v>
@@ -5069,27 +5170,27 @@
         <v>9</v>
       </c>
       <c r="G1" s="51" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="H1" s="51" t="s">
         <v>12</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="41" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="C2" s="41" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="E2" s="41"/>
       <c r="F2" s="41"/>
@@ -5098,16 +5199,16 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="41" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="B3" s="41" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="E3" s="41"/>
       <c r="F3" s="41"/>
@@ -5116,16 +5217,16 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="41" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="C4" s="41" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="E4" s="41"/>
       <c r="F4" s="41"/>
@@ -5134,16 +5235,16 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="41" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="C5" s="41" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="E5" s="41"/>
       <c r="F5" s="41"/>
@@ -5152,16 +5253,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="41" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="C6" s="41" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="D6" s="41" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="E6" s="41"/>
       <c r="F6" s="41"/>
@@ -5170,16 +5271,16 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="41" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="B7" s="41" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="C7" s="41" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="E7" s="41"/>
       <c r="F7" s="41"/>
@@ -5196,7 +5297,7 @@
       <c r="E8" s="41"/>
       <c r="F8" s="41"/>
       <c r="G8" s="41" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="H8" s="41"/>
     </row>
@@ -5210,7 +5311,7 @@
       <c r="E9" s="41"/>
       <c r="F9" s="41"/>
       <c r="G9" s="41" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="H9" s="41"/>
     </row>
@@ -5238,13 +5339,13 @@
       <c r="E11" s="41"/>
       <c r="F11" s="41"/>
       <c r="G11" s="41" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="H11" s="41"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="41" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="B12" s="41"/>
       <c r="C12" s="41"/>
@@ -5252,13 +5353,13 @@
       <c r="E12" s="41"/>
       <c r="F12" s="41"/>
       <c r="G12" s="41" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="H12" s="41"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="B13" s="41"/>
       <c r="C13" s="41"/>
@@ -5266,13 +5367,13 @@
       <c r="E13" s="41"/>
       <c r="F13" s="41"/>
       <c r="G13" s="41" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="H13" s="41"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="41" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="B14" s="41"/>
       <c r="C14" s="41"/>
@@ -5280,22 +5381,22 @@
       <c r="E14" s="41"/>
       <c r="F14" s="41"/>
       <c r="G14" s="41" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="H14" s="41"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="53" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="D15" s="41" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="E15" s="41"/>
       <c r="F15" s="41"/>
@@ -5304,16 +5405,16 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="53" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="D16" s="41" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="E16" s="41"/>
       <c r="F16" s="41"/>
@@ -5322,7 +5423,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="53" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="B17" s="41"/>
       <c r="C17" s="41"/>
@@ -5330,22 +5431,22 @@
       <c r="E17" s="41"/>
       <c r="F17" s="41"/>
       <c r="G17" s="41" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="H17" s="41"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="53" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="B18" s="41" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="C18" s="41" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="D18" s="41" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="E18" s="41"/>
       <c r="F18" s="41"/>
@@ -5354,16 +5455,16 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="53" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="C19" s="41" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="D19" s="41" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="E19" s="41"/>
       <c r="F19" s="41"/>
@@ -5372,16 +5473,16 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="53" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="C20" s="41" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="D20" s="41" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="E20" s="41"/>
       <c r="F20" s="41"/>
@@ -5390,7 +5491,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="53" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="B21" s="41"/>
       <c r="C21" s="41"/>
@@ -5398,7 +5499,7 @@
       <c r="E21" s="41"/>
       <c r="F21" s="41"/>
       <c r="G21" s="41" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="H21" s="41"/>
     </row>
@@ -5407,13 +5508,13 @@
         <v>41</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5421,13 +5522,13 @@
         <v>41</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>271</v>
+        <v>279</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -5437,13 +5538,13 @@
         <v>41</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -5453,13 +5554,13 @@
         <v>41</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -5469,13 +5570,13 @@
         <v>41</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -5485,13 +5586,13 @@
         <v>41</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -5501,13 +5602,13 @@
         <v>41</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -5517,13 +5618,13 @@
         <v>41</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -5533,13 +5634,13 @@
         <v>41</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -5549,13 +5650,13 @@
         <v>41</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
@@ -5565,13 +5666,13 @@
         <v>41</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
@@ -5581,13 +5682,13 @@
         <v>41</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
@@ -5597,13 +5698,13 @@
         <v>41</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5611,13 +5712,13 @@
         <v>41</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="D35" s="31" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5625,13 +5726,13 @@
         <v>41</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="D36" s="31" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5642,10 +5743,10 @@
         <v>117</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="D37" s="31" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5653,13 +5754,13 @@
         <v>115</v>
       </c>
       <c r="B38" s="31" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="D38" s="31" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5667,13 +5768,13 @@
         <v>88</v>
       </c>
       <c r="B39" s="31" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="D39" s="31" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5681,13 +5782,13 @@
         <v>88</v>
       </c>
       <c r="B40" s="31" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>319</v>
+        <v>327</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5695,13 +5796,13 @@
         <v>88</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>321</v>
+        <v>329</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="D41" s="31" t="s">
-        <v>323</v>
+        <v>331</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5709,7 +5810,7 @@
         <v>88</v>
       </c>
       <c r="G42" s="41" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5717,13 +5818,13 @@
         <v>93</v>
       </c>
       <c r="B43" s="31" t="s">
-        <v>324</v>
+        <v>332</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="D43" s="31" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="H43" s="30"/>
     </row>
@@ -5732,13 +5833,13 @@
         <v>93</v>
       </c>
       <c r="B44" s="31" t="s">
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="C44" s="31" t="s">
-        <v>328</v>
+        <v>336</v>
       </c>
       <c r="D44" s="31" t="s">
-        <v>329</v>
+        <v>337</v>
       </c>
       <c r="H44" s="30"/>
     </row>
@@ -5747,13 +5848,13 @@
         <v>93</v>
       </c>
       <c r="B45" s="31" t="s">
-        <v>330</v>
+        <v>338</v>
       </c>
       <c r="C45" s="31" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="D45" s="31" t="s">
-        <v>332</v>
+        <v>340</v>
       </c>
       <c r="H45" s="30"/>
     </row>
@@ -5762,13 +5863,13 @@
         <v>93</v>
       </c>
       <c r="B46" s="31" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="C46" s="31" t="s">
-        <v>334</v>
+        <v>342</v>
       </c>
       <c r="D46" s="31" t="s">
-        <v>335</v>
+        <v>343</v>
       </c>
       <c r="H46" s="30"/>
     </row>
@@ -5989,63 +6090,63 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="54" t="s">
-        <v>336</v>
+        <v>344</v>
       </c>
       <c r="B1" s="54" t="s">
-        <v>337</v>
+        <v>345</v>
       </c>
       <c r="C1" s="54" t="s">
-        <v>338</v>
+        <v>346</v>
       </c>
       <c r="D1" s="54" t="s">
-        <v>339</v>
+        <v>347</v>
       </c>
       <c r="E1" s="54" t="s">
-        <v>340</v>
+        <v>348</v>
       </c>
       <c r="F1" s="54" t="s">
-        <v>341</v>
+        <v>349</v>
       </c>
       <c r="G1" s="54" t="s">
-        <v>342</v>
+        <v>350</v>
       </c>
       <c r="H1" s="54" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="I1" s="54" t="s">
-        <v>344</v>
+        <v>352</v>
       </c>
       <c r="J1" s="54" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
       <c r="K1" s="54" t="s">
-        <v>346</v>
+        <v>354</v>
       </c>
       <c r="L1" s="55" t="s">
-        <v>347</v>
+        <v>355</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="s">
-        <v>348</v>
+        <v>356</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>349</v>
+        <v>357</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>350</v>
+        <v>358</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>351</v>
+        <v>359</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>353</v>
+        <v>361</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>354</v>
+        <v>362</v>
       </c>
       <c r="H2" s="17" t="n">
         <v>-10</v>
@@ -6054,36 +6155,36 @@
         <v>100</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>355</v>
+        <v>363</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>355</v>
+        <v>363</v>
       </c>
       <c r="L2" s="17" t="s">
-        <v>356</v>
+        <v>364</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="17" t="s">
-        <v>357</v>
+        <v>365</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>358</v>
+        <v>366</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>359</v>
+        <v>367</v>
       </c>
       <c r="D3" s="56" t="s">
-        <v>360</v>
+        <v>368</v>
       </c>
       <c r="E3" s="56" t="s">
-        <v>361</v>
+        <v>369</v>
       </c>
       <c r="F3" s="56" t="s">
-        <v>362</v>
+        <v>370</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>363</v>
+        <v>371</v>
       </c>
       <c r="H3" s="17" t="n">
         <v>-10</v>
@@ -6092,36 +6193,36 @@
         <v>100</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>355</v>
+        <v>363</v>
       </c>
       <c r="K3" s="17" t="s">
-        <v>355</v>
+        <v>363</v>
       </c>
       <c r="L3" s="17" t="s">
-        <v>364</v>
+        <v>372</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="s">
-        <v>365</v>
+        <v>373</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>366</v>
+        <v>374</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>367</v>
+        <v>375</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>368</v>
+        <v>376</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>369</v>
+        <v>377</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>370</v>
+        <v>378</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>371</v>
+        <v>379</v>
       </c>
       <c r="H4" s="17" t="n">
         <v>-10</v>
@@ -6130,36 +6231,36 @@
         <v>100</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>355</v>
+        <v>363</v>
       </c>
       <c r="K4" s="17" t="s">
-        <v>355</v>
+        <v>363</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>356</v>
+        <v>364</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="17" t="s">
-        <v>372</v>
+        <v>380</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>358</v>
+        <v>366</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>373</v>
+        <v>381</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>374</v>
+        <v>382</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>361</v>
+        <v>369</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>375</v>
+        <v>383</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>376</v>
+        <v>384</v>
       </c>
       <c r="H5" s="17" t="n">
         <v>-10</v>
@@ -6168,13 +6269,13 @@
         <v>100</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>355</v>
+        <v>363</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>355</v>
+        <v>363</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>356</v>
+        <v>364</v>
       </c>
     </row>
     <row r="1048465" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -6307,8 +6408,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C47" activeCellId="0" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6343,13 +6444,13 @@
         <v>52</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>377</v>
+        <v>385</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>378</v>
+        <v>386</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>379</v>
+        <v>387</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6357,13 +6458,13 @@
         <v>52</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>380</v>
+        <v>388</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>381</v>
+        <v>389</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6371,13 +6472,13 @@
         <v>74</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>377</v>
+        <v>385</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>384</v>
+        <v>392</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6385,13 +6486,13 @@
         <v>74</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>380</v>
+        <v>388</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>385</v>
+        <v>393</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>386</v>
+        <v>394</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6399,13 +6500,13 @@
         <v>154</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>377</v>
+        <v>385</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>387</v>
+        <v>395</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>388</v>
+        <v>396</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6413,13 +6514,13 @@
         <v>154</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>380</v>
+        <v>388</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>389</v>
+        <v>397</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>390</v>
+        <v>398</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6427,19 +6528,19 @@
         <v>171</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>391</v>
+        <v>399</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>392</v>
+        <v>400</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>392</v>
+        <v>400</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>393</v>
+        <v>401</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>393</v>
+        <v>401</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6447,13 +6548,13 @@
         <v>171</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>394</v>
+        <v>402</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>395</v>
+        <v>403</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>395</v>
+        <v>403</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6461,13 +6562,13 @@
         <v>171</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>396</v>
+        <v>404</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>397</v>
+        <v>405</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6475,13 +6576,13 @@
         <v>171</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>398</v>
+        <v>406</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>399</v>
+        <v>407</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>400</v>
+        <v>408</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6489,13 +6590,13 @@
         <v>171</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>401</v>
+        <v>409</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>402</v>
+        <v>410</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>403</v>
+        <v>411</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6503,13 +6604,13 @@
         <v>171</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>404</v>
+        <v>412</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>405</v>
+        <v>413</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>406</v>
+        <v>414</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6517,13 +6618,13 @@
         <v>171</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>407</v>
+        <v>415</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>408</v>
+        <v>416</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6531,13 +6632,27 @@
         <v>171</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>409</v>
+        <v>417</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>410</v>
+        <v>418</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>411</v>
+        <v>419</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B16" s="57" t="s">
+        <v>420</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>421</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="1048376" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
results: make monthly cost widgets always visible
fixes #36

By making the widgets visible and simply adding a version where the
results are not displayed works around Evolution's issue
https://github.com/chairemobilite/evolution/issues/1361 which caused
results not to appear on first display.

Later improvements will probably make those widgets obsolete anyway, so
no need to work more on this fix.
</commit_message>
<xml_diff>
--- a/localisation/references/questionnaireLocalisation.xlsx
+++ b/localisation/references/questionnaireLocalisation.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="423">
   <si>
     <t xml:space="preserve">questionName</t>
   </si>
@@ -1304,19 +1304,104 @@
   <si>
     <t xml:space="preserve">Monthly cost of car possession (according to CAA data)
 -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">monthlyCost.housingCostMonthlyNull</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coût mensuel total du logement
+-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Housing Monthly Cost
+-</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">monthlyCost.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">totalCostMonthly</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Null</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Coût mensuel total
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Total Monthly Cost
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;VRAI&quot;;&quot;VRAI&quot;;&quot;FAUX&quot;"/>
-    <numFmt numFmtId="166" formatCode="General"/>
-    <numFmt numFmtId="167" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1451,6 +1536,12 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1542,7 +1633,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="55">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1595,10 +1686,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1608,10 +1695,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1631,15 +1714,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1672,10 +1751,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1723,7 +1798,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1731,11 +1806,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1747,7 +1822,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1773,6 +1848,10 @@
     </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2084,7 +2163,7 @@
       <selection pane="bottomRight" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.29"/>
@@ -2097,7 +2176,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="10.91"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2174,7 +2253,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" s="14" customFormat="true" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="13" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
@@ -2209,7 +2288,7 @@
       <c r="Q2" s="9"/>
       <c r="R2" s="9"/>
       <c r="S2" s="9"/>
-      <c r="T2" s="13" t="b">
+      <c r="T2" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2217,176 +2296,176 @@
       <c r="V2" s="9"/>
       <c r="W2" s="9"/>
       <c r="X2" s="9"/>
-      <c r="XEE2" s="15"/>
-      <c r="XEF2" s="15"/>
-      <c r="XEG2" s="15"/>
-      <c r="XEH2" s="15"/>
-      <c r="XEI2" s="15"/>
-      <c r="XEJ2" s="15"/>
-      <c r="XEK2" s="15"/>
-      <c r="XEL2" s="15"/>
-      <c r="XEM2" s="15"/>
-      <c r="XEN2" s="15"/>
-      <c r="XEO2" s="15"/>
-      <c r="XEP2" s="15"/>
-      <c r="XEQ2" s="15"/>
-      <c r="XER2" s="15"/>
-      <c r="XES2" s="15"/>
-      <c r="XET2" s="15"/>
-      <c r="XEU2" s="15"/>
-      <c r="XEV2" s="15"/>
-      <c r="XEW2" s="15"/>
-      <c r="XEX2" s="15"/>
-      <c r="XEY2" s="15"/>
-      <c r="XEZ2" s="15"/>
-      <c r="XFA2" s="15"/>
-      <c r="XFB2" s="15"/>
-      <c r="XFC2" s="15"/>
-      <c r="XFD2" s="15"/>
-    </row>
-    <row r="3" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="16" t="s">
+      <c r="XEE2" s="14"/>
+      <c r="XEF2" s="14"/>
+      <c r="XEG2" s="14"/>
+      <c r="XEH2" s="14"/>
+      <c r="XEI2" s="14"/>
+      <c r="XEJ2" s="14"/>
+      <c r="XEK2" s="14"/>
+      <c r="XEL2" s="14"/>
+      <c r="XEM2" s="14"/>
+      <c r="XEN2" s="14"/>
+      <c r="XEO2" s="14"/>
+      <c r="XEP2" s="14"/>
+      <c r="XEQ2" s="14"/>
+      <c r="XER2" s="14"/>
+      <c r="XES2" s="14"/>
+      <c r="XET2" s="14"/>
+      <c r="XEU2" s="14"/>
+      <c r="XEV2" s="14"/>
+      <c r="XEW2" s="14"/>
+      <c r="XEX2" s="14"/>
+      <c r="XEY2" s="14"/>
+      <c r="XEZ2" s="14"/>
+      <c r="XFA2" s="14"/>
+      <c r="XFB2" s="14"/>
+      <c r="XFC2" s="14"/>
+      <c r="XFD2" s="14"/>
+    </row>
+    <row r="3" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="17" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D3" s="16" t="s">
+      <c r="C3" s="15" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16" t="str">
+      <c r="E3" s="15"/>
+      <c r="F3" s="15" t="str">
         <f aca="false">REPLACE(A3, FIND("_", A3), 1, ".")</f>
         <v>household.size</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16" t="s">
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16" t="s">
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="17" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U3" s="16"/>
-      <c r="V3" s="16"/>
-      <c r="W3" s="16"/>
-      <c r="X3" s="16"/>
-      <c r="Y3" s="18"/>
-      <c r="XFD3" s="19"/>
-    </row>
-    <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="16" t="s">
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="15"/>
+      <c r="Y3" s="16"/>
+      <c r="XFD3" s="17"/>
+    </row>
+    <row r="4" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="17" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D4" s="16" t="s">
+      <c r="C4" s="15" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16" t="s">
+      <c r="E4" s="15"/>
+      <c r="F4" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="20" t="s">
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="17" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16"/>
-      <c r="W4" s="16"/>
-      <c r="X4" s="16"/>
-      <c r="Y4" s="18"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="15"/>
+      <c r="Y4" s="16"/>
       <c r="XFD4" s="1"/>
     </row>
-    <row r="5" s="25" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="21" t="s">
+    <row r="5" s="22" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="22" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D5" s="21" t="s">
+      <c r="C5" s="19" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D5" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="24" t="str">
+      <c r="E5" s="20"/>
+      <c r="F5" s="21" t="str">
         <f aca="false">REPLACE(A5, FIND("_", A5), 1, ".")</f>
         <v>home.save</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="22" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U5" s="23"/>
-      <c r="V5" s="23"/>
-      <c r="W5" s="23"/>
-      <c r="X5" s="23"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="19" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U5" s="20"/>
+      <c r="V5" s="20"/>
+      <c r="W5" s="20"/>
+      <c r="X5" s="20"/>
       <c r="XEE5" s="1"/>
       <c r="XEF5" s="1"/>
       <c r="XEG5" s="1"/>
@@ -2412,9 +2491,9 @@
       <c r="XFA5" s="1"/>
       <c r="XFB5" s="1"/>
       <c r="XFC5" s="1"/>
-      <c r="XFD5" s="15"/>
-    </row>
-    <row r="6" s="14" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="XFD5" s="14"/>
+    </row>
+    <row r="6" s="13" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
         <v>46</v>
       </c>
@@ -2449,7 +2528,7 @@
       <c r="Q6" s="9"/>
       <c r="R6" s="9"/>
       <c r="S6" s="9"/>
-      <c r="T6" s="13" t="b">
+      <c r="T6" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2457,70 +2536,70 @@
       <c r="V6" s="9"/>
       <c r="W6" s="9"/>
       <c r="X6" s="9"/>
-      <c r="XEE6" s="15"/>
-      <c r="XEF6" s="15"/>
-      <c r="XEG6" s="15"/>
-      <c r="XEH6" s="15"/>
-      <c r="XEI6" s="15"/>
-      <c r="XEJ6" s="15"/>
-      <c r="XEK6" s="15"/>
-      <c r="XEL6" s="15"/>
-      <c r="XEM6" s="15"/>
-      <c r="XEN6" s="15"/>
-      <c r="XEO6" s="15"/>
-      <c r="XEP6" s="15"/>
-      <c r="XEQ6" s="15"/>
-      <c r="XER6" s="15"/>
-      <c r="XES6" s="15"/>
-      <c r="XET6" s="15"/>
-      <c r="XEU6" s="15"/>
-      <c r="XEV6" s="15"/>
-      <c r="XEW6" s="15"/>
-      <c r="XEX6" s="15"/>
-      <c r="XEY6" s="15"/>
-      <c r="XEZ6" s="15"/>
-      <c r="XFA6" s="15"/>
-      <c r="XFB6" s="15"/>
-      <c r="XFC6" s="15"/>
-      <c r="XFD6" s="26"/>
-    </row>
-    <row r="7" s="18" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27" t="s">
+      <c r="XEE6" s="14"/>
+      <c r="XEF6" s="14"/>
+      <c r="XEG6" s="14"/>
+      <c r="XEH6" s="14"/>
+      <c r="XEI6" s="14"/>
+      <c r="XEJ6" s="14"/>
+      <c r="XEK6" s="14"/>
+      <c r="XEL6" s="14"/>
+      <c r="XEM6" s="14"/>
+      <c r="XEN6" s="14"/>
+      <c r="XEO6" s="14"/>
+      <c r="XEP6" s="14"/>
+      <c r="XEQ6" s="14"/>
+      <c r="XER6" s="14"/>
+      <c r="XES6" s="14"/>
+      <c r="XET6" s="14"/>
+      <c r="XEU6" s="14"/>
+      <c r="XEV6" s="14"/>
+      <c r="XEW6" s="14"/>
+      <c r="XEX6" s="14"/>
+      <c r="XEY6" s="14"/>
+      <c r="XEZ6" s="14"/>
+      <c r="XFA6" s="14"/>
+      <c r="XFB6" s="14"/>
+      <c r="XFC6" s="14"/>
+      <c r="XFD6" s="23"/>
+    </row>
+    <row r="7" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="17" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D7" s="29" t="s">
+      <c r="C7" s="15" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="30"/>
-      <c r="S7" s="30"/>
-      <c r="T7" s="31" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U7" s="30"/>
-      <c r="V7" s="30"/>
-      <c r="W7" s="30"/>
-      <c r="X7" s="30"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="27"/>
+      <c r="T7" s="28" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U7" s="27"/>
+      <c r="V7" s="27"/>
+      <c r="W7" s="27"/>
+      <c r="X7" s="27"/>
       <c r="XEE7" s="1"/>
       <c r="XEF7" s="1"/>
       <c r="XEG7" s="1"/>
@@ -2548,57 +2627,57 @@
       <c r="XFC7" s="1"/>
       <c r="XFD7" s="1"/>
     </row>
-    <row r="8" s="18" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="29" t="s">
+    <row r="8" s="16" customFormat="true" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="17" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D8" s="29" t="s">
+      <c r="C8" s="15" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D8" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="G8" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="29" t="s">
+      <c r="H8" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="I8" s="29" t="s">
+      <c r="I8" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="J8" s="29" t="s">
+      <c r="J8" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="K8" s="29"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32" t="s">
+      <c r="K8" s="26"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="O8" s="32"/>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="32"/>
-      <c r="R8" s="32"/>
-      <c r="S8" s="32"/>
-      <c r="T8" s="31" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U8" s="32"/>
-      <c r="V8" s="32"/>
-      <c r="W8" s="32"/>
-      <c r="X8" s="32"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="29"/>
+      <c r="T8" s="28" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U8" s="29"/>
+      <c r="V8" s="29"/>
+      <c r="W8" s="29"/>
+      <c r="X8" s="29"/>
       <c r="XEE8" s="1"/>
       <c r="XEF8" s="1"/>
       <c r="XEG8" s="1"/>
@@ -2626,55 +2705,55 @@
       <c r="XFC8" s="1"/>
       <c r="XFD8" s="1"/>
     </row>
-    <row r="9" s="18" customFormat="true" ht="128.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="29" t="s">
+    <row r="9" s="16" customFormat="true" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="17" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D9" s="29" t="s">
+      <c r="C9" s="15" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D9" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="H9" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32" t="s">
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32" t="s">
+      <c r="N9" s="29"/>
+      <c r="O9" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="P9" s="32"/>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="32"/>
-      <c r="S9" s="32"/>
-      <c r="T9" s="31" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U9" s="32"/>
-      <c r="V9" s="32"/>
-      <c r="W9" s="32"/>
-      <c r="X9" s="32"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="28" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U9" s="29"/>
+      <c r="V9" s="29"/>
+      <c r="W9" s="29"/>
+      <c r="X9" s="29"/>
       <c r="XEE9" s="1"/>
       <c r="XEF9" s="1"/>
       <c r="XEG9" s="1"/>
@@ -2700,52 +2779,52 @@
       <c r="XFA9" s="1"/>
       <c r="XFB9" s="1"/>
       <c r="XFC9" s="1"/>
-      <c r="XFD9" s="0"/>
-    </row>
-    <row r="10" s="25" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="21" t="s">
+      <c r="XFD9" s="1"/>
+    </row>
+    <row r="10" s="22" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="17" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D10" s="29" t="s">
+      <c r="C10" s="15" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="24" t="str">
+      <c r="E10" s="20"/>
+      <c r="F10" s="21" t="str">
         <f aca="false">REPLACE(A10, FIND("_", A10), 1, ".")</f>
         <v>household.save</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="H10" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="21" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U10" s="23"/>
-      <c r="V10" s="23"/>
-      <c r="W10" s="23"/>
-      <c r="X10" s="23"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="19" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U10" s="20"/>
+      <c r="V10" s="20"/>
+      <c r="W10" s="20"/>
+      <c r="X10" s="20"/>
       <c r="XEE10" s="1"/>
       <c r="XEF10" s="1"/>
       <c r="XEG10" s="1"/>
@@ -2771,9 +2850,9 @@
       <c r="XFA10" s="1"/>
       <c r="XFB10" s="1"/>
       <c r="XFC10" s="1"/>
-      <c r="XFD10" s="0"/>
-    </row>
-    <row r="11" s="14" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="XFD10" s="1"/>
+    </row>
+    <row r="11" s="13" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
         <v>68</v>
       </c>
@@ -2808,7 +2887,7 @@
       <c r="Q11" s="9"/>
       <c r="R11" s="9"/>
       <c r="S11" s="9"/>
-      <c r="T11" s="13" t="b">
+      <c r="T11" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2816,70 +2895,70 @@
       <c r="V11" s="9"/>
       <c r="W11" s="9"/>
       <c r="X11" s="9"/>
-      <c r="XEE11" s="15"/>
-      <c r="XEF11" s="15"/>
-      <c r="XEG11" s="15"/>
-      <c r="XEH11" s="15"/>
-      <c r="XEI11" s="15"/>
-      <c r="XEJ11" s="15"/>
-      <c r="XEK11" s="15"/>
-      <c r="XEL11" s="15"/>
-      <c r="XEM11" s="15"/>
-      <c r="XEN11" s="15"/>
-      <c r="XEO11" s="15"/>
-      <c r="XEP11" s="15"/>
-      <c r="XEQ11" s="15"/>
-      <c r="XER11" s="15"/>
-      <c r="XES11" s="15"/>
-      <c r="XET11" s="15"/>
-      <c r="XEU11" s="15"/>
-      <c r="XEV11" s="15"/>
-      <c r="XEW11" s="15"/>
-      <c r="XEX11" s="15"/>
-      <c r="XEY11" s="15"/>
-      <c r="XEZ11" s="15"/>
-      <c r="XFA11" s="15"/>
-      <c r="XFB11" s="15"/>
-      <c r="XFC11" s="15"/>
-      <c r="XFD11" s="0"/>
-    </row>
-    <row r="12" s="18" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="27" t="s">
+      <c r="XEE11" s="14"/>
+      <c r="XEF11" s="14"/>
+      <c r="XEG11" s="14"/>
+      <c r="XEH11" s="14"/>
+      <c r="XEI11" s="14"/>
+      <c r="XEJ11" s="14"/>
+      <c r="XEK11" s="14"/>
+      <c r="XEL11" s="14"/>
+      <c r="XEM11" s="14"/>
+      <c r="XEN11" s="14"/>
+      <c r="XEO11" s="14"/>
+      <c r="XEP11" s="14"/>
+      <c r="XEQ11" s="14"/>
+      <c r="XER11" s="14"/>
+      <c r="XES11" s="14"/>
+      <c r="XET11" s="14"/>
+      <c r="XEU11" s="14"/>
+      <c r="XEV11" s="14"/>
+      <c r="XEW11" s="14"/>
+      <c r="XEX11" s="14"/>
+      <c r="XEY11" s="14"/>
+      <c r="XEZ11" s="14"/>
+      <c r="XFA11" s="14"/>
+      <c r="XFB11" s="14"/>
+      <c r="XFC11" s="14"/>
+      <c r="XFD11" s="1"/>
+    </row>
+    <row r="12" s="16" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="33" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D12" s="27" t="s">
+      <c r="C12" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D12" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="30"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="30"/>
-      <c r="R12" s="30"/>
-      <c r="S12" s="30"/>
-      <c r="T12" s="31" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U12" s="30"/>
-      <c r="V12" s="30"/>
-      <c r="W12" s="30"/>
-      <c r="X12" s="30"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27"/>
+      <c r="Q12" s="27"/>
+      <c r="R12" s="27"/>
+      <c r="S12" s="27"/>
+      <c r="T12" s="28" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U12" s="27"/>
+      <c r="V12" s="27"/>
+      <c r="W12" s="27"/>
+      <c r="X12" s="27"/>
       <c r="XEE12" s="1"/>
       <c r="XEF12" s="1"/>
       <c r="XEG12" s="1"/>
@@ -2905,53 +2984,53 @@
       <c r="XFA12" s="1"/>
       <c r="XFB12" s="1"/>
       <c r="XFC12" s="1"/>
-      <c r="XFD12" s="0"/>
-    </row>
-    <row r="13" s="18" customFormat="true" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="27" t="s">
+      <c r="XFD12" s="1"/>
+    </row>
+    <row r="13" s="16" customFormat="true" ht="137.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="33" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D13" s="27" t="s">
+      <c r="C13" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D13" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="29" t="s">
+      <c r="E13" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="F13" s="30" t="s">
+      <c r="F13" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="G13" s="29" t="s">
+      <c r="G13" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="H13" s="29" t="s">
+      <c r="H13" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="34"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="30"/>
       <c r="N13" s="1"/>
-      <c r="O13" s="30"/>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="30"/>
-      <c r="R13" s="30"/>
-      <c r="S13" s="30"/>
-      <c r="T13" s="31" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U13" s="30"/>
-      <c r="V13" s="30"/>
-      <c r="W13" s="30"/>
-      <c r="X13" s="30"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="27"/>
+      <c r="Q13" s="27"/>
+      <c r="R13" s="27"/>
+      <c r="S13" s="27"/>
+      <c r="T13" s="28" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U13" s="27"/>
+      <c r="V13" s="27"/>
+      <c r="W13" s="27"/>
+      <c r="X13" s="27"/>
       <c r="XEE13" s="1"/>
       <c r="XEF13" s="1"/>
       <c r="XEG13" s="1"/>
@@ -2977,55 +3056,55 @@
       <c r="XFA13" s="1"/>
       <c r="XFB13" s="1"/>
       <c r="XFC13" s="1"/>
-      <c r="XFD13" s="0"/>
-    </row>
-    <row r="14" s="18" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="29" t="s">
+      <c r="XFD13" s="1"/>
+    </row>
+    <row r="14" s="16" customFormat="true" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="33" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D14" s="29" t="s">
+      <c r="C14" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D14" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="E14" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="F14" s="32" t="s">
+      <c r="F14" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G14" s="29" t="s">
+      <c r="G14" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="H14" s="29" t="s">
+      <c r="H14" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="32"/>
-      <c r="N14" s="32"/>
-      <c r="O14" s="20" t="s">
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="32"/>
-      <c r="S14" s="32"/>
-      <c r="T14" s="31" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U14" s="32"/>
-      <c r="V14" s="32"/>
-      <c r="W14" s="32"/>
-      <c r="X14" s="32"/>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="29"/>
+      <c r="R14" s="29"/>
+      <c r="S14" s="29"/>
+      <c r="T14" s="28" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U14" s="29"/>
+      <c r="V14" s="29"/>
+      <c r="W14" s="29"/>
+      <c r="X14" s="29"/>
       <c r="XEE14" s="1"/>
       <c r="XEF14" s="1"/>
       <c r="XEG14" s="1"/>
@@ -3051,76 +3130,76 @@
       <c r="XFA14" s="1"/>
       <c r="XFB14" s="1"/>
       <c r="XFC14" s="1"/>
-      <c r="XFD14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="XFD14" s="1"/>
+    </row>
+    <row r="15" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="33" t="b">
+      <c r="C15" s="26" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="29" t="s">
+      <c r="E15" s="26" t="s">
         <v>72</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G15" s="29" t="s">
+      <c r="G15" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="H15" s="29" t="s">
+      <c r="H15" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="M15" s="34"/>
-      <c r="O15" s="35" t="s">
+      <c r="M15" s="30"/>
+      <c r="O15" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="T15" s="31" t="n">
+      <c r="T15" s="28" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="XFD15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="33" t="b">
+      <c r="C16" s="26" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E16" s="29"/>
+      <c r="E16" s="26"/>
       <c r="F16" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G16" s="21" t="s">
+      <c r="G16" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="H16" s="21" t="s">
+      <c r="H16" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="M16" s="34"/>
-      <c r="O16" s="35"/>
-      <c r="T16" s="31" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" s="14" customFormat="true" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M16" s="30"/>
+      <c r="O16" s="31"/>
+      <c r="T16" s="28" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" s="13" customFormat="true" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
         <v>90</v>
       </c>
@@ -3155,7 +3234,7 @@
       <c r="Q17" s="9"/>
       <c r="R17" s="9"/>
       <c r="S17" s="9"/>
-      <c r="T17" s="13" t="b">
+      <c r="T17" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3163,105 +3242,105 @@
       <c r="V17" s="9"/>
       <c r="W17" s="9"/>
       <c r="X17" s="9"/>
-      <c r="XEE17" s="15"/>
-      <c r="XEF17" s="15"/>
-      <c r="XEG17" s="15"/>
-      <c r="XEH17" s="15"/>
-      <c r="XEI17" s="15"/>
-      <c r="XEJ17" s="15"/>
-      <c r="XEK17" s="15"/>
-      <c r="XEL17" s="15"/>
-      <c r="XEM17" s="15"/>
-      <c r="XEN17" s="15"/>
-      <c r="XEO17" s="15"/>
-      <c r="XEP17" s="15"/>
-      <c r="XEQ17" s="15"/>
-      <c r="XER17" s="15"/>
-      <c r="XES17" s="15"/>
-      <c r="XET17" s="15"/>
-      <c r="XEU17" s="15"/>
-      <c r="XEV17" s="15"/>
-      <c r="XEW17" s="15"/>
-      <c r="XEX17" s="15"/>
-      <c r="XEY17" s="15"/>
-      <c r="XEZ17" s="15"/>
-      <c r="XFA17" s="15"/>
-      <c r="XFB17" s="15"/>
-      <c r="XFC17" s="15"/>
+      <c r="XEE17" s="14"/>
+      <c r="XEF17" s="14"/>
+      <c r="XEG17" s="14"/>
+      <c r="XEH17" s="14"/>
+      <c r="XEI17" s="14"/>
+      <c r="XEJ17" s="14"/>
+      <c r="XEK17" s="14"/>
+      <c r="XEL17" s="14"/>
+      <c r="XEM17" s="14"/>
+      <c r="XEN17" s="14"/>
+      <c r="XEO17" s="14"/>
+      <c r="XEP17" s="14"/>
+      <c r="XEQ17" s="14"/>
+      <c r="XER17" s="14"/>
+      <c r="XES17" s="14"/>
+      <c r="XET17" s="14"/>
+      <c r="XEU17" s="14"/>
+      <c r="XEV17" s="14"/>
+      <c r="XEW17" s="14"/>
+      <c r="XEX17" s="14"/>
+      <c r="XEY17" s="14"/>
+      <c r="XEZ17" s="14"/>
+      <c r="XFA17" s="14"/>
+      <c r="XFB17" s="14"/>
+      <c r="XFC17" s="14"/>
       <c r="XFD17" s="1"/>
     </row>
-    <row r="18" s="26" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="36" t="s">
+    <row r="18" s="23" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="37" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D18" s="36" t="s">
+      <c r="C18" s="33" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D18" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="M18" s="36"/>
-      <c r="O18" s="36"/>
-      <c r="T18" s="37" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="XFD18" s="15"/>
-    </row>
-    <row r="19" s="18" customFormat="true" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="34" t="s">
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="M18" s="32"/>
+      <c r="O18" s="32"/>
+      <c r="T18" s="33" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="XFD18" s="14"/>
+    </row>
+    <row r="19" s="16" customFormat="true" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="39" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D19" s="16" t="s">
+      <c r="C19" s="35" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D19" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="F19" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="H19" s="16" t="s">
+      <c r="H19" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
-      <c r="L19" s="40"/>
-      <c r="M19" s="40"/>
-      <c r="N19" s="40" t="s">
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="O19" s="40"/>
-      <c r="P19" s="40"/>
-      <c r="Q19" s="40"/>
-      <c r="R19" s="40"/>
-      <c r="S19" s="40"/>
-      <c r="T19" s="16" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U19" s="40"/>
-      <c r="V19" s="40"/>
-      <c r="W19" s="40"/>
-      <c r="X19" s="40"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="36"/>
+      <c r="Q19" s="36"/>
+      <c r="R19" s="36"/>
+      <c r="S19" s="36"/>
+      <c r="T19" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U19" s="36"/>
+      <c r="V19" s="36"/>
+      <c r="W19" s="36"/>
+      <c r="X19" s="36"/>
       <c r="XEE19" s="1"/>
       <c r="XEF19" s="1"/>
       <c r="XEG19" s="1"/>
@@ -3289,52 +3368,52 @@
       <c r="XFC19" s="1"/>
       <c r="XFD19" s="1"/>
     </row>
-    <row r="20" s="18" customFormat="true" ht="96.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="34" t="s">
+    <row r="20" s="16" customFormat="true" ht="96.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="39" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D20" s="16" t="s">
+      <c r="C20" s="35" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D20" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="F20" s="34" t="s">
+      <c r="F20" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="G20" s="34" t="s">
+      <c r="G20" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="H20" s="34" t="s">
+      <c r="H20" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="40"/>
-      <c r="M20" s="40"/>
-      <c r="N20" s="40"/>
-      <c r="O20" s="40"/>
-      <c r="P20" s="40"/>
-      <c r="Q20" s="40"/>
-      <c r="R20" s="40"/>
-      <c r="S20" s="40"/>
-      <c r="T20" s="16" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U20" s="40"/>
-      <c r="V20" s="40"/>
-      <c r="W20" s="40"/>
-      <c r="X20" s="40"/>
-      <c r="Y20" s="18" t="s">
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="36"/>
+      <c r="O20" s="36"/>
+      <c r="P20" s="36"/>
+      <c r="Q20" s="36"/>
+      <c r="R20" s="36"/>
+      <c r="S20" s="36"/>
+      <c r="T20" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U20" s="36"/>
+      <c r="V20" s="36"/>
+      <c r="W20" s="36"/>
+      <c r="X20" s="36"/>
+      <c r="Y20" s="16" t="s">
         <v>104</v>
       </c>
       <c r="XEE20" s="1"/>
@@ -3364,198 +3443,198 @@
       <c r="XFC20" s="1"/>
       <c r="XFD20" s="1"/>
     </row>
-    <row r="21" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="16" t="s">
+    <row r="21" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="17" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D21" s="16" t="s">
+      <c r="C21" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D21" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="G21" s="16" t="s">
+      <c r="G21" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="H21" s="16" t="s">
+      <c r="H21" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="20" t="s">
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="16"/>
-      <c r="S21" s="16"/>
-      <c r="T21" s="16" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U21" s="16"/>
-      <c r="V21" s="16"/>
-      <c r="W21" s="16"/>
-      <c r="X21" s="16"/>
-      <c r="Y21" s="18"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
+      <c r="T21" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U21" s="15"/>
+      <c r="V21" s="15"/>
+      <c r="W21" s="15"/>
+      <c r="X21" s="15"/>
+      <c r="Y21" s="16"/>
       <c r="XFD21" s="1"/>
     </row>
-    <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="41" t="s">
+    <row r="22" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="17" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D22" s="16" t="s">
+      <c r="C22" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D22" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="F22" s="16" t="s">
+      <c r="F22" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="G22" s="29" t="s">
+      <c r="G22" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="H22" s="29" t="s">
+      <c r="H22" s="26" t="s">
         <v>113</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="O22" s="41"/>
-      <c r="T22" s="31" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="41" t="s">
+      <c r="O22" s="37"/>
+      <c r="T22" s="28" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="17" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D23" s="16" t="s">
+      <c r="C23" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D23" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="E23" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="F23" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="G23" s="29" t="s">
+      <c r="G23" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="H23" s="29" t="s">
+      <c r="H23" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="M23" s="34" t="s">
+      <c r="M23" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="O23" s="42" t="s">
+      <c r="O23" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="T23" s="31" t="n">
+      <c r="T23" s="28" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="XFD23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="37" t="s">
         <v>120</v>
       </c>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="17" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D24" s="16" t="s">
+      <c r="C24" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D24" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E24" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="F24" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="G24" s="29" t="s">
+      <c r="G24" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="H24" s="29" t="s">
+      <c r="H24" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="M24" s="34" t="s">
+      <c r="M24" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="O24" s="42"/>
-      <c r="T24" s="31" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="41" t="s">
+      <c r="O24" s="38"/>
+      <c r="T24" s="28" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="17" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D25" s="16" t="s">
+      <c r="C25" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D25" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="F25" s="16" t="s">
+      <c r="F25" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="G25" s="29" t="s">
+      <c r="G25" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="H25" s="29" t="s">
+      <c r="H25" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="M25" s="34" t="s">
+      <c r="M25" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="N25" s="16" t="s">
+      <c r="N25" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="O25" s="42"/>
-      <c r="T25" s="31" t="n">
+      <c r="O25" s="38"/>
+      <c r="T25" s="28" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3563,40 +3642,40 @@
         <v>130</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="41" t="s">
+    <row r="26" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="17" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D26" s="16" t="s">
+      <c r="C26" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D26" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="E26" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="F26" s="16" t="s">
+      <c r="F26" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="G26" s="29" t="s">
+      <c r="G26" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="H26" s="29" t="s">
+      <c r="H26" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="K26" s="16"/>
-      <c r="M26" s="34" t="s">
+      <c r="K26" s="15"/>
+      <c r="M26" s="30" t="s">
         <v>124</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="T26" s="31" t="n">
+      <c r="T26" s="28" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3607,119 +3686,119 @@
         <v>136</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="41" t="s">
+    <row r="27" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="17" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D27" s="16" t="s">
+      <c r="C27" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D27" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="G27" s="29" t="s">
+      <c r="G27" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="H27" s="29" t="s">
+      <c r="H27" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="K27" s="16"/>
-      <c r="M27" s="34" t="s">
+      <c r="K27" s="15"/>
+      <c r="M27" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="T27" s="31" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T27" s="28" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="17" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D28" s="16" t="s">
+      <c r="C28" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D28" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E28" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="F28" s="16" t="s">
+      <c r="F28" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="G28" s="29" t="s">
+      <c r="G28" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="H28" s="29" t="s">
+      <c r="H28" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="M28" s="34" t="s">
+      <c r="M28" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="T28" s="31" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" s="25" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="21" t="s">
+      <c r="T28" s="28" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" s="22" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="22" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D29" s="21" t="s">
+      <c r="C29" s="19" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D29" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="E29" s="23"/>
-      <c r="F29" s="24" t="str">
+      <c r="E29" s="20"/>
+      <c r="F29" s="21" t="str">
         <f aca="false">REPLACE(A29, FIND("_", A29), 1, ".")</f>
         <v>addresses.save</v>
       </c>
-      <c r="G29" s="21" t="s">
+      <c r="G29" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="H29" s="21" t="s">
+      <c r="H29" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="21"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="23"/>
-      <c r="Q29" s="23"/>
-      <c r="R29" s="23"/>
-      <c r="S29" s="23"/>
-      <c r="T29" s="21" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U29" s="23"/>
-      <c r="V29" s="23"/>
-      <c r="W29" s="23"/>
-      <c r="X29" s="23"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="20"/>
+      <c r="P29" s="20"/>
+      <c r="Q29" s="20"/>
+      <c r="R29" s="20"/>
+      <c r="S29" s="20"/>
+      <c r="T29" s="19" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U29" s="20"/>
+      <c r="V29" s="20"/>
+      <c r="W29" s="20"/>
+      <c r="X29" s="20"/>
       <c r="XEE29" s="1"/>
       <c r="XEF29" s="1"/>
       <c r="XEG29" s="1"/>
@@ -3745,16 +3824,16 @@
       <c r="XFA29" s="1"/>
       <c r="XFB29" s="1"/>
       <c r="XFC29" s="1"/>
-      <c r="XFD29" s="0"/>
-    </row>
-    <row r="30" s="14" customFormat="true" ht="229.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="XFD29" s="1"/>
+    </row>
+    <row r="30" s="13" customFormat="true" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="39" t="n">
+      <c r="C30" s="35" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3782,7 +3861,7 @@
       <c r="Q30" s="9"/>
       <c r="R30" s="9"/>
       <c r="S30" s="9"/>
-      <c r="T30" s="13" t="b">
+      <c r="T30" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3790,99 +3869,99 @@
       <c r="V30" s="9"/>
       <c r="W30" s="9"/>
       <c r="X30" s="9"/>
-      <c r="XEE30" s="15"/>
-      <c r="XEF30" s="15"/>
-      <c r="XEG30" s="15"/>
-      <c r="XEH30" s="15"/>
-      <c r="XEI30" s="15"/>
-      <c r="XEJ30" s="15"/>
-      <c r="XEK30" s="15"/>
-      <c r="XEL30" s="15"/>
-      <c r="XEM30" s="15"/>
-      <c r="XEN30" s="15"/>
-      <c r="XEO30" s="15"/>
-      <c r="XEP30" s="15"/>
-      <c r="XEQ30" s="15"/>
-      <c r="XER30" s="15"/>
-      <c r="XES30" s="15"/>
-      <c r="XET30" s="15"/>
-      <c r="XEU30" s="15"/>
-      <c r="XEV30" s="15"/>
-      <c r="XEW30" s="15"/>
-      <c r="XEX30" s="15"/>
-      <c r="XEY30" s="15"/>
-      <c r="XEZ30" s="15"/>
-      <c r="XFA30" s="15"/>
-      <c r="XFB30" s="15"/>
-      <c r="XFC30" s="15"/>
-      <c r="XFD30" s="0"/>
+      <c r="XEE30" s="14"/>
+      <c r="XEF30" s="14"/>
+      <c r="XEG30" s="14"/>
+      <c r="XEH30" s="14"/>
+      <c r="XEI30" s="14"/>
+      <c r="XEJ30" s="14"/>
+      <c r="XEK30" s="14"/>
+      <c r="XEL30" s="14"/>
+      <c r="XEM30" s="14"/>
+      <c r="XEN30" s="14"/>
+      <c r="XEO30" s="14"/>
+      <c r="XEP30" s="14"/>
+      <c r="XEQ30" s="14"/>
+      <c r="XER30" s="14"/>
+      <c r="XES30" s="14"/>
+      <c r="XET30" s="14"/>
+      <c r="XEU30" s="14"/>
+      <c r="XEV30" s="14"/>
+      <c r="XEW30" s="14"/>
+      <c r="XEX30" s="14"/>
+      <c r="XEY30" s="14"/>
+      <c r="XEZ30" s="14"/>
+      <c r="XFA30" s="14"/>
+      <c r="XFB30" s="14"/>
+      <c r="XFC30" s="14"/>
+      <c r="XFD30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="17" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D31" s="34" t="s">
+      <c r="C31" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D31" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="T31" s="16" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" s="18" customFormat="true" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="34" t="s">
+      <c r="T31" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" s="16" customFormat="true" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="30" t="s">
         <v>152</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="C32" s="39" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D32" s="16" t="s">
+      <c r="C32" s="35" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D32" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="E32" s="16" t="s">
+      <c r="E32" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="F32" s="16" t="s">
+      <c r="F32" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="G32" s="16" t="s">
+      <c r="G32" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="H32" s="16" t="s">
+      <c r="H32" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="I32" s="38"/>
-      <c r="J32" s="38"/>
-      <c r="K32" s="38"/>
-      <c r="L32" s="40"/>
-      <c r="M32" s="40"/>
-      <c r="N32" s="40" t="s">
+      <c r="I32" s="34"/>
+      <c r="J32" s="34"/>
+      <c r="K32" s="34"/>
+      <c r="L32" s="36"/>
+      <c r="M32" s="36"/>
+      <c r="N32" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="O32" s="40"/>
-      <c r="P32" s="40"/>
-      <c r="Q32" s="40"/>
-      <c r="R32" s="40"/>
-      <c r="S32" s="40"/>
-      <c r="T32" s="16" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U32" s="40"/>
-      <c r="V32" s="40"/>
-      <c r="W32" s="40"/>
-      <c r="X32" s="40"/>
+      <c r="O32" s="36"/>
+      <c r="P32" s="36"/>
+      <c r="Q32" s="36"/>
+      <c r="R32" s="36"/>
+      <c r="S32" s="36"/>
+      <c r="T32" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U32" s="36"/>
+      <c r="V32" s="36"/>
+      <c r="W32" s="36"/>
+      <c r="X32" s="36"/>
       <c r="XEE32" s="1"/>
       <c r="XEF32" s="1"/>
       <c r="XEG32" s="1"/>
@@ -3908,54 +3987,54 @@
       <c r="XFA32" s="1"/>
       <c r="XFB32" s="1"/>
       <c r="XFC32" s="1"/>
-      <c r="XFD32" s="0"/>
-    </row>
-    <row r="33" s="18" customFormat="true" ht="96.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="34" t="s">
+      <c r="XFD32" s="1"/>
+    </row>
+    <row r="33" s="16" customFormat="true" ht="96.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="39" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D33" s="16" t="s">
+      <c r="C33" s="35" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D33" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="E33" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="F33" s="34" t="s">
+      <c r="F33" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="G33" s="34" t="s">
+      <c r="G33" s="30" t="s">
         <v>156</v>
       </c>
-      <c r="H33" s="34" t="s">
+      <c r="H33" s="30" t="s">
         <v>157</v>
       </c>
-      <c r="I33" s="38"/>
-      <c r="J33" s="38"/>
-      <c r="K33" s="38"/>
-      <c r="L33" s="40"/>
-      <c r="M33" s="40"/>
-      <c r="N33" s="40"/>
-      <c r="O33" s="40"/>
-      <c r="P33" s="32"/>
-      <c r="Q33" s="32"/>
-      <c r="R33" s="32"/>
-      <c r="S33" s="32"/>
-      <c r="T33" s="16" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U33" s="32"/>
-      <c r="V33" s="32"/>
-      <c r="W33" s="32"/>
-      <c r="X33" s="32"/>
-      <c r="Y33" s="18" t="s">
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="34"/>
+      <c r="L33" s="36"/>
+      <c r="M33" s="36"/>
+      <c r="N33" s="36"/>
+      <c r="O33" s="36"/>
+      <c r="P33" s="29"/>
+      <c r="Q33" s="29"/>
+      <c r="R33" s="29"/>
+      <c r="S33" s="29"/>
+      <c r="T33" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U33" s="29"/>
+      <c r="V33" s="29"/>
+      <c r="W33" s="29"/>
+      <c r="X33" s="29"/>
+      <c r="Y33" s="16" t="s">
         <v>104</v>
       </c>
       <c r="XEE33" s="1"/>
@@ -3983,87 +4062,87 @@
       <c r="XFA33" s="1"/>
       <c r="XFB33" s="1"/>
       <c r="XFC33" s="1"/>
-      <c r="XFD33" s="0"/>
-    </row>
-    <row r="34" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="XFD33" s="1"/>
+    </row>
+    <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B34" s="29" t="s">
+      <c r="B34" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="43" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D34" s="16" t="s">
+      <c r="C34" s="39" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D34" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="E34" s="16" t="s">
+      <c r="E34" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="F34" s="16" t="s">
+      <c r="F34" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="G34" s="29" t="s">
+      <c r="G34" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="H34" s="29" t="s">
+      <c r="H34" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="K34" s="16" t="s">
+      <c r="K34" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="M34" s="34"/>
-      <c r="T34" s="16" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" s="25" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="21" t="s">
+      <c r="M34" s="30"/>
+      <c r="T34" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" s="22" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="22" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D35" s="16" t="s">
+      <c r="C35" s="19" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D35" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="24" t="str">
+      <c r="E35" s="20"/>
+      <c r="F35" s="21" t="str">
         <f aca="false">REPLACE(A35, FIND("_", A35), 1, ".")</f>
         <v>destinations.save</v>
       </c>
-      <c r="G35" s="21" t="s">
+      <c r="G35" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="H35" s="21" t="s">
+      <c r="H35" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="21"/>
-      <c r="L35" s="23"/>
-      <c r="M35" s="23"/>
-      <c r="N35" s="23"/>
-      <c r="O35" s="23"/>
-      <c r="P35" s="23"/>
-      <c r="Q35" s="23"/>
-      <c r="R35" s="23"/>
-      <c r="S35" s="23"/>
-      <c r="T35" s="21" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U35" s="23"/>
-      <c r="V35" s="23"/>
-      <c r="W35" s="23"/>
-      <c r="X35" s="23"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="20"/>
+      <c r="M35" s="20"/>
+      <c r="N35" s="20"/>
+      <c r="O35" s="20"/>
+      <c r="P35" s="20"/>
+      <c r="Q35" s="20"/>
+      <c r="R35" s="20"/>
+      <c r="S35" s="20"/>
+      <c r="T35" s="19" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U35" s="20"/>
+      <c r="V35" s="20"/>
+      <c r="W35" s="20"/>
+      <c r="X35" s="20"/>
       <c r="XEE35" s="1"/>
       <c r="XEF35" s="1"/>
       <c r="XEG35" s="1"/>
@@ -4089,23 +4168,23 @@
       <c r="XFA35" s="1"/>
       <c r="XFB35" s="1"/>
       <c r="XFC35" s="1"/>
-      <c r="XFD35" s="0"/>
+      <c r="XFD35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="39" t="n">
+      <c r="C36" s="35" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="F36" s="16" t="s">
+      <c r="F36" s="15" t="s">
         <v>164</v>
       </c>
       <c r="G36" s="2" t="s">
@@ -4114,7 +4193,7 @@
       <c r="H36" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="T36" s="16" t="n">
+      <c r="T36" s="15" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4126,7 +4205,7 @@
       <c r="B37" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="39" t="n">
+      <c r="C37" s="35" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4150,7 +4229,7 @@
       <c r="B38" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="39" t="n">
+      <c r="C38" s="35" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4168,7 +4247,7 @@
       <c r="B39" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="39" t="n">
+      <c r="C39" s="35" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4178,16 +4257,16 @@
       <c r="E39" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F39" s="44" t="s">
+      <c r="F39" s="40" t="s">
         <v>173</v>
       </c>
-      <c r="G39" s="34" t="s">
+      <c r="G39" s="30" t="s">
         <v>174</v>
       </c>
-      <c r="H39" s="34" t="s">
+      <c r="H39" s="30" t="s">
         <v>175</v>
       </c>
-      <c r="T39" s="31" t="n">
+      <c r="T39" s="28" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4202,7 +4281,7 @@
       <c r="B40" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C40" s="39" t="n">
+      <c r="C40" s="35" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4212,16 +4291,16 @@
       <c r="E40" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F40" s="44" t="s">
+      <c r="F40" s="40" t="s">
         <v>178</v>
       </c>
-      <c r="G40" s="34" t="s">
+      <c r="G40" s="30" t="s">
         <v>179</v>
       </c>
-      <c r="H40" s="34" t="s">
+      <c r="H40" s="30" t="s">
         <v>180</v>
       </c>
-      <c r="T40" s="31"/>
+      <c r="T40" s="28"/>
       <c r="Y40" s="1"/>
     </row>
     <row r="41" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4231,7 +4310,7 @@
       <c r="B41" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C41" s="39" t="n">
+      <c r="C41" s="35" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4241,16 +4320,16 @@
       <c r="E41" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F41" s="44" t="s">
+      <c r="F41" s="40" t="s">
         <v>182</v>
       </c>
-      <c r="G41" s="34" t="s">
+      <c r="G41" s="30" t="s">
         <v>183</v>
       </c>
-      <c r="H41" s="34" t="s">
+      <c r="H41" s="30" t="s">
         <v>184</v>
       </c>
-      <c r="T41" s="31"/>
+      <c r="T41" s="28"/>
       <c r="Y41" s="1"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4260,7 +4339,7 @@
       <c r="B42" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C42" s="39" t="n">
+      <c r="C42" s="35" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4270,7 +4349,7 @@
       <c r="E42" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F42" s="34" t="s">
+      <c r="F42" s="30" t="s">
         <v>186</v>
       </c>
       <c r="G42" s="2" t="s">
@@ -4287,7 +4366,7 @@
       <c r="B43" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C43" s="39" t="n">
+      <c r="C43" s="35" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4311,10 +4390,10 @@
       <c r="A44" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="C44" s="39" t="n">
+      <c r="C44" s="35" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4338,10 +4417,10 @@
       <c r="A45" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="C45" s="39" t="n">
+      <c r="C45" s="35" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4396,52 +4475,52 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="34" width="38.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="34" width="15.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="34" width="31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="45" width="20.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="34" width="19.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="34" width="12.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="34" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="38.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="15.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="30" width="31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="41" width="20.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="30" width="19.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="30" width="12.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="30" width="8.59"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="46" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="42" t="s">
         <v>200</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="42" t="s">
         <v>201</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="43" t="s">
         <v>202</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="42" t="s">
         <v>203</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="42" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="30" t="s">
         <v>205</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="44" t="s">
         <v>206</v>
       </c>
-      <c r="E2" s="34" t="n">
+      <c r="E2" s="30" t="n">
         <v>16</v>
       </c>
     </row>
@@ -4682,196 +4761,196 @@
       <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="34" width="10.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="34" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="34" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="34" width="12.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="34" width="10.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="34" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="34" width="15.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="34" width="10.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="10.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="30" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="30" width="12.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="30" width="10.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="30" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="30" width="15.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="30" width="10.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="46" t="s">
         <v>207</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="45" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="45" t="s">
         <v>209</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="45" t="s">
         <v>210</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="45" t="s">
         <v>211</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="H1" s="45" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="30" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="30" t="s">
         <v>215</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="30" t="s">
         <v>216</v>
       </c>
-      <c r="E2" s="51" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F2" s="51" t="b">
+      <c r="E2" s="47" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="47" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G2" s="51" t="b">
+      <c r="G2" s="47" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="30" t="s">
         <v>217</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="30" t="s">
         <v>218</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="30" t="s">
         <v>219</v>
       </c>
-      <c r="E3" s="51" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F3" s="51" t="b">
+      <c r="E3" s="47" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="47" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G3" s="51" t="b">
+      <c r="G3" s="47" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="30" t="s">
         <v>220</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="30" t="s">
         <v>221</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="30" t="s">
         <v>222</v>
       </c>
-      <c r="E4" s="51" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F4" s="51" t="b">
+      <c r="E4" s="47" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="47" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G4" s="51" t="b">
+      <c r="G4" s="47" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="30" t="s">
         <v>223</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="30" t="s">
         <v>224</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="30" t="s">
         <v>225</v>
       </c>
-      <c r="E5" s="51" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F5" s="51" t="b">
+      <c r="E5" s="47" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="47" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G5" s="51" t="b">
+      <c r="G5" s="47" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="30" t="s">
         <v>226</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="30" t="s">
         <v>227</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="30" t="s">
         <v>228</v>
       </c>
-      <c r="E6" s="51" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F6" s="51" t="b">
+      <c r="E6" s="47" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="47" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G6" s="51" t="b">
+      <c r="G6" s="47" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="30" t="s">
         <v>229</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="30" t="s">
         <v>230</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="30" t="s">
         <v>231</v>
       </c>
-      <c r="E7" s="51" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F7" s="51" t="b">
+      <c r="E7" s="47" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="47" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G7" s="51" t="b">
+      <c r="G7" s="47" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5067,385 +5146,385 @@
       <selection pane="topLeft" activeCell="G42" activeCellId="0" sqref="G42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="29.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="35" width="19.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="35" width="30.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="35" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="35" width="24.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="35" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="29.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="19.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="31" width="30.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="31" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="31" width="24.29"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="31" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="48" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="48" t="s">
         <v>203</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="48" t="s">
         <v>233</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="31" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="38" t="s">
         <v>235</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="38" t="s">
         <v>235</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="38" t="s">
         <v>236</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="38" t="s">
         <v>238</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="38" t="s">
         <v>238</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="38" t="s">
         <v>239</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="38" t="s">
         <v>240</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="38" t="s">
         <v>241</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="38" t="s">
         <v>241</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="38" t="s">
         <v>242</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="38" t="s">
         <v>244</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="38" t="s">
         <v>241</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="38" t="s">
         <v>245</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="38" t="s">
         <v>246</v>
       </c>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="38" t="s">
         <v>247</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="38" t="s">
         <v>247</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="38" t="s">
         <v>248</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="38" t="s">
         <v>249</v>
       </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="38" t="s">
         <v>250</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="38" t="s">
         <v>250</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="38" t="s">
         <v>251</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="38" t="s">
         <v>252</v>
       </c>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42" t="s">
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38" t="s">
         <v>235</v>
       </c>
-      <c r="H8" s="42"/>
+      <c r="H8" s="38"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42" t="s">
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38" t="s">
         <v>238</v>
       </c>
-      <c r="H9" s="42"/>
+      <c r="H9" s="38"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42" t="s">
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="H10" s="42"/>
+      <c r="H10" s="38"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42" t="s">
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38" t="s">
         <v>247</v>
       </c>
-      <c r="H11" s="42"/>
+      <c r="H11" s="38"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="38" t="s">
         <v>253</v>
       </c>
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42" t="s">
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38" t="s">
         <v>235</v>
       </c>
-      <c r="H12" s="42"/>
+      <c r="H12" s="38"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="38" t="s">
         <v>253</v>
       </c>
-      <c r="B13" s="42"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42" t="s">
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38" t="s">
         <v>238</v>
       </c>
-      <c r="H13" s="42"/>
+      <c r="H13" s="38"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="38" t="s">
         <v>253</v>
       </c>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42" t="s">
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38" t="s">
         <v>250</v>
       </c>
-      <c r="H14" s="42"/>
+      <c r="H14" s="38"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="54" t="s">
+      <c r="A15" s="50" t="s">
         <v>254</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="38" t="s">
         <v>255</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="38" t="s">
         <v>256</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="38" t="s">
         <v>257</v>
       </c>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="54" t="s">
+      <c r="A16" s="50" t="s">
         <v>254</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="38" t="s">
         <v>258</v>
       </c>
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="38" t="s">
         <v>259</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="38" t="s">
         <v>260</v>
       </c>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="54" t="s">
+      <c r="A17" s="50" t="s">
         <v>254</v>
       </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42" t="s">
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38" t="s">
         <v>250</v>
       </c>
-      <c r="H17" s="42"/>
+      <c r="H17" s="38"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="54" t="s">
+      <c r="A18" s="50" t="s">
         <v>261</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="38" t="s">
         <v>255</v>
       </c>
-      <c r="C18" s="42" t="s">
+      <c r="C18" s="38" t="s">
         <v>256</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="38" t="s">
         <v>262</v>
       </c>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="54" t="s">
+      <c r="A19" s="50" t="s">
         <v>261</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="38" t="s">
         <v>258</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="38" t="s">
         <v>259</v>
       </c>
-      <c r="D19" s="42" t="s">
+      <c r="D19" s="38" t="s">
         <v>263</v>
       </c>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="54" t="s">
+      <c r="A20" s="50" t="s">
         <v>261</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="38" t="s">
         <v>264</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="38" t="s">
         <v>265</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="38" t="s">
         <v>266</v>
       </c>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="54" t="s">
+      <c r="A21" s="50" t="s">
         <v>261</v>
       </c>
-      <c r="B21" s="42"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42" t="s">
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38" t="s">
         <v>250</v>
       </c>
-      <c r="H21" s="42"/>
+      <c r="H21" s="38"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="31" t="s">
         <v>267</v>
       </c>
-      <c r="C22" s="35" t="s">
+      <c r="C22" s="31" t="s">
         <v>268</v>
       </c>
-      <c r="D22" s="35" t="s">
+      <c r="D22" s="31" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="31" t="s">
         <v>41</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -5461,7 +5540,7 @@
       <c r="F23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="31" t="s">
         <v>41</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -5477,7 +5556,7 @@
       <c r="F24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="31" t="s">
         <v>41</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -5493,7 +5572,7 @@
       <c r="F25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="31" t="s">
         <v>41</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -5509,7 +5588,7 @@
       <c r="F26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="31" t="s">
         <v>41</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -5525,7 +5604,7 @@
       <c r="F27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="31" t="s">
         <v>41</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -5541,7 +5620,7 @@
       <c r="F28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="31" t="s">
         <v>41</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -5557,7 +5636,7 @@
       <c r="F29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="31" t="s">
         <v>41</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -5573,7 +5652,7 @@
       <c r="F30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="31" t="s">
         <v>41</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -5589,7 +5668,7 @@
       <c r="F31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="31" t="s">
         <v>41</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -5605,7 +5684,7 @@
       <c r="F32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="35" t="s">
+      <c r="A33" s="31" t="s">
         <v>41</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -5621,184 +5700,184 @@
       <c r="F33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="35" t="s">
+      <c r="A34" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="31" t="s">
         <v>303</v>
       </c>
-      <c r="C34" s="35" t="s">
+      <c r="C34" s="31" t="s">
         <v>304</v>
       </c>
-      <c r="D34" s="35" t="s">
+      <c r="D34" s="31" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="35" t="s">
+      <c r="B35" s="31" t="s">
         <v>247</v>
       </c>
-      <c r="C35" s="35" t="s">
+      <c r="C35" s="31" t="s">
         <v>306</v>
       </c>
-      <c r="D35" s="35" t="s">
+      <c r="D35" s="31" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="35" t="s">
+      <c r="A36" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="35" t="s">
+      <c r="B36" s="31" t="s">
         <v>308</v>
       </c>
-      <c r="C36" s="35" t="s">
+      <c r="C36" s="31" t="s">
         <v>309</v>
       </c>
-      <c r="D36" s="35" t="s">
+      <c r="D36" s="31" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="35" t="s">
+      <c r="A37" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="B37" s="35" t="s">
+      <c r="B37" s="31" t="s">
         <v>311</v>
       </c>
-      <c r="C37" s="35" t="s">
+      <c r="C37" s="31" t="s">
         <v>312</v>
       </c>
-      <c r="D37" s="35" t="s">
+      <c r="D37" s="31" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="35" t="s">
+      <c r="A38" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="B38" s="35" t="s">
+      <c r="B38" s="31" t="s">
         <v>314</v>
       </c>
-      <c r="C38" s="35" t="s">
+      <c r="C38" s="31" t="s">
         <v>315</v>
       </c>
-      <c r="D38" s="35" t="s">
+      <c r="D38" s="31" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="35" t="s">
+      <c r="A39" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="35" t="s">
+      <c r="B39" s="31" t="s">
         <v>317</v>
       </c>
-      <c r="C39" s="35" t="s">
+      <c r="C39" s="31" t="s">
         <v>318</v>
       </c>
-      <c r="D39" s="35" t="s">
+      <c r="D39" s="31" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="35" t="s">
+      <c r="A40" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="B40" s="35" t="s">
+      <c r="B40" s="31" t="s">
         <v>320</v>
       </c>
-      <c r="C40" s="35" t="s">
+      <c r="C40" s="31" t="s">
         <v>321</v>
       </c>
-      <c r="D40" s="35" t="s">
+      <c r="D40" s="31" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="B41" s="35" t="s">
+      <c r="B41" s="31" t="s">
         <v>323</v>
       </c>
-      <c r="C41" s="35" t="s">
+      <c r="C41" s="31" t="s">
         <v>324</v>
       </c>
-      <c r="D41" s="35" t="s">
+      <c r="D41" s="31" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="35" t="s">
+      <c r="A42" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="G42" s="42" t="s">
+      <c r="G42" s="38" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="35" t="s">
+      <c r="A43" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="B43" s="35" t="s">
+      <c r="B43" s="31" t="s">
         <v>326</v>
       </c>
-      <c r="C43" s="35" t="s">
+      <c r="C43" s="31" t="s">
         <v>327</v>
       </c>
-      <c r="D43" s="35" t="s">
+      <c r="D43" s="31" t="s">
         <v>328</v>
       </c>
-      <c r="H43" s="34"/>
+      <c r="H43" s="30"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="35" t="s">
+      <c r="A44" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="B44" s="35" t="s">
+      <c r="B44" s="31" t="s">
         <v>329</v>
       </c>
-      <c r="C44" s="35" t="s">
+      <c r="C44" s="31" t="s">
         <v>330</v>
       </c>
-      <c r="D44" s="35" t="s">
+      <c r="D44" s="31" t="s">
         <v>331</v>
       </c>
-      <c r="H44" s="34"/>
+      <c r="H44" s="30"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="B45" s="35" t="s">
+      <c r="B45" s="31" t="s">
         <v>332</v>
       </c>
-      <c r="C45" s="35" t="s">
+      <c r="C45" s="31" t="s">
         <v>333</v>
       </c>
-      <c r="D45" s="35" t="s">
+      <c r="D45" s="31" t="s">
         <v>334</v>
       </c>
-      <c r="H45" s="34"/>
+      <c r="H45" s="30"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="35" t="s">
+      <c r="A46" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="B46" s="35" t="s">
+      <c r="B46" s="31" t="s">
         <v>335</v>
       </c>
-      <c r="C46" s="35" t="s">
+      <c r="C46" s="31" t="s">
         <v>336</v>
       </c>
-      <c r="D46" s="35" t="s">
+      <c r="D46" s="31" t="s">
         <v>337</v>
       </c>
-      <c r="H46" s="34"/>
+      <c r="H46" s="30"/>
     </row>
     <row r="1048398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -6001,7 +6080,7 @@
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.71"/>
@@ -6015,193 +6094,193 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="24.39"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="55" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="51" t="s">
         <v>338</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="51" t="s">
         <v>339</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="51" t="s">
         <v>340</v>
       </c>
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="51" t="s">
         <v>341</v>
       </c>
-      <c r="E1" s="55" t="s">
+      <c r="E1" s="51" t="s">
         <v>342</v>
       </c>
-      <c r="F1" s="55" t="s">
+      <c r="F1" s="51" t="s">
         <v>343</v>
       </c>
-      <c r="G1" s="55" t="s">
+      <c r="G1" s="51" t="s">
         <v>344</v>
       </c>
-      <c r="H1" s="55" t="s">
+      <c r="H1" s="51" t="s">
         <v>345</v>
       </c>
-      <c r="I1" s="55" t="s">
+      <c r="I1" s="51" t="s">
         <v>346</v>
       </c>
-      <c r="J1" s="55" t="s">
+      <c r="J1" s="51" t="s">
         <v>347</v>
       </c>
-      <c r="K1" s="55" t="s">
+      <c r="K1" s="51" t="s">
         <v>348</v>
       </c>
-      <c r="L1" s="56" t="s">
+      <c r="L1" s="52" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="18" t="s">
         <v>350</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="18" t="s">
         <v>351</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="18" t="s">
         <v>352</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="18" t="s">
         <v>353</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="18" t="s">
         <v>354</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="18" t="s">
         <v>355</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="18" t="s">
         <v>356</v>
       </c>
-      <c r="H2" s="20" t="n">
+      <c r="H2" s="18" t="n">
         <v>-10</v>
       </c>
-      <c r="I2" s="20" t="n">
+      <c r="I2" s="18" t="n">
         <v>100</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="18" t="s">
         <v>357</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="18" t="s">
         <v>357</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="18" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="18" t="s">
         <v>359</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="18" t="s">
         <v>360</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="18" t="s">
         <v>361</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="D3" s="53" t="s">
         <v>362</v>
       </c>
-      <c r="E3" s="57" t="s">
+      <c r="E3" s="53" t="s">
         <v>363</v>
       </c>
-      <c r="F3" s="57" t="s">
+      <c r="F3" s="53" t="s">
         <v>364</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="18" t="s">
         <v>365</v>
       </c>
-      <c r="H3" s="20" t="n">
+      <c r="H3" s="18" t="n">
         <v>-10</v>
       </c>
-      <c r="I3" s="20" t="n">
+      <c r="I3" s="18" t="n">
         <v>100</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="18" t="s">
         <v>357</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="18" t="s">
         <v>357</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="18" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="18" t="s">
         <v>367</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="18" t="s">
         <v>368</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="18" t="s">
         <v>369</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="18" t="s">
         <v>370</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="18" t="s">
         <v>371</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="18" t="s">
         <v>372</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="18" t="s">
         <v>373</v>
       </c>
-      <c r="H4" s="20" t="n">
+      <c r="H4" s="18" t="n">
         <v>-10</v>
       </c>
-      <c r="I4" s="20" t="n">
+      <c r="I4" s="18" t="n">
         <v>100</v>
       </c>
-      <c r="J4" s="20" t="s">
+      <c r="J4" s="18" t="s">
         <v>357</v>
       </c>
-      <c r="K4" s="20" t="s">
+      <c r="K4" s="18" t="s">
         <v>357</v>
       </c>
-      <c r="L4" s="20" t="s">
+      <c r="L4" s="18" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>374</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="18" t="s">
         <v>360</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="18" t="s">
         <v>375</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="18" t="s">
         <v>376</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="18" t="s">
         <v>363</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="18" t="s">
         <v>377</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="18" t="s">
         <v>378</v>
       </c>
-      <c r="H5" s="20" t="n">
+      <c r="H5" s="18" t="n">
         <v>-10</v>
       </c>
-      <c r="I5" s="20" t="n">
+      <c r="I5" s="18" t="n">
         <v>100</v>
       </c>
-      <c r="J5" s="20" t="s">
+      <c r="J5" s="18" t="s">
         <v>357</v>
       </c>
-      <c r="K5" s="20" t="s">
+      <c r="K5" s="18" t="s">
         <v>357</v>
       </c>
-      <c r="L5" s="20" t="s">
+      <c r="L5" s="18" t="s">
         <v>358</v>
       </c>
     </row>
@@ -6335,18 +6414,18 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="33.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -6387,10 +6466,10 @@
       <c r="B3" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="30" t="s">
         <v>383</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="30" t="s">
         <v>384</v>
       </c>
     </row>
@@ -6415,14 +6494,14 @@
       <c r="B5" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="30" t="s">
         <v>387</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="30" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>148</v>
       </c>
@@ -6443,10 +6522,10 @@
       <c r="B7" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="30" t="s">
         <v>391</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="30" t="s">
         <v>392</v>
       </c>
     </row>
@@ -6454,7 +6533,7 @@
       <c r="A8" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="30" t="s">
         <v>393</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -6474,7 +6553,7 @@
       <c r="A9" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="30" t="s">
         <v>396</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -6491,10 +6570,10 @@
       <c r="B10" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="30" t="s">
         <v>227</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="30" t="s">
         <v>399</v>
       </c>
     </row>
@@ -6502,10 +6581,10 @@
       <c r="A11" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="30" t="s">
         <v>400</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="30" t="s">
         <v>401</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -6572,14 +6651,42 @@
       <c r="A16" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="30" t="s">
         <v>414</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="30" t="s">
         <v>416</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>417</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>418</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>420</v>
+      </c>
+      <c r="C18" s="54" t="s">
+        <v>421</v>
+      </c>
+      <c r="D18" s="54" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="1048376" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Make the cars nickname question optional.
Also add a helper function that will return the nickname if one was entered, and if it doesn't return a label that will depend on both the language and the car's number.
Fix: #38
</commit_message>
<xml_diff>
--- a/localisation/references/questionnaireLocalisation.xlsx
+++ b/localisation/references/questionnaireLocalisation.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="426">
   <si>
     <t xml:space="preserve">questionName</t>
   </si>
@@ -262,11 +262,14 @@
   </si>
   <si>
     <t xml:space="preserve">**Modèle ou surnom** pour identifier cette voiture pour la suite de l'entrevue
-__Peut être la marque de la voiture, son rôle (ex: 'Voiture principale', 'Voiture de maman'), ou tout autre appellation qui permet de l’identifier.__</t>
+__Peut être la marque de la voiture, son rôle (ex: 'Voiture principale', 'Voiture de maman'), ou tout autre appellation qui permet de l’identifier. Optionnel.__</t>
   </si>
   <si>
     <t xml:space="preserve">**Model or nickname** that will allow you to identify this car for the remainder of the interview
-__Can be the brand of the car, its role (ex: 'Primary car', 'Mom’s car'), or any other designation that will allow you to identify it.__</t>
+__Can be the brand of the car, its role (ex: 'Primary car', 'Mom’s car'), or any other designation that will allow you to identify it. Optional.__</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optionalValidation</t>
   </si>
   <si>
     <t xml:space="preserve">carCategory</t>
@@ -334,9 +337,6 @@
   </si>
   <si>
     <t xml:space="preserve">Name or address of the home</t>
-  </si>
-  <si>
-    <t xml:space="preserve">optionalValidation</t>
   </si>
   <si>
     <t xml:space="preserve">addressGeography</t>
@@ -1220,6 +1220,15 @@
     <t xml:space="preserve">Delete this car</t>
   </si>
   <si>
+    <t xml:space="preserve">numberedCar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voiture {{number}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Car {{number}}</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ajouter une destination manquante</t>
   </si>
   <si>
@@ -1317,91 +1326,28 @@
 -</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">monthlyCost.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">totalCostMonthly</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Null</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Coût mensuel total
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Total Monthly Cost
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">-</t>
-    </r>
+    <t xml:space="preserve">monthlyCost.totalCostMonthlyNull</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coût mensuel total
+-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Monthly Cost
+-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;VRAI&quot;;&quot;VRAI&quot;;&quot;FAUX&quot;"/>
-    <numFmt numFmtId="166" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="General"/>
+    <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1536,12 +1482,6 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1633,7 +1573,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1686,6 +1626,10 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1695,6 +1639,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1714,11 +1662,15 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1754,8 +1706,16 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1778,10 +1738,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1798,7 +1754,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1806,11 +1762,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1822,7 +1778,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1848,10 +1804,6 @@
     </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2156,14 +2108,14 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="L17" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H4" activeCellId="0" sqref="H4"/>
+      <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="L13" activeCellId="0" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.29"/>
@@ -2176,7 +2128,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="10.91"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2253,7 +2205,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" s="13" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="14" customFormat="true" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
@@ -2288,7 +2240,7 @@
       <c r="Q2" s="9"/>
       <c r="R2" s="9"/>
       <c r="S2" s="9"/>
-      <c r="T2" s="12" t="b">
+      <c r="T2" s="13" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2296,176 +2248,176 @@
       <c r="V2" s="9"/>
       <c r="W2" s="9"/>
       <c r="X2" s="9"/>
-      <c r="XEE2" s="14"/>
-      <c r="XEF2" s="14"/>
-      <c r="XEG2" s="14"/>
-      <c r="XEH2" s="14"/>
-      <c r="XEI2" s="14"/>
-      <c r="XEJ2" s="14"/>
-      <c r="XEK2" s="14"/>
-      <c r="XEL2" s="14"/>
-      <c r="XEM2" s="14"/>
-      <c r="XEN2" s="14"/>
-      <c r="XEO2" s="14"/>
-      <c r="XEP2" s="14"/>
-      <c r="XEQ2" s="14"/>
-      <c r="XER2" s="14"/>
-      <c r="XES2" s="14"/>
-      <c r="XET2" s="14"/>
-      <c r="XEU2" s="14"/>
-      <c r="XEV2" s="14"/>
-      <c r="XEW2" s="14"/>
-      <c r="XEX2" s="14"/>
-      <c r="XEY2" s="14"/>
-      <c r="XEZ2" s="14"/>
-      <c r="XFA2" s="14"/>
-      <c r="XFB2" s="14"/>
-      <c r="XFC2" s="14"/>
-      <c r="XFD2" s="14"/>
-    </row>
-    <row r="3" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
+      <c r="XEE2" s="15"/>
+      <c r="XEF2" s="15"/>
+      <c r="XEG2" s="15"/>
+      <c r="XEH2" s="15"/>
+      <c r="XEI2" s="15"/>
+      <c r="XEJ2" s="15"/>
+      <c r="XEK2" s="15"/>
+      <c r="XEL2" s="15"/>
+      <c r="XEM2" s="15"/>
+      <c r="XEN2" s="15"/>
+      <c r="XEO2" s="15"/>
+      <c r="XEP2" s="15"/>
+      <c r="XEQ2" s="15"/>
+      <c r="XER2" s="15"/>
+      <c r="XES2" s="15"/>
+      <c r="XET2" s="15"/>
+      <c r="XEU2" s="15"/>
+      <c r="XEV2" s="15"/>
+      <c r="XEW2" s="15"/>
+      <c r="XEX2" s="15"/>
+      <c r="XEY2" s="15"/>
+      <c r="XEZ2" s="15"/>
+      <c r="XFA2" s="15"/>
+      <c r="XFB2" s="15"/>
+      <c r="XFC2" s="15"/>
+      <c r="XFD2" s="15"/>
+    </row>
+    <row r="3" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="15" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D3" s="15" t="s">
+      <c r="C3" s="17" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15" t="str">
+      <c r="E3" s="16"/>
+      <c r="F3" s="16" t="str">
         <f aca="false">REPLACE(A3, FIND("_", A3), 1, ".")</f>
         <v>household.size</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15" t="s">
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15" t="s">
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15"/>
-      <c r="T3" s="15" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U3" s="15"/>
-      <c r="V3" s="15"/>
-      <c r="W3" s="15"/>
-      <c r="X3" s="15"/>
-      <c r="Y3" s="16"/>
-      <c r="XFD3" s="17"/>
-    </row>
-    <row r="4" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="17" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U3" s="16"/>
+      <c r="V3" s="16"/>
+      <c r="W3" s="16"/>
+      <c r="X3" s="16"/>
+      <c r="Y3" s="18"/>
+      <c r="XFD3" s="19"/>
+    </row>
+    <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="15" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D4" s="15" t="s">
+      <c r="C4" s="17" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D4" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15" t="s">
+      <c r="E4" s="16"/>
+      <c r="F4" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="18" t="s">
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="17" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="18"/>
       <c r="XFD4" s="1"/>
     </row>
-    <row r="5" s="22" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="19" t="s">
+    <row r="5" s="25" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="19" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D5" s="19" t="s">
+      <c r="C5" s="22" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D5" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="21" t="str">
+      <c r="E5" s="23"/>
+      <c r="F5" s="24" t="str">
         <f aca="false">REPLACE(A5, FIND("_", A5), 1, ".")</f>
         <v>home.save</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="20"/>
-      <c r="T5" s="19" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U5" s="20"/>
-      <c r="V5" s="20"/>
-      <c r="W5" s="20"/>
-      <c r="X5" s="20"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="22" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="23"/>
+      <c r="X5" s="23"/>
       <c r="XEE5" s="1"/>
       <c r="XEF5" s="1"/>
       <c r="XEG5" s="1"/>
@@ -2491,9 +2443,9 @@
       <c r="XFA5" s="1"/>
       <c r="XFB5" s="1"/>
       <c r="XFC5" s="1"/>
-      <c r="XFD5" s="14"/>
-    </row>
-    <row r="6" s="13" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="XFD5" s="15"/>
+    </row>
+    <row r="6" s="14" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
         <v>46</v>
       </c>
@@ -2528,7 +2480,7 @@
       <c r="Q6" s="9"/>
       <c r="R6" s="9"/>
       <c r="S6" s="9"/>
-      <c r="T6" s="12" t="b">
+      <c r="T6" s="13" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2536,70 +2488,70 @@
       <c r="V6" s="9"/>
       <c r="W6" s="9"/>
       <c r="X6" s="9"/>
-      <c r="XEE6" s="14"/>
-      <c r="XEF6" s="14"/>
-      <c r="XEG6" s="14"/>
-      <c r="XEH6" s="14"/>
-      <c r="XEI6" s="14"/>
-      <c r="XEJ6" s="14"/>
-      <c r="XEK6" s="14"/>
-      <c r="XEL6" s="14"/>
-      <c r="XEM6" s="14"/>
-      <c r="XEN6" s="14"/>
-      <c r="XEO6" s="14"/>
-      <c r="XEP6" s="14"/>
-      <c r="XEQ6" s="14"/>
-      <c r="XER6" s="14"/>
-      <c r="XES6" s="14"/>
-      <c r="XET6" s="14"/>
-      <c r="XEU6" s="14"/>
-      <c r="XEV6" s="14"/>
-      <c r="XEW6" s="14"/>
-      <c r="XEX6" s="14"/>
-      <c r="XEY6" s="14"/>
-      <c r="XEZ6" s="14"/>
-      <c r="XFA6" s="14"/>
-      <c r="XFB6" s="14"/>
-      <c r="XFC6" s="14"/>
-      <c r="XFD6" s="23"/>
-    </row>
-    <row r="7" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="24" t="s">
+      <c r="XEE6" s="15"/>
+      <c r="XEF6" s="15"/>
+      <c r="XEG6" s="15"/>
+      <c r="XEH6" s="15"/>
+      <c r="XEI6" s="15"/>
+      <c r="XEJ6" s="15"/>
+      <c r="XEK6" s="15"/>
+      <c r="XEL6" s="15"/>
+      <c r="XEM6" s="15"/>
+      <c r="XEN6" s="15"/>
+      <c r="XEO6" s="15"/>
+      <c r="XEP6" s="15"/>
+      <c r="XEQ6" s="15"/>
+      <c r="XER6" s="15"/>
+      <c r="XES6" s="15"/>
+      <c r="XET6" s="15"/>
+      <c r="XEU6" s="15"/>
+      <c r="XEV6" s="15"/>
+      <c r="XEW6" s="15"/>
+      <c r="XEX6" s="15"/>
+      <c r="XEY6" s="15"/>
+      <c r="XEZ6" s="15"/>
+      <c r="XFA6" s="15"/>
+      <c r="XFB6" s="15"/>
+      <c r="XFC6" s="15"/>
+      <c r="XFD6" s="26"/>
+    </row>
+    <row r="7" s="18" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="15" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D7" s="26" t="s">
+      <c r="C7" s="17" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="27"/>
-      <c r="R7" s="27"/>
-      <c r="S7" s="27"/>
-      <c r="T7" s="28" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U7" s="27"/>
-      <c r="V7" s="27"/>
-      <c r="W7" s="27"/>
-      <c r="X7" s="27"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="30"/>
+      <c r="R7" s="30"/>
+      <c r="S7" s="30"/>
+      <c r="T7" s="31" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U7" s="30"/>
+      <c r="V7" s="30"/>
+      <c r="W7" s="30"/>
+      <c r="X7" s="30"/>
       <c r="XEE7" s="1"/>
       <c r="XEF7" s="1"/>
       <c r="XEG7" s="1"/>
@@ -2627,57 +2579,57 @@
       <c r="XFC7" s="1"/>
       <c r="XFD7" s="1"/>
     </row>
-    <row r="8" s="16" customFormat="true" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="26" t="s">
+    <row r="8" s="18" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="15" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D8" s="26" t="s">
+      <c r="C8" s="17" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D8" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="26" t="s">
+      <c r="G8" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="26" t="s">
+      <c r="H8" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="I8" s="26" t="s">
+      <c r="I8" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="J8" s="26" t="s">
+      <c r="J8" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="K8" s="26"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29" t="s">
+      <c r="K8" s="29"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="29"/>
-      <c r="S8" s="29"/>
-      <c r="T8" s="28" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U8" s="29"/>
-      <c r="V8" s="29"/>
-      <c r="W8" s="29"/>
-      <c r="X8" s="29"/>
+      <c r="O8" s="32"/>
+      <c r="P8" s="32"/>
+      <c r="Q8" s="32"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="32"/>
+      <c r="T8" s="31" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U8" s="32"/>
+      <c r="V8" s="32"/>
+      <c r="W8" s="32"/>
+      <c r="X8" s="32"/>
       <c r="XEE8" s="1"/>
       <c r="XEF8" s="1"/>
       <c r="XEG8" s="1"/>
@@ -2705,55 +2657,55 @@
       <c r="XFC8" s="1"/>
       <c r="XFD8" s="1"/>
     </row>
-    <row r="9" s="16" customFormat="true" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="26" t="s">
+    <row r="9" s="18" customFormat="true" ht="128.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="15" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D9" s="26" t="s">
+      <c r="C9" s="17" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D9" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="29" t="s">
+      <c r="F9" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="26" t="s">
+      <c r="G9" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="H9" s="26" t="s">
+      <c r="H9" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29" t="s">
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29" t="s">
+      <c r="N9" s="32"/>
+      <c r="O9" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29"/>
-      <c r="S9" s="29"/>
-      <c r="T9" s="28" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U9" s="29"/>
-      <c r="V9" s="29"/>
-      <c r="W9" s="29"/>
-      <c r="X9" s="29"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="32"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="32"/>
+      <c r="T9" s="31" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U9" s="32"/>
+      <c r="V9" s="32"/>
+      <c r="W9" s="32"/>
+      <c r="X9" s="32"/>
       <c r="XEE9" s="1"/>
       <c r="XEF9" s="1"/>
       <c r="XEG9" s="1"/>
@@ -2781,50 +2733,50 @@
       <c r="XFC9" s="1"/>
       <c r="XFD9" s="1"/>
     </row>
-    <row r="10" s="22" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="19" t="s">
+    <row r="10" s="25" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="15" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D10" s="26" t="s">
+      <c r="C10" s="17" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="21" t="str">
+      <c r="E10" s="23"/>
+      <c r="F10" s="24" t="str">
         <f aca="false">REPLACE(A10, FIND("_", A10), 1, ".")</f>
         <v>household.save</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="H10" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20"/>
-      <c r="R10" s="20"/>
-      <c r="S10" s="20"/>
-      <c r="T10" s="19" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U10" s="20"/>
-      <c r="V10" s="20"/>
-      <c r="W10" s="20"/>
-      <c r="X10" s="20"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="23"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="21" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U10" s="23"/>
+      <c r="V10" s="23"/>
+      <c r="W10" s="23"/>
+      <c r="X10" s="23"/>
       <c r="XEE10" s="1"/>
       <c r="XEF10" s="1"/>
       <c r="XEG10" s="1"/>
@@ -2852,7 +2804,7 @@
       <c r="XFC10" s="1"/>
       <c r="XFD10" s="1"/>
     </row>
-    <row r="11" s="13" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" s="14" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
         <v>68</v>
       </c>
@@ -2887,7 +2839,7 @@
       <c r="Q11" s="9"/>
       <c r="R11" s="9"/>
       <c r="S11" s="9"/>
-      <c r="T11" s="12" t="b">
+      <c r="T11" s="13" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2895,70 +2847,70 @@
       <c r="V11" s="9"/>
       <c r="W11" s="9"/>
       <c r="X11" s="9"/>
-      <c r="XEE11" s="14"/>
-      <c r="XEF11" s="14"/>
-      <c r="XEG11" s="14"/>
-      <c r="XEH11" s="14"/>
-      <c r="XEI11" s="14"/>
-      <c r="XEJ11" s="14"/>
-      <c r="XEK11" s="14"/>
-      <c r="XEL11" s="14"/>
-      <c r="XEM11" s="14"/>
-      <c r="XEN11" s="14"/>
-      <c r="XEO11" s="14"/>
-      <c r="XEP11" s="14"/>
-      <c r="XEQ11" s="14"/>
-      <c r="XER11" s="14"/>
-      <c r="XES11" s="14"/>
-      <c r="XET11" s="14"/>
-      <c r="XEU11" s="14"/>
-      <c r="XEV11" s="14"/>
-      <c r="XEW11" s="14"/>
-      <c r="XEX11" s="14"/>
-      <c r="XEY11" s="14"/>
-      <c r="XEZ11" s="14"/>
-      <c r="XFA11" s="14"/>
-      <c r="XFB11" s="14"/>
-      <c r="XFC11" s="14"/>
+      <c r="XEE11" s="15"/>
+      <c r="XEF11" s="15"/>
+      <c r="XEG11" s="15"/>
+      <c r="XEH11" s="15"/>
+      <c r="XEI11" s="15"/>
+      <c r="XEJ11" s="15"/>
+      <c r="XEK11" s="15"/>
+      <c r="XEL11" s="15"/>
+      <c r="XEM11" s="15"/>
+      <c r="XEN11" s="15"/>
+      <c r="XEO11" s="15"/>
+      <c r="XEP11" s="15"/>
+      <c r="XEQ11" s="15"/>
+      <c r="XER11" s="15"/>
+      <c r="XES11" s="15"/>
+      <c r="XET11" s="15"/>
+      <c r="XEU11" s="15"/>
+      <c r="XEV11" s="15"/>
+      <c r="XEW11" s="15"/>
+      <c r="XEX11" s="15"/>
+      <c r="XEY11" s="15"/>
+      <c r="XEZ11" s="15"/>
+      <c r="XFA11" s="15"/>
+      <c r="XFB11" s="15"/>
+      <c r="XFC11" s="15"/>
       <c r="XFD11" s="1"/>
     </row>
-    <row r="12" s="16" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="24" t="s">
+    <row r="12" s="18" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="26" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D12" s="24" t="s">
+      <c r="C12" s="33" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D12" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="27"/>
-      <c r="P12" s="27"/>
-      <c r="Q12" s="27"/>
-      <c r="R12" s="27"/>
-      <c r="S12" s="27"/>
-      <c r="T12" s="28" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U12" s="27"/>
-      <c r="V12" s="27"/>
-      <c r="W12" s="27"/>
-      <c r="X12" s="27"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="30"/>
+      <c r="T12" s="31" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U12" s="30"/>
+      <c r="V12" s="30"/>
+      <c r="W12" s="30"/>
+      <c r="X12" s="30"/>
       <c r="XEE12" s="1"/>
       <c r="XEF12" s="1"/>
       <c r="XEG12" s="1"/>
@@ -2986,51 +2938,53 @@
       <c r="XFC12" s="1"/>
       <c r="XFD12" s="1"/>
     </row>
-    <row r="13" s="16" customFormat="true" ht="137.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="24" t="s">
+    <row r="13" s="18" customFormat="true" ht="204.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="26" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D13" s="24" t="s">
+      <c r="C13" s="33" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D13" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="E13" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="F13" s="27" t="s">
+      <c r="F13" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="G13" s="26" t="s">
+      <c r="G13" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="H13" s="26" t="s">
+      <c r="H13" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="27"/>
-      <c r="R13" s="27"/>
-      <c r="S13" s="27"/>
-      <c r="T13" s="28" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U13" s="27"/>
-      <c r="V13" s="27"/>
-      <c r="W13" s="27"/>
-      <c r="X13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="O13" s="30"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="30"/>
+      <c r="S13" s="30"/>
+      <c r="T13" s="31" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U13" s="30"/>
+      <c r="V13" s="30"/>
+      <c r="W13" s="30"/>
+      <c r="X13" s="30"/>
       <c r="XEE13" s="1"/>
       <c r="XEF13" s="1"/>
       <c r="XEG13" s="1"/>
@@ -3058,53 +3012,53 @@
       <c r="XFC13" s="1"/>
       <c r="XFD13" s="1"/>
     </row>
-    <row r="14" s="16" customFormat="true" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="B14" s="26" t="s">
+    <row r="14" s="18" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="26" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D14" s="26" t="s">
+      <c r="C14" s="33" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D14" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="26" t="s">
+      <c r="E14" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="F14" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="G14" s="26" t="s">
+      <c r="F14" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="H14" s="26" t="s">
+      <c r="G14" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="18" t="s">
+      <c r="H14" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="29"/>
-      <c r="R14" s="29"/>
-      <c r="S14" s="29"/>
-      <c r="T14" s="28" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U14" s="29"/>
-      <c r="V14" s="29"/>
-      <c r="W14" s="29"/>
-      <c r="X14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="32"/>
+      <c r="O14" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="32"/>
+      <c r="R14" s="32"/>
+      <c r="S14" s="32"/>
+      <c r="T14" s="31" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U14" s="32"/>
+      <c r="V14" s="32"/>
+      <c r="W14" s="32"/>
+      <c r="X14" s="32"/>
       <c r="XEE14" s="1"/>
       <c r="XEF14" s="1"/>
       <c r="XEG14" s="1"/>
@@ -3132,76 +3086,76 @@
       <c r="XFC14" s="1"/>
       <c r="XFD14" s="1"/>
     </row>
-    <row r="15" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B15" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="26" t="b">
+      <c r="C15" s="33" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="E15" s="29" t="s">
         <v>72</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G15" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="H15" s="26" t="s">
+      <c r="G15" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="M15" s="30"/>
-      <c r="O15" s="31" t="s">
+      <c r="H15" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="T15" s="28" t="n">
+      <c r="M15" s="34"/>
+      <c r="O15" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="T15" s="31" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="XFD15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B16" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="26" t="b">
+      <c r="C16" s="33" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E16" s="26"/>
+      <c r="E16" s="29"/>
       <c r="F16" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G16" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="H16" s="19" t="s">
+      <c r="H16" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="M16" s="30"/>
-      <c r="O16" s="31"/>
-      <c r="T16" s="28" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" s="13" customFormat="true" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M16" s="34"/>
+      <c r="O16" s="36"/>
+      <c r="T16" s="31" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" s="14" customFormat="true" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>26</v>
@@ -3211,17 +3165,17 @@
         <v>1</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
@@ -3234,7 +3188,7 @@
       <c r="Q17" s="9"/>
       <c r="R17" s="9"/>
       <c r="S17" s="9"/>
-      <c r="T17" s="12" t="b">
+      <c r="T17" s="13" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3242,105 +3196,105 @@
       <c r="V17" s="9"/>
       <c r="W17" s="9"/>
       <c r="X17" s="9"/>
-      <c r="XEE17" s="14"/>
-      <c r="XEF17" s="14"/>
-      <c r="XEG17" s="14"/>
-      <c r="XEH17" s="14"/>
-      <c r="XEI17" s="14"/>
-      <c r="XEJ17" s="14"/>
-      <c r="XEK17" s="14"/>
-      <c r="XEL17" s="14"/>
-      <c r="XEM17" s="14"/>
-      <c r="XEN17" s="14"/>
-      <c r="XEO17" s="14"/>
-      <c r="XEP17" s="14"/>
-      <c r="XEQ17" s="14"/>
-      <c r="XER17" s="14"/>
-      <c r="XES17" s="14"/>
-      <c r="XET17" s="14"/>
-      <c r="XEU17" s="14"/>
-      <c r="XEV17" s="14"/>
-      <c r="XEW17" s="14"/>
-      <c r="XEX17" s="14"/>
-      <c r="XEY17" s="14"/>
-      <c r="XEZ17" s="14"/>
-      <c r="XFA17" s="14"/>
-      <c r="XFB17" s="14"/>
-      <c r="XFC17" s="14"/>
+      <c r="XEE17" s="15"/>
+      <c r="XEF17" s="15"/>
+      <c r="XEG17" s="15"/>
+      <c r="XEH17" s="15"/>
+      <c r="XEI17" s="15"/>
+      <c r="XEJ17" s="15"/>
+      <c r="XEK17" s="15"/>
+      <c r="XEL17" s="15"/>
+      <c r="XEM17" s="15"/>
+      <c r="XEN17" s="15"/>
+      <c r="XEO17" s="15"/>
+      <c r="XEP17" s="15"/>
+      <c r="XEQ17" s="15"/>
+      <c r="XER17" s="15"/>
+      <c r="XES17" s="15"/>
+      <c r="XET17" s="15"/>
+      <c r="XEU17" s="15"/>
+      <c r="XEV17" s="15"/>
+      <c r="XEW17" s="15"/>
+      <c r="XEX17" s="15"/>
+      <c r="XEY17" s="15"/>
+      <c r="XEZ17" s="15"/>
+      <c r="XFA17" s="15"/>
+      <c r="XFB17" s="15"/>
+      <c r="XFC17" s="15"/>
       <c r="XFD17" s="1"/>
     </row>
-    <row r="18" s="23" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="B18" s="25" t="s">
+    <row r="18" s="26" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="33" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D18" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="M18" s="32"/>
-      <c r="O18" s="32"/>
-      <c r="T18" s="33" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="XFD18" s="14"/>
-    </row>
-    <row r="19" s="16" customFormat="true" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="30" t="s">
+      <c r="C18" s="38" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D18" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="M18" s="37"/>
+      <c r="O18" s="37"/>
+      <c r="T18" s="38" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="XFD18" s="15"/>
+    </row>
+    <row r="19" s="18" customFormat="true" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="40" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B19" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" s="35" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="G19" s="15" t="s">
+      <c r="F19" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="H19" s="15" t="s">
+      <c r="G19" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="36"/>
-      <c r="N19" s="36" t="s">
+      <c r="H19" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="O19" s="36"/>
-      <c r="P19" s="36"/>
-      <c r="Q19" s="36"/>
-      <c r="R19" s="36"/>
-      <c r="S19" s="36"/>
-      <c r="T19" s="15" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U19" s="36"/>
-      <c r="V19" s="36"/>
-      <c r="W19" s="36"/>
-      <c r="X19" s="36"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="35"/>
+      <c r="N19" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="O19" s="35"/>
+      <c r="P19" s="35"/>
+      <c r="Q19" s="35"/>
+      <c r="R19" s="35"/>
+      <c r="S19" s="35"/>
+      <c r="T19" s="16" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U19" s="35"/>
+      <c r="V19" s="35"/>
+      <c r="W19" s="35"/>
+      <c r="X19" s="35"/>
       <c r="XEE19" s="1"/>
       <c r="XEF19" s="1"/>
       <c r="XEG19" s="1"/>
@@ -3368,52 +3322,52 @@
       <c r="XFC19" s="1"/>
       <c r="XFD19" s="1"/>
     </row>
-    <row r="20" s="16" customFormat="true" ht="96.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="30" t="s">
+    <row r="20" s="18" customFormat="true" ht="96.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="35" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="F20" s="30" t="s">
+      <c r="C20" s="40" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="F20" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="G20" s="30" t="s">
+      <c r="G20" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="36"/>
-      <c r="N20" s="36"/>
-      <c r="O20" s="36"/>
-      <c r="P20" s="36"/>
-      <c r="Q20" s="36"/>
-      <c r="R20" s="36"/>
-      <c r="S20" s="36"/>
-      <c r="T20" s="15" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U20" s="36"/>
-      <c r="V20" s="36"/>
-      <c r="W20" s="36"/>
-      <c r="X20" s="36"/>
-      <c r="Y20" s="16" t="s">
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="35"/>
+      <c r="N20" s="35"/>
+      <c r="O20" s="35"/>
+      <c r="P20" s="35"/>
+      <c r="Q20" s="35"/>
+      <c r="R20" s="35"/>
+      <c r="S20" s="35"/>
+      <c r="T20" s="16" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U20" s="35"/>
+      <c r="V20" s="35"/>
+      <c r="W20" s="35"/>
+      <c r="X20" s="35"/>
+      <c r="Y20" s="18" t="s">
         <v>104</v>
       </c>
       <c r="XEE20" s="1"/>
@@ -3443,198 +3397,198 @@
       <c r="XFC20" s="1"/>
       <c r="XFD20" s="1"/>
     </row>
-    <row r="21" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="15" t="s">
+    <row r="21" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="15" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="F21" s="15" t="s">
+      <c r="C21" s="17" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="F21" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="G21" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="H21" s="15" t="s">
+      <c r="H21" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="18" t="s">
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
-      <c r="S21" s="15"/>
-      <c r="T21" s="15" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U21" s="15"/>
-      <c r="V21" s="15"/>
-      <c r="W21" s="15"/>
-      <c r="X21" s="15"/>
-      <c r="Y21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="16"/>
+      <c r="S21" s="16"/>
+      <c r="T21" s="16" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U21" s="16"/>
+      <c r="V21" s="16"/>
+      <c r="W21" s="16"/>
+      <c r="X21" s="16"/>
+      <c r="Y21" s="18"/>
       <c r="XFD21" s="1"/>
     </row>
-    <row r="22" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="37" t="s">
+    <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="15" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="F22" s="15" t="s">
+      <c r="C22" s="17" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="F22" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="G22" s="26" t="s">
+      <c r="G22" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="H22" s="26" t="s">
+      <c r="H22" s="29" t="s">
         <v>113</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="O22" s="37"/>
-      <c r="T22" s="28" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="37" t="s">
+      <c r="O22" s="41"/>
+      <c r="T22" s="31" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="15" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="F23" s="15" t="s">
+      <c r="C23" s="17" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="F23" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="G23" s="26" t="s">
+      <c r="G23" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="H23" s="26" t="s">
+      <c r="H23" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="M23" s="30" t="s">
+      <c r="M23" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="O23" s="38" t="s">
+      <c r="O23" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="T23" s="28" t="n">
+      <c r="T23" s="31" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="XFD23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="37" t="s">
+      <c r="A24" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="15" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="F24" s="15" t="s">
+      <c r="C24" s="17" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="F24" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="G24" s="26" t="s">
+      <c r="G24" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="H24" s="26" t="s">
+      <c r="H24" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="M24" s="30" t="s">
+      <c r="M24" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="O24" s="38"/>
-      <c r="T24" s="28" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="37" t="s">
+      <c r="O24" s="42"/>
+      <c r="T24" s="31" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="15" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="F25" s="15" t="s">
+      <c r="C25" s="17" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="F25" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="G25" s="26" t="s">
+      <c r="G25" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="H25" s="26" t="s">
+      <c r="H25" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="M25" s="30" t="s">
+      <c r="M25" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="N25" s="15" t="s">
+      <c r="N25" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="O25" s="38"/>
-      <c r="T25" s="28" t="n">
+      <c r="O25" s="42"/>
+      <c r="T25" s="31" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3642,40 +3596,40 @@
         <v>130</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="37" t="s">
+    <row r="26" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="41" t="s">
         <v>131</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="15" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="F26" s="15" t="s">
+      <c r="C26" s="17" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="F26" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="G26" s="26" t="s">
+      <c r="G26" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="H26" s="26" t="s">
+      <c r="H26" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="K26" s="15"/>
-      <c r="M26" s="30" t="s">
+      <c r="K26" s="16"/>
+      <c r="M26" s="34" t="s">
         <v>124</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="T26" s="28" t="n">
+      <c r="T26" s="31" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3686,119 +3640,119 @@
         <v>136</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="37" t="s">
+    <row r="27" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="15" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="F27" s="15" t="s">
+      <c r="C27" s="17" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="G27" s="26" t="s">
+      <c r="G27" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="H27" s="26" t="s">
+      <c r="H27" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="K27" s="15"/>
-      <c r="M27" s="30" t="s">
+      <c r="K27" s="16"/>
+      <c r="M27" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="T27" s="28" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T27" s="31" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="15" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="F28" s="15" t="s">
+      <c r="C28" s="17" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="F28" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="G28" s="26" t="s">
+      <c r="G28" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="H28" s="26" t="s">
+      <c r="H28" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="M28" s="30" t="s">
+      <c r="M28" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="T28" s="28" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" s="22" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="19" t="s">
+      <c r="T28" s="31" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" s="25" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="19" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E29" s="20"/>
-      <c r="F29" s="21" t="str">
+      <c r="C29" s="22" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E29" s="23"/>
+      <c r="F29" s="24" t="str">
         <f aca="false">REPLACE(A29, FIND("_", A29), 1, ".")</f>
         <v>addresses.save</v>
       </c>
-      <c r="G29" s="19" t="s">
+      <c r="G29" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="H29" s="19" t="s">
+      <c r="H29" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
-      <c r="L29" s="20"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="20"/>
-      <c r="O29" s="20"/>
-      <c r="P29" s="20"/>
-      <c r="Q29" s="20"/>
-      <c r="R29" s="20"/>
-      <c r="S29" s="20"/>
-      <c r="T29" s="19" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U29" s="20"/>
-      <c r="V29" s="20"/>
-      <c r="W29" s="20"/>
-      <c r="X29" s="20"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="23"/>
+      <c r="R29" s="23"/>
+      <c r="S29" s="23"/>
+      <c r="T29" s="21" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U29" s="23"/>
+      <c r="V29" s="23"/>
+      <c r="W29" s="23"/>
+      <c r="X29" s="23"/>
       <c r="XEE29" s="1"/>
       <c r="XEF29" s="1"/>
       <c r="XEG29" s="1"/>
@@ -3826,14 +3780,14 @@
       <c r="XFC29" s="1"/>
       <c r="XFD29" s="1"/>
     </row>
-    <row r="30" s="13" customFormat="true" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" s="14" customFormat="true" ht="229.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="35" t="n">
+      <c r="C30" s="40" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3861,7 +3815,7 @@
       <c r="Q30" s="9"/>
       <c r="R30" s="9"/>
       <c r="S30" s="9"/>
-      <c r="T30" s="12" t="b">
+      <c r="T30" s="13" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3869,99 +3823,99 @@
       <c r="V30" s="9"/>
       <c r="W30" s="9"/>
       <c r="X30" s="9"/>
-      <c r="XEE30" s="14"/>
-      <c r="XEF30" s="14"/>
-      <c r="XEG30" s="14"/>
-      <c r="XEH30" s="14"/>
-      <c r="XEI30" s="14"/>
-      <c r="XEJ30" s="14"/>
-      <c r="XEK30" s="14"/>
-      <c r="XEL30" s="14"/>
-      <c r="XEM30" s="14"/>
-      <c r="XEN30" s="14"/>
-      <c r="XEO30" s="14"/>
-      <c r="XEP30" s="14"/>
-      <c r="XEQ30" s="14"/>
-      <c r="XER30" s="14"/>
-      <c r="XES30" s="14"/>
-      <c r="XET30" s="14"/>
-      <c r="XEU30" s="14"/>
-      <c r="XEV30" s="14"/>
-      <c r="XEW30" s="14"/>
-      <c r="XEX30" s="14"/>
-      <c r="XEY30" s="14"/>
-      <c r="XEZ30" s="14"/>
-      <c r="XFA30" s="14"/>
-      <c r="XFB30" s="14"/>
-      <c r="XFC30" s="14"/>
+      <c r="XEE30" s="15"/>
+      <c r="XEF30" s="15"/>
+      <c r="XEG30" s="15"/>
+      <c r="XEH30" s="15"/>
+      <c r="XEI30" s="15"/>
+      <c r="XEJ30" s="15"/>
+      <c r="XEK30" s="15"/>
+      <c r="XEL30" s="15"/>
+      <c r="XEM30" s="15"/>
+      <c r="XEN30" s="15"/>
+      <c r="XEO30" s="15"/>
+      <c r="XEP30" s="15"/>
+      <c r="XEQ30" s="15"/>
+      <c r="XER30" s="15"/>
+      <c r="XES30" s="15"/>
+      <c r="XET30" s="15"/>
+      <c r="XEU30" s="15"/>
+      <c r="XEV30" s="15"/>
+      <c r="XEW30" s="15"/>
+      <c r="XEX30" s="15"/>
+      <c r="XEY30" s="15"/>
+      <c r="XEZ30" s="15"/>
+      <c r="XFA30" s="15"/>
+      <c r="XFB30" s="15"/>
+      <c r="XFC30" s="15"/>
       <c r="XFD30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="15" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D31" s="30" t="s">
+      <c r="C31" s="17" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D31" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="T31" s="15" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" s="16" customFormat="true" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="30" t="s">
+      <c r="T31" s="16" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" s="18" customFormat="true" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="B32" s="34" t="s">
+      <c r="B32" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="C32" s="35" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D32" s="15" t="s">
+      <c r="C32" s="40" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D32" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="E32" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="F32" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="G32" s="15" t="s">
+      <c r="F32" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="G32" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="H32" s="15" t="s">
+      <c r="H32" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="I32" s="34"/>
-      <c r="J32" s="34"/>
-      <c r="K32" s="34"/>
-      <c r="L32" s="36"/>
-      <c r="M32" s="36"/>
-      <c r="N32" s="36" t="s">
-        <v>99</v>
-      </c>
-      <c r="O32" s="36"/>
-      <c r="P32" s="36"/>
-      <c r="Q32" s="36"/>
-      <c r="R32" s="36"/>
-      <c r="S32" s="36"/>
-      <c r="T32" s="15" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U32" s="36"/>
-      <c r="V32" s="36"/>
-      <c r="W32" s="36"/>
-      <c r="X32" s="36"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="39"/>
+      <c r="L32" s="35"/>
+      <c r="M32" s="35"/>
+      <c r="N32" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="O32" s="35"/>
+      <c r="P32" s="35"/>
+      <c r="Q32" s="35"/>
+      <c r="R32" s="35"/>
+      <c r="S32" s="35"/>
+      <c r="T32" s="16" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U32" s="35"/>
+      <c r="V32" s="35"/>
+      <c r="W32" s="35"/>
+      <c r="X32" s="35"/>
       <c r="XEE32" s="1"/>
       <c r="XEF32" s="1"/>
       <c r="XEG32" s="1"/>
@@ -3989,52 +3943,52 @@
       <c r="XFC32" s="1"/>
       <c r="XFD32" s="1"/>
     </row>
-    <row r="33" s="16" customFormat="true" ht="96.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="30" t="s">
+    <row r="33" s="18" customFormat="true" ht="96.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="B33" s="34" t="s">
+      <c r="B33" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="35" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D33" s="15" t="s">
+      <c r="C33" s="40" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D33" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E33" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="F33" s="30" t="s">
+      <c r="F33" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="G33" s="30" t="s">
+      <c r="G33" s="34" t="s">
         <v>156</v>
       </c>
-      <c r="H33" s="30" t="s">
+      <c r="H33" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="I33" s="34"/>
-      <c r="J33" s="34"/>
-      <c r="K33" s="34"/>
-      <c r="L33" s="36"/>
-      <c r="M33" s="36"/>
-      <c r="N33" s="36"/>
-      <c r="O33" s="36"/>
-      <c r="P33" s="29"/>
-      <c r="Q33" s="29"/>
-      <c r="R33" s="29"/>
-      <c r="S33" s="29"/>
-      <c r="T33" s="15" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U33" s="29"/>
-      <c r="V33" s="29"/>
-      <c r="W33" s="29"/>
-      <c r="X33" s="29"/>
-      <c r="Y33" s="16" t="s">
+      <c r="I33" s="39"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="39"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="35"/>
+      <c r="N33" s="35"/>
+      <c r="O33" s="35"/>
+      <c r="P33" s="32"/>
+      <c r="Q33" s="32"/>
+      <c r="R33" s="32"/>
+      <c r="S33" s="32"/>
+      <c r="T33" s="16" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U33" s="32"/>
+      <c r="V33" s="32"/>
+      <c r="W33" s="32"/>
+      <c r="X33" s="32"/>
+      <c r="Y33" s="18" t="s">
         <v>104</v>
       </c>
       <c r="XEE33" s="1"/>
@@ -4064,85 +4018,85 @@
       <c r="XFC33" s="1"/>
       <c r="XFD33" s="1"/>
     </row>
-    <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="39" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D34" s="15" t="s">
+      <c r="C34" s="43" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D34" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="F34" s="15" t="s">
+      <c r="F34" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="G34" s="26" t="s">
+      <c r="G34" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="H34" s="26" t="s">
+      <c r="H34" s="29" t="s">
         <v>161</v>
       </c>
-      <c r="K34" s="15" t="s">
+      <c r="K34" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="M34" s="30"/>
-      <c r="T34" s="15" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" s="22" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="19" t="s">
+      <c r="M34" s="34"/>
+      <c r="T34" s="16" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" s="25" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="19" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D35" s="15" t="s">
+      <c r="C35" s="22" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D35" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="E35" s="20"/>
-      <c r="F35" s="21" t="str">
+      <c r="E35" s="23"/>
+      <c r="F35" s="24" t="str">
         <f aca="false">REPLACE(A35, FIND("_", A35), 1, ".")</f>
         <v>destinations.save</v>
       </c>
-      <c r="G35" s="19" t="s">
+      <c r="G35" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="H35" s="19" t="s">
+      <c r="H35" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
-      <c r="L35" s="20"/>
-      <c r="M35" s="20"/>
-      <c r="N35" s="20"/>
-      <c r="O35" s="20"/>
-      <c r="P35" s="20"/>
-      <c r="Q35" s="20"/>
-      <c r="R35" s="20"/>
-      <c r="S35" s="20"/>
-      <c r="T35" s="19" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U35" s="20"/>
-      <c r="V35" s="20"/>
-      <c r="W35" s="20"/>
-      <c r="X35" s="20"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="21"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="23"/>
+      <c r="M35" s="23"/>
+      <c r="N35" s="23"/>
+      <c r="O35" s="23"/>
+      <c r="P35" s="23"/>
+      <c r="Q35" s="23"/>
+      <c r="R35" s="23"/>
+      <c r="S35" s="23"/>
+      <c r="T35" s="21" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U35" s="23"/>
+      <c r="V35" s="23"/>
+      <c r="W35" s="23"/>
+      <c r="X35" s="23"/>
       <c r="XEE35" s="1"/>
       <c r="XEF35" s="1"/>
       <c r="XEG35" s="1"/>
@@ -4174,17 +4128,17 @@
       <c r="A36" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="35" t="n">
+      <c r="C36" s="40" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="F36" s="15" t="s">
+      <c r="F36" s="16" t="s">
         <v>164</v>
       </c>
       <c r="G36" s="2" t="s">
@@ -4193,7 +4147,7 @@
       <c r="H36" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="T36" s="15" t="n">
+      <c r="T36" s="16" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4205,7 +4159,7 @@
       <c r="B37" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="35" t="n">
+      <c r="C37" s="40" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4229,7 +4183,7 @@
       <c r="B38" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="35" t="n">
+      <c r="C38" s="40" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4237,7 +4191,7 @@
         <v>165</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4247,7 +4201,7 @@
       <c r="B39" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="35" t="n">
+      <c r="C39" s="40" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4257,16 +4211,16 @@
       <c r="E39" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F39" s="40" t="s">
+      <c r="F39" s="44" t="s">
         <v>173</v>
       </c>
-      <c r="G39" s="30" t="s">
+      <c r="G39" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="H39" s="30" t="s">
+      <c r="H39" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="T39" s="28" t="n">
+      <c r="T39" s="31" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4281,7 +4235,7 @@
       <c r="B40" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C40" s="35" t="n">
+      <c r="C40" s="40" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4291,16 +4245,16 @@
       <c r="E40" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F40" s="40" t="s">
+      <c r="F40" s="44" t="s">
         <v>178</v>
       </c>
-      <c r="G40" s="30" t="s">
+      <c r="G40" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="H40" s="30" t="s">
+      <c r="H40" s="34" t="s">
         <v>180</v>
       </c>
-      <c r="T40" s="28"/>
+      <c r="T40" s="31"/>
       <c r="Y40" s="1"/>
     </row>
     <row r="41" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4310,7 +4264,7 @@
       <c r="B41" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C41" s="35" t="n">
+      <c r="C41" s="40" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4320,16 +4274,16 @@
       <c r="E41" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F41" s="40" t="s">
+      <c r="F41" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="G41" s="30" t="s">
+      <c r="G41" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="H41" s="30" t="s">
+      <c r="H41" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="T41" s="28"/>
+      <c r="T41" s="31"/>
       <c r="Y41" s="1"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4339,7 +4293,7 @@
       <c r="B42" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C42" s="35" t="n">
+      <c r="C42" s="40" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4349,7 +4303,7 @@
       <c r="E42" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F42" s="30" t="s">
+      <c r="F42" s="34" t="s">
         <v>186</v>
       </c>
       <c r="G42" s="2" t="s">
@@ -4366,7 +4320,7 @@
       <c r="B43" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C43" s="35" t="n">
+      <c r="C43" s="40" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4390,10 +4344,10 @@
       <c r="A44" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="C44" s="35" t="n">
+      <c r="C44" s="40" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4417,10 +4371,10 @@
       <c r="A45" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="C45" s="35" t="n">
+      <c r="C45" s="40" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4479,48 +4433,48 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="38.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="15.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="30" width="31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="41" width="20.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="30" width="19.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="30" width="12.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="30" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="34" width="38.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="34" width="15.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="34" width="31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="45" width="20.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="34" width="19.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="34" width="12.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="34" width="8.59"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="42" t="s">
+    <row r="1" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="46" t="s">
         <v>200</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="47" t="s">
         <v>202</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="46" t="s">
         <v>203</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="46" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="34" t="s">
         <v>205</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="48" t="s">
         <v>206</v>
       </c>
-      <c r="E2" s="30" t="n">
+      <c r="E2" s="34" t="n">
         <v>16</v>
       </c>
     </row>
@@ -4761,196 +4715,196 @@
       <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="10.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="30" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="30" width="12.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="30" width="10.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="30" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="30" width="15.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="30" width="10.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="34" width="10.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="34" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="34" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="34" width="12.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="34" width="10.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="34" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="34" width="15.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="34" width="10.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="50" t="s">
         <v>207</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="49" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="49" t="s">
         <v>209</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="49" t="s">
         <v>210</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="49" t="s">
         <v>211</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="49" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="34" t="s">
         <v>215</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="34" t="s">
         <v>216</v>
       </c>
-      <c r="E2" s="47" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F2" s="47" t="b">
+      <c r="E2" s="51" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="51" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G2" s="47" t="b">
+      <c r="G2" s="51" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="34" t="s">
         <v>217</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="34" t="s">
         <v>218</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="34" t="s">
         <v>219</v>
       </c>
-      <c r="E3" s="47" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F3" s="47" t="b">
+      <c r="E3" s="51" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="51" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G3" s="47" t="b">
+      <c r="G3" s="51" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="34" t="s">
         <v>220</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="34" t="s">
         <v>221</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="E4" s="47" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F4" s="47" t="b">
+      <c r="E4" s="51" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="51" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G4" s="47" t="b">
+      <c r="G4" s="51" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" s="30" t="s">
+      <c r="A5" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="34" t="s">
         <v>223</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="34" t="s">
         <v>224</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="E5" s="47" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F5" s="47" t="b">
+      <c r="E5" s="51" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="51" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G5" s="47" t="b">
+      <c r="G5" s="51" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="34" t="s">
         <v>226</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="34" t="s">
         <v>228</v>
       </c>
-      <c r="E6" s="47" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F6" s="47" t="b">
+      <c r="E6" s="51" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="51" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G6" s="47" t="b">
+      <c r="G6" s="51" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="34" t="s">
         <v>229</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="34" t="s">
         <v>230</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="34" t="s">
         <v>231</v>
       </c>
-      <c r="E7" s="47" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F7" s="47" t="b">
+      <c r="E7" s="51" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="51" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G7" s="47" t="b">
+      <c r="G7" s="51" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5146,385 +5100,385 @@
       <selection pane="topLeft" activeCell="G42" activeCellId="0" sqref="G42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="29.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="19.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="31" width="30.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="31" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="31" width="24.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="31" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="36" width="29.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="36" width="19.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="36" width="30.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="36" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="36" width="24.29"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="36" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="52" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="52" t="s">
         <v>203</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="52" t="s">
         <v>233</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="36" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="42" t="s">
         <v>235</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="42" t="s">
         <v>235</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="42" t="s">
         <v>236</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="42" t="s">
         <v>237</v>
       </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="42" t="s">
         <v>238</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="42" t="s">
         <v>238</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="42" t="s">
         <v>239</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="42" t="s">
         <v>240</v>
       </c>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="42" t="s">
         <v>241</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="42" t="s">
         <v>241</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="42" t="s">
         <v>242</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="42" t="s">
         <v>243</v>
       </c>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="42" t="s">
         <v>244</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="42" t="s">
         <v>241</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="42" t="s">
         <v>245</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="D5" s="42" t="s">
         <v>246</v>
       </c>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="42" t="s">
         <v>247</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="42" t="s">
         <v>247</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="42" t="s">
         <v>248</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="42" t="s">
         <v>249</v>
       </c>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="42" t="s">
         <v>250</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="42" t="s">
         <v>250</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="42" t="s">
         <v>251</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="D7" s="42" t="s">
         <v>252</v>
       </c>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38" t="s">
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42" t="s">
         <v>235</v>
       </c>
-      <c r="H8" s="38"/>
+      <c r="H8" s="42"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38" t="s">
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42" t="s">
         <v>238</v>
       </c>
-      <c r="H9" s="38"/>
+      <c r="H9" s="42"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38" t="s">
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="H10" s="38"/>
+      <c r="H10" s="42"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38" t="s">
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42" t="s">
         <v>247</v>
       </c>
-      <c r="H11" s="38"/>
+      <c r="H11" s="42"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="42" t="s">
         <v>253</v>
       </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38" t="s">
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42" t="s">
         <v>235</v>
       </c>
-      <c r="H12" s="38"/>
+      <c r="H12" s="42"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="42" t="s">
         <v>253</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38" t="s">
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42" t="s">
         <v>238</v>
       </c>
-      <c r="H13" s="38"/>
+      <c r="H13" s="42"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="42" t="s">
         <v>253</v>
       </c>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38" t="s">
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42" t="s">
         <v>250</v>
       </c>
-      <c r="H14" s="38"/>
+      <c r="H14" s="42"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="50" t="s">
+      <c r="A15" s="54" t="s">
         <v>254</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="42" t="s">
         <v>255</v>
       </c>
-      <c r="C15" s="38" t="s">
+      <c r="C15" s="42" t="s">
         <v>256</v>
       </c>
-      <c r="D15" s="38" t="s">
+      <c r="D15" s="42" t="s">
         <v>257</v>
       </c>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="50" t="s">
+      <c r="A16" s="54" t="s">
         <v>254</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="42" t="s">
         <v>258</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="D16" s="38" t="s">
+      <c r="D16" s="42" t="s">
         <v>260</v>
       </c>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="50" t="s">
+      <c r="A17" s="54" t="s">
         <v>254</v>
       </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38" t="s">
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42" t="s">
         <v>250</v>
       </c>
-      <c r="H17" s="38"/>
+      <c r="H17" s="42"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="50" t="s">
+      <c r="A18" s="54" t="s">
         <v>261</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="42" t="s">
         <v>255</v>
       </c>
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="42" t="s">
         <v>256</v>
       </c>
-      <c r="D18" s="38" t="s">
+      <c r="D18" s="42" t="s">
         <v>262</v>
       </c>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="54" t="s">
         <v>261</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="42" t="s">
         <v>258</v>
       </c>
-      <c r="C19" s="38" t="s">
+      <c r="C19" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="D19" s="38" t="s">
+      <c r="D19" s="42" t="s">
         <v>263</v>
       </c>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="54" t="s">
         <v>261</v>
       </c>
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="42" t="s">
         <v>264</v>
       </c>
-      <c r="C20" s="38" t="s">
+      <c r="C20" s="42" t="s">
         <v>265</v>
       </c>
-      <c r="D20" s="38" t="s">
+      <c r="D20" s="42" t="s">
         <v>266</v>
       </c>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="50" t="s">
+      <c r="A21" s="54" t="s">
         <v>261</v>
       </c>
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38" t="s">
+      <c r="B21" s="42"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42" t="s">
         <v>250</v>
       </c>
-      <c r="H21" s="38"/>
+      <c r="H21" s="42"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="36" t="s">
         <v>267</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="36" t="s">
         <v>268</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="36" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="36" t="s">
         <v>41</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -5540,7 +5494,7 @@
       <c r="F23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="36" t="s">
         <v>41</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -5556,7 +5510,7 @@
       <c r="F24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="36" t="s">
         <v>41</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -5572,7 +5526,7 @@
       <c r="F25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="36" t="s">
         <v>41</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -5588,7 +5542,7 @@
       <c r="F26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="36" t="s">
         <v>41</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -5604,7 +5558,7 @@
       <c r="F27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="36" t="s">
         <v>41</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -5620,7 +5574,7 @@
       <c r="F28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="36" t="s">
         <v>41</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -5636,7 +5590,7 @@
       <c r="F29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="36" t="s">
         <v>41</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -5652,7 +5606,7 @@
       <c r="F30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="36" t="s">
         <v>41</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -5668,7 +5622,7 @@
       <c r="F31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="36" t="s">
         <v>41</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -5684,7 +5638,7 @@
       <c r="F32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="36" t="s">
         <v>41</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -5700,184 +5654,184 @@
       <c r="F33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="36" t="s">
         <v>303</v>
       </c>
-      <c r="C34" s="31" t="s">
+      <c r="C34" s="36" t="s">
         <v>304</v>
       </c>
-      <c r="D34" s="31" t="s">
+      <c r="D34" s="36" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="36" t="s">
         <v>247</v>
       </c>
-      <c r="C35" s="31" t="s">
+      <c r="C35" s="36" t="s">
         <v>306</v>
       </c>
-      <c r="D35" s="31" t="s">
+      <c r="D35" s="36" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="31" t="s">
+      <c r="B36" s="36" t="s">
         <v>308</v>
       </c>
-      <c r="C36" s="31" t="s">
+      <c r="C36" s="36" t="s">
         <v>309</v>
       </c>
-      <c r="D36" s="31" t="s">
+      <c r="D36" s="36" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="B37" s="31" t="s">
+      <c r="B37" s="36" t="s">
         <v>311</v>
       </c>
-      <c r="C37" s="31" t="s">
+      <c r="C37" s="36" t="s">
         <v>312</v>
       </c>
-      <c r="D37" s="31" t="s">
+      <c r="D37" s="36" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="B38" s="31" t="s">
+      <c r="B38" s="36" t="s">
         <v>314</v>
       </c>
-      <c r="C38" s="31" t="s">
+      <c r="C38" s="36" t="s">
         <v>315</v>
       </c>
-      <c r="D38" s="31" t="s">
+      <c r="D38" s="36" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="B39" s="31" t="s">
+      <c r="A39" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" s="36" t="s">
         <v>317</v>
       </c>
-      <c r="C39" s="31" t="s">
+      <c r="C39" s="36" t="s">
         <v>318</v>
       </c>
-      <c r="D39" s="31" t="s">
+      <c r="D39" s="36" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="B40" s="31" t="s">
+      <c r="A40" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" s="36" t="s">
         <v>320</v>
       </c>
-      <c r="C40" s="31" t="s">
+      <c r="C40" s="36" t="s">
         <v>321</v>
       </c>
-      <c r="D40" s="31" t="s">
+      <c r="D40" s="36" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="B41" s="31" t="s">
+      <c r="A41" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="36" t="s">
         <v>323</v>
       </c>
-      <c r="C41" s="31" t="s">
+      <c r="C41" s="36" t="s">
         <v>324</v>
       </c>
-      <c r="D41" s="31" t="s">
+      <c r="D41" s="36" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="G42" s="38" t="s">
+      <c r="A42" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="G42" s="42" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="B43" s="31" t="s">
+      <c r="A43" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="B43" s="36" t="s">
         <v>326</v>
       </c>
-      <c r="C43" s="31" t="s">
+      <c r="C43" s="36" t="s">
         <v>327</v>
       </c>
-      <c r="D43" s="31" t="s">
+      <c r="D43" s="36" t="s">
         <v>328</v>
       </c>
-      <c r="H43" s="30"/>
+      <c r="H43" s="34"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="B44" s="31" t="s">
+      <c r="A44" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44" s="36" t="s">
         <v>329</v>
       </c>
-      <c r="C44" s="31" t="s">
+      <c r="C44" s="36" t="s">
         <v>330</v>
       </c>
-      <c r="D44" s="31" t="s">
+      <c r="D44" s="36" t="s">
         <v>331</v>
       </c>
-      <c r="H44" s="30"/>
+      <c r="H44" s="34"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="B45" s="31" t="s">
+      <c r="A45" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="36" t="s">
         <v>332</v>
       </c>
-      <c r="C45" s="31" t="s">
+      <c r="C45" s="36" t="s">
         <v>333</v>
       </c>
-      <c r="D45" s="31" t="s">
+      <c r="D45" s="36" t="s">
         <v>334</v>
       </c>
-      <c r="H45" s="30"/>
+      <c r="H45" s="34"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="B46" s="31" t="s">
+      <c r="A46" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" s="36" t="s">
         <v>335</v>
       </c>
-      <c r="C46" s="31" t="s">
+      <c r="C46" s="36" t="s">
         <v>336</v>
       </c>
-      <c r="D46" s="31" t="s">
+      <c r="D46" s="36" t="s">
         <v>337</v>
       </c>
-      <c r="H46" s="30"/>
+      <c r="H46" s="34"/>
     </row>
     <row r="1048398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -6080,7 +6034,7 @@
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.71"/>
@@ -6094,193 +6048,193 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="24.39"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="51" t="s">
+    <row r="1" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="55" t="s">
         <v>338</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="55" t="s">
         <v>339</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="55" t="s">
         <v>340</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="55" t="s">
         <v>341</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="55" t="s">
         <v>342</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="55" t="s">
         <v>343</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="G1" s="55" t="s">
         <v>344</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="H1" s="55" t="s">
         <v>345</v>
       </c>
-      <c r="I1" s="51" t="s">
+      <c r="I1" s="55" t="s">
         <v>346</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="55" t="s">
         <v>347</v>
       </c>
-      <c r="K1" s="51" t="s">
+      <c r="K1" s="55" t="s">
         <v>348</v>
       </c>
-      <c r="L1" s="52" t="s">
+      <c r="L1" s="56" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="20" t="s">
         <v>350</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="20" t="s">
         <v>351</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="20" t="s">
         <v>352</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="20" t="s">
         <v>353</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="20" t="s">
         <v>354</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="20" t="s">
         <v>355</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="20" t="s">
         <v>356</v>
       </c>
-      <c r="H2" s="18" t="n">
+      <c r="H2" s="20" t="n">
         <v>-10</v>
       </c>
-      <c r="I2" s="18" t="n">
+      <c r="I2" s="20" t="n">
         <v>100</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="20" t="s">
         <v>357</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="20" t="s">
         <v>357</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="L2" s="20" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="20" t="s">
         <v>359</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="20" t="s">
         <v>360</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="20" t="s">
         <v>361</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="57" t="s">
         <v>362</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="57" t="s">
         <v>363</v>
       </c>
-      <c r="F3" s="53" t="s">
+      <c r="F3" s="57" t="s">
         <v>364</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="20" t="s">
         <v>365</v>
       </c>
-      <c r="H3" s="18" t="n">
+      <c r="H3" s="20" t="n">
         <v>-10</v>
       </c>
-      <c r="I3" s="18" t="n">
+      <c r="I3" s="20" t="n">
         <v>100</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="J3" s="20" t="s">
         <v>357</v>
       </c>
-      <c r="K3" s="18" t="s">
+      <c r="K3" s="20" t="s">
         <v>357</v>
       </c>
-      <c r="L3" s="18" t="s">
+      <c r="L3" s="20" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="20" t="s">
         <v>367</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="20" t="s">
         <v>368</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="20" t="s">
         <v>369</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="20" t="s">
         <v>370</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="20" t="s">
         <v>371</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="20" t="s">
         <v>372</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="20" t="s">
         <v>373</v>
       </c>
-      <c r="H4" s="18" t="n">
+      <c r="H4" s="20" t="n">
         <v>-10</v>
       </c>
-      <c r="I4" s="18" t="n">
+      <c r="I4" s="20" t="n">
         <v>100</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="20" t="s">
         <v>357</v>
       </c>
-      <c r="K4" s="18" t="s">
+      <c r="K4" s="20" t="s">
         <v>357</v>
       </c>
-      <c r="L4" s="18" t="s">
+      <c r="L4" s="20" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="20" t="s">
         <v>374</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="20" t="s">
         <v>360</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="20" t="s">
         <v>375</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="20" t="s">
         <v>376</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="20" t="s">
         <v>363</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="20" t="s">
         <v>377</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="20" t="s">
         <v>378</v>
       </c>
-      <c r="H5" s="18" t="n">
+      <c r="H5" s="20" t="n">
         <v>-10</v>
       </c>
-      <c r="I5" s="18" t="n">
+      <c r="I5" s="20" t="n">
         <v>100</v>
       </c>
-      <c r="J5" s="18" t="s">
+      <c r="J5" s="20" t="s">
         <v>357</v>
       </c>
-      <c r="K5" s="18" t="s">
+      <c r="K5" s="20" t="s">
         <v>357</v>
       </c>
-      <c r="L5" s="18" t="s">
+      <c r="L5" s="20" t="s">
         <v>358</v>
       </c>
     </row>
@@ -6415,17 +6369,17 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="33.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -6466,10 +6420,10 @@
       <c r="B3" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="34" t="s">
         <v>383</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="34" t="s">
         <v>384</v>
       </c>
     </row>
@@ -6494,58 +6448,52 @@
       <c r="B5" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="34" t="s">
         <v>387</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="34" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>148</v>
+        <v>69</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="C6" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="34" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D6" s="34" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>148</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="C7" s="30" t="s">
-        <v>391</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>393</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="34" t="s">
         <v>394</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="D8" s="34" t="s">
         <v>395</v>
       </c>
     </row>
@@ -6553,7 +6501,7 @@
       <c r="A9" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="34" t="s">
         <v>396</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -6562,43 +6510,49 @@
       <c r="D9" s="1" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>227</v>
-      </c>
-      <c r="D10" s="30" t="s">
+      <c r="B10" s="34" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B11" s="30" t="s">
-        <v>400</v>
-      </c>
-      <c r="C11" s="30" t="s">
+      <c r="B11" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="C11" s="34" t="s">
+        <v>227</v>
+      </c>
+      <c r="D11" s="34" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="34" t="s">
         <v>403</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="34" t="s">
         <v>404</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -6627,10 +6581,10 @@
         <v>409</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>318</v>
+        <v>410</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6638,40 +6592,40 @@
         <v>165</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>412</v>
+        <v>318</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="1" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="34" t="s">
         <v>417</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="34" t="s">
         <v>418</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="34" t="s">
         <v>419</v>
       </c>
     </row>
@@ -6679,17 +6633,30 @@
       <c r="A18" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="34" t="s">
         <v>420</v>
       </c>
-      <c r="C18" s="54" t="s">
+      <c r="C18" s="34" t="s">
         <v>421</v>
       </c>
-      <c r="D18" s="54" t="s">
+      <c r="D18" s="34" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="1048376" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>423</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>424</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>425</v>
+      </c>
+    </row>
     <row r="1048377" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048378" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048379" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Refactor: Remove unused widgets in results section
Did 'yarn generate Survey'
Note: We don't need them anymore, because the results logic is now in the template, so we have more control.
</commit_message>
<xml_diff>
--- a/localisation/references/questionnaireLocalisation.xlsx
+++ b/localisation/references/questionnaireLocalisation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="367">
   <si>
     <t xml:space="preserve">questionName</t>
   </si>
@@ -560,99 +560,6 @@
     <t xml:space="preserve">Accessibility comparison</t>
   </si>
   <si>
-    <t xml:space="preserve">resultsByAddress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">monthlyHousingCost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">monthlyCost.housingCostMonthly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coût mensuel total du logement
-**{{housingCostMonthly}}** $</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Housing Monthly Cost
-$**{{housingCostMonthly}}**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Custom because of the label with placeholder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">monthlyCarCost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">monthlyCost.carCostMonthly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coût mensuel de la possession de véhicules (selon les données de la CAA)
-**{{carCostMonthly}}** $</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monthly cost of car possession (according to CAA data)
-$**{{carCostMonthly}}**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">monthlyTotalCost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">monthlyCost.totalCostMonthly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coût mensuel total
-**{{monthlyCost}}** $</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Monthly Cost
-$**{{monthlyCost}}**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">destinationsRouting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">routingTimeDistances</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcul de chemin vers les destinations fréquentes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Routing calculation to frequent destinations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tripMode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resultsByMode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Par mode de déplacement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">By transportation mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tripTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">travelTimeSeconds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Durée: {{minutes}} minutes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duration: {{minutes}} minutes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tripDistance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">distanceMeters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Distance: {{distance}} km</t>
-  </si>
-  <si>
     <t xml:space="preserve">conditional_name</t>
   </si>
   <si>
@@ -1239,102 +1146,6 @@
   </si>
   <si>
     <t xml:space="preserve">Delete this destination</t>
-  </si>
-  <si>
-    <t xml:space="preserve">addressGroupName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Option B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Option A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DestinationGroupName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Destination {{sequence}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FrequentDestinationTitle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frequent Destinations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RoutingResultsByMode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Résultats par mode de transport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Results by transportation mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">modeNames.walking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marche</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Walking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">modeNames.cycling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vélo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cycling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">modeNames.driving</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Driving</t>
-  </si>
-  <si>
-    <t xml:space="preserve">modeNames.transit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transport collectif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">monthlyCost.carCostMonthlyNull</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coût mensuel de la possession de véhicules (selon les données de la CAA)
--</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monthly cost of car possession (according to CAA data)
--</t>
-  </si>
-  <si>
-    <t xml:space="preserve">monthlyCost.housingCostMonthlyNull</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coût mensuel total du logement
--</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Housing Monthly Cost
--</t>
-  </si>
-  <si>
-    <t xml:space="preserve">monthlyCost.totalCostMonthlyNull</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coût mensuel total
--</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Monthly Cost
--</t>
   </si>
 </sst>
 </file>
@@ -1347,7 +1158,7 @@
     <numFmt numFmtId="166" formatCode="General"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1442,13 +1253,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1573,7 +1377,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1750,19 +1554,15 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1770,11 +1570,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1782,7 +1582,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1794,15 +1594,15 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2107,12 +1907,12 @@
   </sheetPr>
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L17" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="L13" activeCellId="0" sqref="L13"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+      <selection pane="bottomRight" activeCell="A38" activeCellId="0" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2128,7 +1928,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="10.91"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2205,7 +2005,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" s="14" customFormat="true" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="14" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
@@ -2275,7 +2075,7 @@
       <c r="XFC2" s="15"/>
       <c r="XFD2" s="15"/>
     </row>
-    <row r="3" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
         <v>30</v>
       </c>
@@ -2326,7 +2126,7 @@
       <c r="Y3" s="18"/>
       <c r="XFD3" s="19"/>
     </row>
-    <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
         <v>36</v>
       </c>
@@ -2374,7 +2174,7 @@
       <c r="Y4" s="18"/>
       <c r="XFD4" s="1"/>
     </row>
-    <row r="5" s="25" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="25" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="21" t="s">
         <v>42</v>
       </c>
@@ -2445,7 +2245,7 @@
       <c r="XFC5" s="1"/>
       <c r="XFD5" s="15"/>
     </row>
-    <row r="6" s="14" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="14" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
         <v>46</v>
       </c>
@@ -2515,7 +2315,7 @@
       <c r="XFC6" s="15"/>
       <c r="XFD6" s="26"/>
     </row>
-    <row r="7" s="18" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="18" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="27" t="s">
         <v>50</v>
       </c>
@@ -2579,7 +2379,7 @@
       <c r="XFC7" s="1"/>
       <c r="XFD7" s="1"/>
     </row>
-    <row r="8" s="18" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="18" customFormat="true" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="29" t="s">
         <v>52</v>
       </c>
@@ -2657,7 +2457,7 @@
       <c r="XFC8" s="1"/>
       <c r="XFD8" s="1"/>
     </row>
-    <row r="9" s="18" customFormat="true" ht="128.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="18" customFormat="true" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
         <v>60</v>
       </c>
@@ -2731,7 +2531,7 @@
       <c r="XFA9" s="1"/>
       <c r="XFB9" s="1"/>
       <c r="XFC9" s="1"/>
-      <c r="XFD9" s="1"/>
+      <c r="XFD9" s="0"/>
     </row>
     <row r="10" s="25" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="21" t="s">
@@ -2802,9 +2602,9 @@
       <c r="XFA10" s="1"/>
       <c r="XFB10" s="1"/>
       <c r="XFC10" s="1"/>
-      <c r="XFD10" s="1"/>
-    </row>
-    <row r="11" s="14" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="XFD10" s="0"/>
+    </row>
+    <row r="11" s="14" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
         <v>68</v>
       </c>
@@ -2872,7 +2672,7 @@
       <c r="XFA11" s="15"/>
       <c r="XFB11" s="15"/>
       <c r="XFC11" s="15"/>
-      <c r="XFD11" s="1"/>
+      <c r="XFD11" s="0"/>
     </row>
     <row r="12" s="18" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="27" t="s">
@@ -2936,9 +2736,9 @@
       <c r="XFA12" s="1"/>
       <c r="XFB12" s="1"/>
       <c r="XFC12" s="1"/>
-      <c r="XFD12" s="1"/>
-    </row>
-    <row r="13" s="18" customFormat="true" ht="204.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="XFD12" s="0"/>
+    </row>
+    <row r="13" s="18" customFormat="true" ht="137.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="27" t="s">
         <v>73</v>
       </c>
@@ -3010,9 +2810,9 @@
       <c r="XFA13" s="1"/>
       <c r="XFB13" s="1"/>
       <c r="XFC13" s="1"/>
-      <c r="XFD13" s="1"/>
-    </row>
-    <row r="14" s="18" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="XFD13" s="0"/>
+    </row>
+    <row r="14" s="18" customFormat="true" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="29" t="s">
         <v>79</v>
       </c>
@@ -3086,7 +2886,7 @@
       <c r="XFC14" s="1"/>
       <c r="XFD14" s="1"/>
     </row>
-    <row r="15" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>84</v>
       </c>
@@ -3122,7 +2922,7 @@
       </c>
       <c r="XFD15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
         <v>89</v>
       </c>
@@ -3153,7 +2953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" s="14" customFormat="true" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" s="14" customFormat="true" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
         <v>91</v>
       </c>
@@ -3223,7 +3023,7 @@
       <c r="XFC17" s="15"/>
       <c r="XFD17" s="1"/>
     </row>
-    <row r="18" s="26" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="37" t="s">
         <v>95</v>
       </c>
@@ -3246,7 +3046,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="XFD18" s="15"/>
+      <c r="XFD18" s="1"/>
     </row>
     <row r="19" s="18" customFormat="true" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="34" t="s">
@@ -3320,7 +3120,7 @@
       <c r="XFA19" s="1"/>
       <c r="XFB19" s="1"/>
       <c r="XFC19" s="1"/>
-      <c r="XFD19" s="1"/>
+      <c r="XFD19" s="0"/>
     </row>
     <row r="20" s="18" customFormat="true" ht="96.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="34" t="s">
@@ -3397,7 +3197,7 @@
       <c r="XFC20" s="1"/>
       <c r="XFD20" s="1"/>
     </row>
-    <row r="21" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="16" t="s">
         <v>105</v>
       </c>
@@ -3445,9 +3245,8 @@
       <c r="W21" s="16"/>
       <c r="X21" s="16"/>
       <c r="Y21" s="18"/>
-      <c r="XFD21" s="1"/>
-    </row>
-    <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="22" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="41" t="s">
         <v>110</v>
       </c>
@@ -3482,7 +3281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="41" t="s">
         <v>115</v>
       </c>
@@ -3518,7 +3317,6 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="XFD23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="41" t="s">
@@ -3555,7 +3353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="41" t="s">
         <v>125</v>
       </c>
@@ -3596,7 +3394,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="41" t="s">
         <v>131</v>
       </c>
@@ -3640,7 +3438,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="41" t="s">
         <v>137</v>
       </c>
@@ -3675,7 +3473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
         <v>141</v>
       </c>
@@ -3709,7 +3507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" s="25" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" s="25" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="21" t="s">
         <v>146</v>
       </c>
@@ -3778,9 +3576,9 @@
       <c r="XFA29" s="1"/>
       <c r="XFB29" s="1"/>
       <c r="XFC29" s="1"/>
-      <c r="XFD29" s="1"/>
-    </row>
-    <row r="30" s="14" customFormat="true" ht="229.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="XFD29" s="0"/>
+    </row>
+    <row r="30" s="14" customFormat="true" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
         <v>147</v>
       </c>
@@ -3848,7 +3646,7 @@
       <c r="XFA30" s="15"/>
       <c r="XFB30" s="15"/>
       <c r="XFC30" s="15"/>
-      <c r="XFD30" s="1"/>
+      <c r="XFD30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
@@ -3941,7 +3739,7 @@
       <c r="XFA32" s="1"/>
       <c r="XFB32" s="1"/>
       <c r="XFC32" s="1"/>
-      <c r="XFD32" s="1"/>
+      <c r="XFD32" s="0"/>
     </row>
     <row r="33" s="18" customFormat="true" ht="96.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="34" t="s">
@@ -4016,9 +3814,9 @@
       <c r="XFA33" s="1"/>
       <c r="XFB33" s="1"/>
       <c r="XFC33" s="1"/>
-      <c r="XFD33" s="1"/>
-    </row>
-    <row r="34" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="XFD33" s="0"/>
+    </row>
+    <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
         <v>158</v>
       </c>
@@ -4053,7 +3851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" s="25" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" s="25" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="21" t="s">
         <v>163</v>
       </c>
@@ -4122,7 +3920,7 @@
       <c r="XFA35" s="1"/>
       <c r="XFB35" s="1"/>
       <c r="XFC35" s="1"/>
-      <c r="XFD35" s="1"/>
+      <c r="XFD35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
@@ -4176,224 +3974,15 @@
         <v>170</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C38" s="40" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="40" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="F39" s="44" t="s">
-        <v>173</v>
-      </c>
-      <c r="G39" s="34" t="s">
-        <v>174</v>
-      </c>
-      <c r="H39" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="T39" s="31" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="Y39" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="120.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C40" s="40" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="F40" s="44" t="s">
-        <v>178</v>
-      </c>
-      <c r="G40" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="H40" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="T40" s="31"/>
-      <c r="Y40" s="1"/>
-    </row>
-    <row r="41" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C41" s="40" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="F41" s="44" t="s">
-        <v>182</v>
-      </c>
-      <c r="G41" s="34" t="s">
-        <v>183</v>
-      </c>
-      <c r="H41" s="34" t="s">
-        <v>184</v>
-      </c>
-      <c r="T41" s="31"/>
-      <c r="Y41" s="1"/>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C42" s="40" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="F42" s="34" t="s">
-        <v>186</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C43" s="40" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B44" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C44" s="40" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C45" s="40" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <conditionalFormatting sqref="C20:C28 C3:C4 C18 C7:C10 C1 C31">
@@ -4404,7 +3993,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11:C17 C5:C6 C19:C20 C29:C30 C2 C32:C45">
+  <conditionalFormatting sqref="C11:C17 C5:C6 C19:C20 C29:C30 C2 C32:C37">
     <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="2">
       <formula>NOT(ISERROR(SEARCH("FALSE",C2)))</formula>
     </cfRule>
@@ -4438,30 +4027,30 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="34" width="38.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="34" width="15.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="34" width="31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="45" width="20.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="44" width="20.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="34" width="19.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="34" width="12.14"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="34" width="8.59"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="46" t="s">
-        <v>200</v>
-      </c>
-      <c r="B1" s="46" t="s">
-        <v>201</v>
-      </c>
-      <c r="C1" s="46" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="45" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="47" t="s">
-        <v>202</v>
-      </c>
-      <c r="E1" s="46" t="s">
-        <v>203</v>
-      </c>
-      <c r="F1" s="46" t="s">
-        <v>204</v>
+      <c r="D1" s="46" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4469,10 +4058,10 @@
         <v>65</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="D2" s="48" t="s">
-        <v>206</v>
+        <v>176</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>177</v>
       </c>
       <c r="E2" s="34" t="n">
         <v>16</v>
@@ -4728,29 +4317,29 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="50" t="s">
-        <v>207</v>
-      </c>
-      <c r="C1" s="49" t="s">
-        <v>208</v>
-      </c>
-      <c r="D1" s="49" t="s">
-        <v>209</v>
-      </c>
-      <c r="E1" s="49" t="s">
-        <v>210</v>
-      </c>
-      <c r="F1" s="49" t="s">
-        <v>211</v>
+      <c r="B1" s="49" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>180</v>
+      </c>
+      <c r="E1" s="48" t="s">
+        <v>181</v>
+      </c>
+      <c r="F1" s="48" t="s">
+        <v>182</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="H1" s="49" t="s">
-        <v>213</v>
+        <v>183</v>
+      </c>
+      <c r="H1" s="48" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4758,23 +4347,23 @@
         <v>27</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>214</v>
+        <v>185</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>215</v>
+        <v>186</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>216</v>
-      </c>
-      <c r="E2" s="51" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F2" s="51" t="b">
+        <v>187</v>
+      </c>
+      <c r="E2" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="50" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G2" s="51" t="b">
+      <c r="G2" s="50" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4784,23 +4373,23 @@
         <v>47</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>217</v>
+        <v>188</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>219</v>
-      </c>
-      <c r="E3" s="51" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F3" s="51" t="b">
+        <v>190</v>
+      </c>
+      <c r="E3" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="50" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G3" s="51" t="b">
+      <c r="G3" s="50" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4810,23 +4399,23 @@
         <v>69</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>220</v>
+        <v>191</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>221</v>
+        <v>192</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>222</v>
-      </c>
-      <c r="E4" s="51" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F4" s="51" t="b">
+        <v>193</v>
+      </c>
+      <c r="E4" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="50" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G4" s="51" t="b">
+      <c r="G4" s="50" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4836,23 +4425,23 @@
         <v>92</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>223</v>
+        <v>194</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>224</v>
+        <v>195</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="E5" s="51" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F5" s="51" t="b">
+        <v>196</v>
+      </c>
+      <c r="E5" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="50" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G5" s="51" t="b">
+      <c r="G5" s="50" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4862,23 +4451,23 @@
         <v>148</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>226</v>
+        <v>197</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>227</v>
+        <v>198</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>228</v>
-      </c>
-      <c r="E6" s="51" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F6" s="51" t="b">
+        <v>199</v>
+      </c>
+      <c r="E6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="50" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G6" s="51" t="b">
+      <c r="G6" s="50" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4888,23 +4477,23 @@
         <v>165</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>229</v>
+        <v>200</v>
       </c>
       <c r="C7" s="34" t="s">
-        <v>230</v>
+        <v>201</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>231</v>
-      </c>
-      <c r="E7" s="51" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F7" s="51" t="b">
+        <v>202</v>
+      </c>
+      <c r="E7" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="50" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G7" s="51" t="b">
+      <c r="G7" s="50" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5111,46 +4700,46 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="52" t="s">
-        <v>232</v>
-      </c>
-      <c r="B1" s="52" t="s">
+      <c r="A1" s="51" t="s">
         <v>203</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="B1" s="51" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="52" t="s">
-        <v>233</v>
-      </c>
-      <c r="H1" s="52" t="s">
+      <c r="G1" s="51" t="s">
+        <v>204</v>
+      </c>
+      <c r="H1" s="51" t="s">
         <v>12</v>
       </c>
       <c r="I1" s="36" t="s">
-        <v>234</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="42" t="s">
-        <v>235</v>
+        <v>206</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>235</v>
+        <v>206</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>236</v>
+        <v>207</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>237</v>
+        <v>208</v>
       </c>
       <c r="E2" s="42"/>
       <c r="F2" s="42"/>
@@ -5159,16 +4748,16 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="42" t="s">
-        <v>238</v>
+        <v>209</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>238</v>
+        <v>209</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>239</v>
+        <v>210</v>
       </c>
       <c r="D3" s="42" t="s">
-        <v>240</v>
+        <v>211</v>
       </c>
       <c r="E3" s="42"/>
       <c r="F3" s="42"/>
@@ -5177,16 +4766,16 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="42" t="s">
-        <v>241</v>
+        <v>212</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>241</v>
+        <v>212</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>242</v>
+        <v>213</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>243</v>
+        <v>214</v>
       </c>
       <c r="E4" s="42"/>
       <c r="F4" s="42"/>
@@ -5195,16 +4784,16 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="42" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>241</v>
+        <v>212</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>245</v>
+        <v>216</v>
       </c>
       <c r="D5" s="42" t="s">
-        <v>246</v>
+        <v>217</v>
       </c>
       <c r="E5" s="42"/>
       <c r="F5" s="42"/>
@@ -5213,16 +4802,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="42" t="s">
-        <v>247</v>
+        <v>218</v>
       </c>
       <c r="B6" s="42" t="s">
-        <v>247</v>
+        <v>218</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="D6" s="42" t="s">
-        <v>249</v>
+        <v>220</v>
       </c>
       <c r="E6" s="42"/>
       <c r="F6" s="42"/>
@@ -5231,16 +4820,16 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="42" t="s">
-        <v>250</v>
+        <v>221</v>
       </c>
       <c r="B7" s="42" t="s">
-        <v>250</v>
+        <v>221</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>251</v>
+        <v>222</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>252</v>
+        <v>223</v>
       </c>
       <c r="E7" s="42"/>
       <c r="F7" s="42"/>
@@ -5257,7 +4846,7 @@
       <c r="E8" s="42"/>
       <c r="F8" s="42"/>
       <c r="G8" s="42" t="s">
-        <v>235</v>
+        <v>206</v>
       </c>
       <c r="H8" s="42"/>
     </row>
@@ -5271,7 +4860,7 @@
       <c r="E9" s="42"/>
       <c r="F9" s="42"/>
       <c r="G9" s="42" t="s">
-        <v>238</v>
+        <v>209</v>
       </c>
       <c r="H9" s="42"/>
     </row>
@@ -5299,13 +4888,13 @@
       <c r="E11" s="42"/>
       <c r="F11" s="42"/>
       <c r="G11" s="42" t="s">
-        <v>247</v>
+        <v>218</v>
       </c>
       <c r="H11" s="42"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="42" t="s">
-        <v>253</v>
+        <v>224</v>
       </c>
       <c r="B12" s="42"/>
       <c r="C12" s="42"/>
@@ -5313,13 +4902,13 @@
       <c r="E12" s="42"/>
       <c r="F12" s="42"/>
       <c r="G12" s="42" t="s">
-        <v>235</v>
+        <v>206</v>
       </c>
       <c r="H12" s="42"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="42" t="s">
-        <v>253</v>
+        <v>224</v>
       </c>
       <c r="B13" s="42"/>
       <c r="C13" s="42"/>
@@ -5327,13 +4916,13 @@
       <c r="E13" s="42"/>
       <c r="F13" s="42"/>
       <c r="G13" s="42" t="s">
-        <v>238</v>
+        <v>209</v>
       </c>
       <c r="H13" s="42"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="42" t="s">
-        <v>253</v>
+        <v>224</v>
       </c>
       <c r="B14" s="42"/>
       <c r="C14" s="42"/>
@@ -5341,22 +4930,22 @@
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
       <c r="G14" s="42" t="s">
-        <v>250</v>
+        <v>221</v>
       </c>
       <c r="H14" s="42"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="54" t="s">
-        <v>254</v>
+      <c r="A15" s="53" t="s">
+        <v>225</v>
       </c>
       <c r="B15" s="42" t="s">
-        <v>255</v>
+        <v>226</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="D15" s="42" t="s">
-        <v>257</v>
+        <v>228</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -5364,17 +4953,17 @@
       <c r="H15" s="42"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="54" t="s">
-        <v>254</v>
+      <c r="A16" s="53" t="s">
+        <v>225</v>
       </c>
       <c r="B16" s="42" t="s">
-        <v>258</v>
+        <v>229</v>
       </c>
       <c r="C16" s="42" t="s">
-        <v>259</v>
+        <v>230</v>
       </c>
       <c r="D16" s="42" t="s">
-        <v>260</v>
+        <v>231</v>
       </c>
       <c r="E16" s="42"/>
       <c r="F16" s="42"/>
@@ -5382,8 +4971,8 @@
       <c r="H16" s="42"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="54" t="s">
-        <v>254</v>
+      <c r="A17" s="53" t="s">
+        <v>225</v>
       </c>
       <c r="B17" s="42"/>
       <c r="C17" s="42"/>
@@ -5391,22 +4980,22 @@
       <c r="E17" s="42"/>
       <c r="F17" s="42"/>
       <c r="G17" s="42" t="s">
-        <v>250</v>
+        <v>221</v>
       </c>
       <c r="H17" s="42"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="54" t="s">
-        <v>261</v>
+      <c r="A18" s="53" t="s">
+        <v>232</v>
       </c>
       <c r="B18" s="42" t="s">
-        <v>255</v>
+        <v>226</v>
       </c>
       <c r="C18" s="42" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="D18" s="42" t="s">
-        <v>262</v>
+        <v>233</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -5414,17 +5003,17 @@
       <c r="H18" s="42"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="54" t="s">
-        <v>261</v>
+      <c r="A19" s="53" t="s">
+        <v>232</v>
       </c>
       <c r="B19" s="42" t="s">
-        <v>258</v>
+        <v>229</v>
       </c>
       <c r="C19" s="42" t="s">
-        <v>259</v>
+        <v>230</v>
       </c>
       <c r="D19" s="42" t="s">
-        <v>263</v>
+        <v>234</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -5432,17 +5021,17 @@
       <c r="H19" s="42"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="54" t="s">
-        <v>261</v>
+      <c r="A20" s="53" t="s">
+        <v>232</v>
       </c>
       <c r="B20" s="42" t="s">
-        <v>264</v>
+        <v>235</v>
       </c>
       <c r="C20" s="42" t="s">
-        <v>265</v>
+        <v>236</v>
       </c>
       <c r="D20" s="42" t="s">
-        <v>266</v>
+        <v>237</v>
       </c>
       <c r="E20" s="42"/>
       <c r="F20" s="42"/>
@@ -5450,8 +5039,8 @@
       <c r="H20" s="42"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="54" t="s">
-        <v>261</v>
+      <c r="A21" s="53" t="s">
+        <v>232</v>
       </c>
       <c r="B21" s="42"/>
       <c r="C21" s="42"/>
@@ -5459,7 +5048,7 @@
       <c r="E21" s="42"/>
       <c r="F21" s="42"/>
       <c r="G21" s="42" t="s">
-        <v>250</v>
+        <v>221</v>
       </c>
       <c r="H21" s="42"/>
     </row>
@@ -5468,13 +5057,13 @@
         <v>41</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>267</v>
+        <v>238</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>268</v>
+        <v>239</v>
       </c>
       <c r="D22" s="36" t="s">
-        <v>269</v>
+        <v>240</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5482,13 +5071,13 @@
         <v>41</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>270</v>
+        <v>241</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>271</v>
+        <v>242</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>272</v>
+        <v>243</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -5498,13 +5087,13 @@
         <v>41</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>273</v>
+        <v>244</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>274</v>
+        <v>245</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>275</v>
+        <v>246</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -5514,13 +5103,13 @@
         <v>41</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>276</v>
+        <v>247</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>277</v>
+        <v>248</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>278</v>
+        <v>249</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -5530,13 +5119,13 @@
         <v>41</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>279</v>
+        <v>250</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>280</v>
+        <v>251</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>281</v>
+        <v>252</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -5546,13 +5135,13 @@
         <v>41</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>282</v>
+        <v>253</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>283</v>
+        <v>254</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>284</v>
+        <v>255</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -5562,13 +5151,13 @@
         <v>41</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>285</v>
+        <v>256</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>286</v>
+        <v>257</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>287</v>
+        <v>258</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -5578,13 +5167,13 @@
         <v>41</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>288</v>
+        <v>259</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>289</v>
+        <v>260</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>290</v>
+        <v>261</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -5594,13 +5183,13 @@
         <v>41</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>291</v>
+        <v>262</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>292</v>
+        <v>263</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>293</v>
+        <v>264</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -5610,13 +5199,13 @@
         <v>41</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>294</v>
+        <v>265</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>295</v>
+        <v>266</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>296</v>
+        <v>267</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
@@ -5626,13 +5215,13 @@
         <v>41</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>297</v>
+        <v>268</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>298</v>
+        <v>269</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>299</v>
+        <v>270</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
@@ -5642,13 +5231,13 @@
         <v>41</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>300</v>
+        <v>271</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>301</v>
+        <v>272</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>302</v>
+        <v>273</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
@@ -5658,13 +5247,13 @@
         <v>41</v>
       </c>
       <c r="B34" s="36" t="s">
-        <v>303</v>
+        <v>274</v>
       </c>
       <c r="C34" s="36" t="s">
-        <v>304</v>
+        <v>275</v>
       </c>
       <c r="D34" s="36" t="s">
-        <v>305</v>
+        <v>276</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5672,13 +5261,13 @@
         <v>41</v>
       </c>
       <c r="B35" s="36" t="s">
-        <v>247</v>
+        <v>218</v>
       </c>
       <c r="C35" s="36" t="s">
-        <v>306</v>
+        <v>277</v>
       </c>
       <c r="D35" s="36" t="s">
-        <v>307</v>
+        <v>278</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5686,13 +5275,13 @@
         <v>41</v>
       </c>
       <c r="B36" s="36" t="s">
-        <v>308</v>
+        <v>279</v>
       </c>
       <c r="C36" s="36" t="s">
-        <v>309</v>
+        <v>280</v>
       </c>
       <c r="D36" s="36" t="s">
-        <v>310</v>
+        <v>281</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5700,13 +5289,13 @@
         <v>109</v>
       </c>
       <c r="B37" s="36" t="s">
-        <v>311</v>
+        <v>282</v>
       </c>
       <c r="C37" s="36" t="s">
-        <v>312</v>
+        <v>283</v>
       </c>
       <c r="D37" s="36" t="s">
-        <v>313</v>
+        <v>284</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5714,13 +5303,13 @@
         <v>109</v>
       </c>
       <c r="B38" s="36" t="s">
-        <v>314</v>
+        <v>285</v>
       </c>
       <c r="C38" s="36" t="s">
-        <v>315</v>
+        <v>286</v>
       </c>
       <c r="D38" s="36" t="s">
-        <v>316</v>
+        <v>287</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5728,13 +5317,13 @@
         <v>83</v>
       </c>
       <c r="B39" s="36" t="s">
-        <v>317</v>
+        <v>288</v>
       </c>
       <c r="C39" s="36" t="s">
-        <v>318</v>
+        <v>289</v>
       </c>
       <c r="D39" s="36" t="s">
-        <v>319</v>
+        <v>290</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5742,13 +5331,13 @@
         <v>83</v>
       </c>
       <c r="B40" s="36" t="s">
-        <v>320</v>
+        <v>291</v>
       </c>
       <c r="C40" s="36" t="s">
-        <v>321</v>
+        <v>292</v>
       </c>
       <c r="D40" s="36" t="s">
-        <v>322</v>
+        <v>293</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5756,13 +5345,13 @@
         <v>83</v>
       </c>
       <c r="B41" s="36" t="s">
-        <v>323</v>
+        <v>294</v>
       </c>
       <c r="C41" s="36" t="s">
-        <v>324</v>
+        <v>295</v>
       </c>
       <c r="D41" s="36" t="s">
-        <v>325</v>
+        <v>296</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5770,7 +5359,7 @@
         <v>83</v>
       </c>
       <c r="G42" s="42" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5778,13 +5367,13 @@
         <v>88</v>
       </c>
       <c r="B43" s="36" t="s">
-        <v>326</v>
+        <v>297</v>
       </c>
       <c r="C43" s="36" t="s">
-        <v>327</v>
+        <v>298</v>
       </c>
       <c r="D43" s="36" t="s">
-        <v>328</v>
+        <v>299</v>
       </c>
       <c r="H43" s="34"/>
     </row>
@@ -5793,13 +5382,13 @@
         <v>88</v>
       </c>
       <c r="B44" s="36" t="s">
-        <v>329</v>
+        <v>300</v>
       </c>
       <c r="C44" s="36" t="s">
-        <v>330</v>
+        <v>301</v>
       </c>
       <c r="D44" s="36" t="s">
-        <v>331</v>
+        <v>302</v>
       </c>
       <c r="H44" s="34"/>
     </row>
@@ -5808,13 +5397,13 @@
         <v>88</v>
       </c>
       <c r="B45" s="36" t="s">
-        <v>332</v>
+        <v>303</v>
       </c>
       <c r="C45" s="36" t="s">
-        <v>333</v>
+        <v>304</v>
       </c>
       <c r="D45" s="36" t="s">
-        <v>334</v>
+        <v>305</v>
       </c>
       <c r="H45" s="34"/>
     </row>
@@ -5823,13 +5412,13 @@
         <v>88</v>
       </c>
       <c r="B46" s="36" t="s">
-        <v>335</v>
+        <v>306</v>
       </c>
       <c r="C46" s="36" t="s">
-        <v>336</v>
+        <v>307</v>
       </c>
       <c r="D46" s="36" t="s">
-        <v>337</v>
+        <v>308</v>
       </c>
       <c r="H46" s="34"/>
     </row>
@@ -6048,65 +5637,65 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="24.39"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="55" t="s">
-        <v>338</v>
-      </c>
-      <c r="B1" s="55" t="s">
-        <v>339</v>
-      </c>
-      <c r="C1" s="55" t="s">
-        <v>340</v>
-      </c>
-      <c r="D1" s="55" t="s">
-        <v>341</v>
-      </c>
-      <c r="E1" s="55" t="s">
-        <v>342</v>
-      </c>
-      <c r="F1" s="55" t="s">
-        <v>343</v>
-      </c>
-      <c r="G1" s="55" t="s">
-        <v>344</v>
-      </c>
-      <c r="H1" s="55" t="s">
-        <v>345</v>
-      </c>
-      <c r="I1" s="55" t="s">
-        <v>346</v>
-      </c>
-      <c r="J1" s="55" t="s">
-        <v>347</v>
-      </c>
-      <c r="K1" s="55" t="s">
-        <v>348</v>
-      </c>
-      <c r="L1" s="56" t="s">
-        <v>349</v>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="54" t="s">
+        <v>309</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>310</v>
+      </c>
+      <c r="C1" s="54" t="s">
+        <v>311</v>
+      </c>
+      <c r="D1" s="54" t="s">
+        <v>312</v>
+      </c>
+      <c r="E1" s="54" t="s">
+        <v>313</v>
+      </c>
+      <c r="F1" s="54" t="s">
+        <v>314</v>
+      </c>
+      <c r="G1" s="54" t="s">
+        <v>315</v>
+      </c>
+      <c r="H1" s="54" t="s">
+        <v>316</v>
+      </c>
+      <c r="I1" s="54" t="s">
+        <v>317</v>
+      </c>
+      <c r="J1" s="54" t="s">
+        <v>318</v>
+      </c>
+      <c r="K1" s="54" t="s">
+        <v>319</v>
+      </c>
+      <c r="L1" s="55" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="20" t="s">
-        <v>350</v>
+        <v>321</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>351</v>
+        <v>322</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>352</v>
+        <v>323</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>353</v>
+        <v>324</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>354</v>
+        <v>325</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>355</v>
+        <v>326</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>356</v>
+        <v>327</v>
       </c>
       <c r="H2" s="20" t="n">
         <v>-10</v>
@@ -6115,36 +5704,36 @@
         <v>100</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>357</v>
+        <v>328</v>
       </c>
       <c r="K2" s="20" t="s">
-        <v>357</v>
+        <v>328</v>
       </c>
       <c r="L2" s="20" t="s">
-        <v>358</v>
+        <v>329</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
-        <v>359</v>
+        <v>330</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>360</v>
+        <v>331</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>361</v>
-      </c>
-      <c r="D3" s="57" t="s">
-        <v>362</v>
-      </c>
-      <c r="E3" s="57" t="s">
-        <v>363</v>
-      </c>
-      <c r="F3" s="57" t="s">
-        <v>364</v>
+        <v>332</v>
+      </c>
+      <c r="D3" s="56" t="s">
+        <v>333</v>
+      </c>
+      <c r="E3" s="56" t="s">
+        <v>334</v>
+      </c>
+      <c r="F3" s="56" t="s">
+        <v>335</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>365</v>
+        <v>336</v>
       </c>
       <c r="H3" s="20" t="n">
         <v>-10</v>
@@ -6153,36 +5742,36 @@
         <v>100</v>
       </c>
       <c r="J3" s="20" t="s">
-        <v>357</v>
+        <v>328</v>
       </c>
       <c r="K3" s="20" t="s">
-        <v>357</v>
+        <v>328</v>
       </c>
       <c r="L3" s="20" t="s">
-        <v>366</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="20" t="s">
-        <v>367</v>
+        <v>338</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>368</v>
+        <v>339</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>369</v>
+        <v>340</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>370</v>
+        <v>341</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>371</v>
+        <v>342</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>372</v>
+        <v>343</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>373</v>
+        <v>344</v>
       </c>
       <c r="H4" s="20" t="n">
         <v>-10</v>
@@ -6191,36 +5780,36 @@
         <v>100</v>
       </c>
       <c r="J4" s="20" t="s">
-        <v>357</v>
+        <v>328</v>
       </c>
       <c r="K4" s="20" t="s">
-        <v>357</v>
+        <v>328</v>
       </c>
       <c r="L4" s="20" t="s">
-        <v>358</v>
+        <v>329</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="20" t="s">
-        <v>374</v>
+        <v>345</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>360</v>
+        <v>331</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>375</v>
+        <v>346</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>376</v>
+        <v>347</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>363</v>
+        <v>334</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>377</v>
+        <v>348</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>378</v>
+        <v>349</v>
       </c>
       <c r="H5" s="20" t="n">
         <v>-10</v>
@@ -6229,13 +5818,13 @@
         <v>100</v>
       </c>
       <c r="J5" s="20" t="s">
-        <v>357</v>
+        <v>328</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>357</v>
+        <v>328</v>
       </c>
       <c r="L5" s="20" t="s">
-        <v>358</v>
+        <v>329</v>
       </c>
     </row>
     <row r="1048465" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -6368,8 +5957,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6379,7 +5968,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -6404,13 +5993,13 @@
         <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>379</v>
+        <v>350</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>380</v>
+        <v>351</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>381</v>
+        <v>352</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6418,13 +6007,13 @@
         <v>47</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>382</v>
+        <v>353</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>383</v>
+        <v>354</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>384</v>
+        <v>355</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6432,13 +6021,13 @@
         <v>69</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>379</v>
+        <v>350</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>385</v>
+        <v>356</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>386</v>
+        <v>357</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6446,13 +6035,13 @@
         <v>69</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>382</v>
+        <v>353</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>387</v>
+        <v>358</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>388</v>
+        <v>359</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6460,27 +6049,27 @@
         <v>69</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>389</v>
+        <v>360</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>390</v>
+        <v>361</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>148</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>379</v>
+        <v>350</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>392</v>
+        <v>363</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>393</v>
+        <v>364</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6488,175 +6077,30 @@
         <v>148</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>382</v>
+        <v>353</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>394</v>
+        <v>365</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B9" s="34" t="s">
-        <v>396</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B10" s="34" t="s">
-        <v>399</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>227</v>
-      </c>
-      <c r="D11" s="34" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B12" s="34" t="s">
-        <v>403</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>404</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>417</v>
-      </c>
-      <c r="C17" s="34" t="s">
-        <v>418</v>
-      </c>
-      <c r="D17" s="34" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B18" s="34" t="s">
-        <v>420</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>421</v>
-      </c>
-      <c r="D18" s="34" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B19" s="34" t="s">
-        <v>423</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>424</v>
-      </c>
-      <c r="D19" s="34" t="s">
-        <v>425</v>
-      </c>
-    </row>
+        <v>366</v>
+      </c>
+    </row>
+    <row r="1048362" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048363" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048364" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048365" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048366" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048367" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048368" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048369" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048370" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048371" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048372" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048373" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048374" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048375" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048376" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048377" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048378" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048379" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Localization: Update English and French result templates with location comparison details and cost information
Fix: #75
</commit_message>
<xml_diff>
--- a/localisation/references/questionnaireLocalisation.xlsx
+++ b/localisation/references/questionnaireLocalisation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="438">
   <si>
     <t xml:space="preserve">questionName</t>
   </si>
@@ -1146,6 +1146,239 @@
   </si>
   <si>
     <t xml:space="preserve">Delete this destination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notApplicable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locationComparison.title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comparateur de logement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Housing comparison tool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locationComparison.address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pour {{address}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For {{address}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locationComparison.defaultAddressName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logement #{{number}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">house #{{number}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locationComparison.costsTitle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coûts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Costs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locationComparison.costsMonthly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mensuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monthly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locationComparison.costsAnnual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locationComparison.costs25years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 ans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locationComparison.costsHousing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Housing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locationComparison.costsTransport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locationComparison.costsTotal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locationComparison.costsPercentageOfIncome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{percentageOfIncome}}% du revenu brut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{percentageOfIncome}}% of gross income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locationComparison.tooMuchSpendingWarning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il est à noter qu'il n'est pas recommandé de consacrer plus de 45 % de son revenu brut au logement et aux transports.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note that it is not recommended to spend more than 45% of gross income on housing and transportation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locationComparison.tooManyCarsWarning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notre modèle estime que les ménages dans cette situation possèdent {{numberOfCars}} voitures.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our model estimates that households in this situation have {{numberOfCars}} cars.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locationComparison.environmentTitle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Environnement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Environment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locationComparison.environmentPointsOfInterest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Points d'intérêt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Points of interest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locationComparison.environmentCo2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CO</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">locationComparison.environmentCo2Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{value}} tonnes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{value}} tons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locationComparison.frequentDestinationsTitle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequent Destinations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Destination fréquente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequent destination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locationComparison.frequentDestinationsFrom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De {{address}} à {{destination}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From {{address}} to {{destination}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locationComparison.destinationNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Destination #{{number}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modeNames.walking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modeNames.cycling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vélo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cycling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modeNames.driving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Driving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modeNames.transit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport collectif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transit</t>
   </si>
 </sst>
 </file>
@@ -1158,7 +1391,7 @@
     <numFmt numFmtId="166" formatCode="General"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1286,6 +1519,21 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1377,7 +1625,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1603,6 +1851,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1907,7 +2159,7 @@
   </sheetPr>
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -2531,7 +2783,7 @@
       <c r="XFA9" s="1"/>
       <c r="XFB9" s="1"/>
       <c r="XFC9" s="1"/>
-      <c r="XFD9" s="0"/>
+      <c r="XFD9" s="1"/>
     </row>
     <row r="10" s="25" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="21" t="s">
@@ -2602,7 +2854,7 @@
       <c r="XFA10" s="1"/>
       <c r="XFB10" s="1"/>
       <c r="XFC10" s="1"/>
-      <c r="XFD10" s="0"/>
+      <c r="XFD10" s="1"/>
     </row>
     <row r="11" s="14" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
@@ -2672,7 +2924,7 @@
       <c r="XFA11" s="15"/>
       <c r="XFB11" s="15"/>
       <c r="XFC11" s="15"/>
-      <c r="XFD11" s="0"/>
+      <c r="XFD11" s="1"/>
     </row>
     <row r="12" s="18" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="27" t="s">
@@ -2736,7 +2988,7 @@
       <c r="XFA12" s="1"/>
       <c r="XFB12" s="1"/>
       <c r="XFC12" s="1"/>
-      <c r="XFD12" s="0"/>
+      <c r="XFD12" s="1"/>
     </row>
     <row r="13" s="18" customFormat="true" ht="137.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="27" t="s">
@@ -2810,7 +3062,7 @@
       <c r="XFA13" s="1"/>
       <c r="XFB13" s="1"/>
       <c r="XFC13" s="1"/>
-      <c r="XFD13" s="0"/>
+      <c r="XFD13" s="1"/>
     </row>
     <row r="14" s="18" customFormat="true" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="29" t="s">
@@ -2920,7 +3172,6 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="XFD15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
@@ -2952,6 +3203,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="XFD16" s="1"/>
     </row>
     <row r="17" s="14" customFormat="true" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
@@ -3120,7 +3372,7 @@
       <c r="XFA19" s="1"/>
       <c r="XFB19" s="1"/>
       <c r="XFC19" s="1"/>
-      <c r="XFD19" s="0"/>
+      <c r="XFD19" s="1"/>
     </row>
     <row r="20" s="18" customFormat="true" ht="96.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="34" t="s">
@@ -3472,6 +3724,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="XFD27" s="1"/>
     </row>
     <row r="28" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
@@ -3506,6 +3759,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="XFD28" s="1"/>
     </row>
     <row r="29" s="25" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="21" t="s">
@@ -3576,7 +3830,7 @@
       <c r="XFA29" s="1"/>
       <c r="XFB29" s="1"/>
       <c r="XFC29" s="1"/>
-      <c r="XFD29" s="0"/>
+      <c r="XFD29" s="1"/>
     </row>
     <row r="30" s="14" customFormat="true" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
@@ -3646,7 +3900,7 @@
       <c r="XFA30" s="15"/>
       <c r="XFB30" s="15"/>
       <c r="XFC30" s="15"/>
-      <c r="XFD30" s="0"/>
+      <c r="XFD30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
@@ -3666,6 +3920,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="XFD31" s="1"/>
     </row>
     <row r="32" s="18" customFormat="true" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="34" t="s">
@@ -3739,7 +3994,7 @@
       <c r="XFA32" s="1"/>
       <c r="XFB32" s="1"/>
       <c r="XFC32" s="1"/>
-      <c r="XFD32" s="0"/>
+      <c r="XFD32" s="1"/>
     </row>
     <row r="33" s="18" customFormat="true" ht="96.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="34" t="s">
@@ -3814,7 +4069,7 @@
       <c r="XFA33" s="1"/>
       <c r="XFB33" s="1"/>
       <c r="XFC33" s="1"/>
-      <c r="XFD33" s="0"/>
+      <c r="XFD33" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
@@ -3920,7 +4175,7 @@
       <c r="XFA35" s="1"/>
       <c r="XFB35" s="1"/>
       <c r="XFC35" s="1"/>
-      <c r="XFD35" s="0"/>
+      <c r="XFD35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
@@ -5957,18 +6212,20 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="33.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.91"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -6086,21 +6343,362 @@
         <v>366</v>
       </c>
     </row>
-    <row r="1048362" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048363" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048364" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048365" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048366" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048367" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048368" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048369" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048370" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048371" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048372" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048373" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048374" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048375" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048376" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B9" s="57" t="s">
+        <v>367</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>368</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>375</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>387</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>437</v>
+      </c>
+    </row>
     <row r="1048377" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048378" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048379" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Result: Allow input of up to 10 frequent destinations.
Fix: #47
- Adjusted related logic in custom widgets to manage destination count and button visibility accordingly.
- Allow to remove and add destinations up to 10 and at least 1.
</commit_message>
<xml_diff>
--- a/localisation/references/questionnaireLocalisation.xlsx
+++ b/localisation/references/questionnaireLocalisation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -488,11 +488,11 @@
     <t xml:space="preserve">destinations</t>
   </si>
   <si>
-    <t xml:space="preserve">Veuillez entrer **deux lieux** d’où vous faites fréquemment et régulièrement un aller-retour depuis votre maison.
+    <t xml:space="preserve">Veuillez entrer jusqu’à **10 lieux** d’où vous faites fréquemment et régulièrement un aller-retour depuis votre maison.
 __Ce devraient être des endroits que vous allez visiter à partir des deux lieux entrés dans la section précédente (travail, école, …).__</t>
   </si>
   <si>
-    <t xml:space="preserve">Please enter **two locations** that you frequently and regularly travel to from your home.
+    <t xml:space="preserve">Please enter up to **10 locations** that you frequently and regularly travel to from your home.
 __These should be places that you’ll be visiting from both of the locations entered in the previous section (work, school, ...).__</t>
   </si>
   <si>
@@ -2159,12 +2159,12 @@
   </sheetPr>
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
-      <selection pane="bottomRight" activeCell="A38" activeCellId="0" sqref="A38"/>
+      <selection pane="bottomLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="bottomRight" activeCell="H30" activeCellId="0" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6212,7 +6212,7 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Results: Update income-related prompts and calculations for percentage of housing and transport costs
Fix: #5, fix: #18

- Enhanced English and French prompts in home.yaml to clarify the use of household income information.
- Implemented a new function to calculate the percentage of income spent on housing and trasnport based on user input.
- Adjusted income range values in choices.tsx to reflect updated financial brackets.
- Updated results template to conditionally display percentage of income when available.
- Get only the minimum income for the high income household.
</commit_message>
<xml_diff>
--- a/localisation/references/questionnaireLocalisation.xlsx
+++ b/localisation/references/questionnaireLocalisation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -148,10 +148,12 @@
     <t xml:space="preserve">household.income</t>
   </si>
   <si>
-    <t xml:space="preserve">**Tranche de revenu** avant impôts (brut) **du ménage**, en 2024?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What was your **household's income range** before taxes (gross income), in 2024?</t>
+    <t xml:space="preserve">**Tranche de revenu** avant impôts (brut) **du ménage**, en 2024?
+__Cette information sert à calculer le pourcentage du revenu brut consacré aux transports et au logement.__</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What was your **household's income range** before taxes (gross income), in 2024?
+__This information is used to calculate the percentage of gross income spent on transportation and housing.__</t>
   </si>
   <si>
     <t xml:space="preserve">householdIncomeChoices</t>
@@ -860,22 +862,22 @@
     <t xml:space="preserve">$100,000 to $149,999</t>
   </si>
   <si>
-    <t xml:space="preserve">150000_199999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">150 000$ à 199 999$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$150,000 to $199,999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">200000_999999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">200 000 $ et plus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$200,000 and more</t>
+    <t xml:space="preserve">150000_209999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150 000$ à 209 999$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$150,000 to $209,999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">210000_999999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">210 000$ et plus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$210,000 and more</t>
   </si>
   <si>
     <t xml:space="preserve">Je ne sais pas (notez que la précision des résultats pourrait être affectée)</t>
@@ -1244,10 +1246,10 @@
     <t xml:space="preserve">locationComparison.costsPercentageOfIncome</t>
   </si>
   <si>
-    <t xml:space="preserve">{{percentageOfIncome}}% du revenu brut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{percentageOfIncome}}% of gross income</t>
+    <t xml:space="preserve">({{percentageOfIncome}}% du revenu brut)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">({{percentageOfIncome}}% of gross income)</t>
   </si>
   <si>
     <t xml:space="preserve">locationComparison.tooMuchSpendingWarning</t>
@@ -2159,12 +2161,12 @@
   </sheetPr>
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
-      <selection pane="bottomRight" activeCell="H30" activeCellId="0" sqref="H30"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2378,7 +2380,7 @@
       <c r="Y3" s="18"/>
       <c r="XFD3" s="19"/>
     </row>
-    <row r="4" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
         <v>36</v>
       </c>
@@ -4940,8 +4942,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G42" activeCellId="0" sqref="G42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6213,7 +6215,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Results: Add accessibility panel in results section
Fix: #79
- Added an Accessibility Panel component to allow users to select locations, travel times, and modes of transport.
- Updated English and French localization files with new accessibility-related strings.
- Improved styles for the accessibility panel to ensure proper positioning and visibility above the map.
- Added minimize and expand functionality to the accessibility panel in the results section.
</commit_message>
<xml_diff>
--- a/localisation/references/questionnaireLocalisation.xlsx
+++ b/localisation/references/questionnaireLocalisation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="470">
   <si>
     <t xml:space="preserve">questionName</t>
   </si>
@@ -1291,27 +1291,7 @@
     <t xml:space="preserve">locationComparison.environmentCo2</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">CO</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2</t>
-    </r>
+    <t xml:space="preserve">CO2</t>
   </si>
   <si>
     <t xml:space="preserve">locationComparison.environmentCo2Value</t>
@@ -1381,6 +1361,102 @@
   </si>
   <si>
     <t xml:space="preserve">Transit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accessibilityPanel.title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accessibilité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accessibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accessibilityPanel.locationsTitle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accessibilityPanel.bothAddresses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les deux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accessibilityPanel.firstAddressOnly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logement #1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">House #1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accessibilityPanel.secondAddressOnly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logement #2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">House #2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accessibilityPanel.travelTimeTitle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temps de trajet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travel time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accessibilityPanel.15min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 min.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accessibilityPanel.30min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 min.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accessibilityPanel.45min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45 min.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accessibilityPanel.modeOfTransportTitle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mode de transport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mode of transport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accessibilityPanel.minimize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réduire la fenêtre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimize the panel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accessibilityPanel.expand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agrandir la fenêtre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximize the panel</t>
   </si>
 </sst>
 </file>
@@ -1393,7 +1469,7 @@
     <numFmt numFmtId="166" formatCode="General"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1523,14 +1599,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <vertAlign val="subscript"/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -4942,7 +5010,7 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
@@ -6214,8 +6282,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6699,6 +6767,174 @@
       </c>
       <c r="D33" s="2" t="s">
         <v>437</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="1048377" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Results: Refine accessibility panel attributes
- Use useMemo to avoid stale renders in template.tsx
- Enhanced the results template and custom widgets to utilize the new AccessibilityPanelAttrs type for better type safety.
- Keep color for each house in accessibility panel.
</commit_message>
<xml_diff>
--- a/localisation/references/questionnaireLocalisation.xlsx
+++ b/localisation/references/questionnaireLocalisation.xlsx
@@ -1441,13 +1441,13 @@
     <t xml:space="preserve">Mode of transport</t>
   </si>
   <si>
-    <t xml:space="preserve">accessibilityPanel.minimize</t>
+    <t xml:space="preserve">accessibilityPanel.collapse</t>
   </si>
   <si>
     <t xml:space="preserve">Réduire la fenêtre</t>
   </si>
   <si>
-    <t xml:space="preserve">Minimize the panel</t>
+    <t xml:space="preserve">Collapse the panel</t>
   </si>
   <si>
     <t xml:space="preserve">accessibilityPanel.expand</t>
@@ -1456,7 +1456,7 @@
     <t xml:space="preserve">Agrandir la fenêtre</t>
   </si>
   <si>
-    <t xml:space="preserve">Maximize the panel</t>
+    <t xml:space="preserve">Expand the panel</t>
   </si>
 </sst>
 </file>
@@ -6282,8 +6282,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B44" activeCellId="0" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6637,7 +6637,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>165</v>
       </c>

</xml_diff>

<commit_message>
Update income brackets in car ownership calculations and localization
- Adjusted income ranges in carOwnership.ts to reflect brackets from the car cost model
</commit_message>
<xml_diff>
--- a/localisation/references/questionnaireLocalisation.xlsx
+++ b/localisation/references/questionnaireLocalisation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="476">
   <si>
     <t xml:space="preserve">questionName</t>
   </si>
@@ -853,22 +853,40 @@
     <t xml:space="preserve">$90,000 to $99,999</t>
   </si>
   <si>
-    <t xml:space="preserve">100000_149999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100 000$ à 149 999$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$100,000 to $149,999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">150000_209999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">150 000$ à 209 999$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$150,000 to $209,999</t>
+    <t xml:space="preserve">100000_119999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 000$ à 119 999$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$100,000 to $119,999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">120000_149999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">120 000$ à 149 999$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$120,000 to $149,999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150000_179999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150 000$ à 179 999$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$150,000 to $179,999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">180000_209999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">180 000$ à 209 999$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$180,000 to $209,999</t>
   </si>
   <si>
     <t xml:space="preserve">210000_999999</t>
@@ -4139,7 +4157,7 @@
       <c r="XFA33" s="1"/>
       <c r="XFB33" s="1"/>
       <c r="XFC33" s="1"/>
-      <c r="XFD33" s="1"/>
+      <c r="XFD33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
@@ -4175,6 +4193,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="XFD34" s="1"/>
     </row>
     <row r="35" s="25" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="21" t="s">
@@ -4245,7 +4264,7 @@
       <c r="XFA35" s="1"/>
       <c r="XFB35" s="1"/>
       <c r="XFC35" s="1"/>
-      <c r="XFD35" s="1"/>
+      <c r="XFD35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
@@ -5010,8 +5029,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5571,50 +5590,54 @@
       <c r="A34" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="36" t="s">
+      <c r="B34" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="C34" s="36" t="s">
+      <c r="C34" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="D34" s="36" t="s">
+      <c r="D34" s="2" t="s">
         <v>276</v>
       </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="36" t="s">
-        <v>218</v>
-      </c>
-      <c r="C35" s="36" t="s">
+      <c r="B35" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="D35" s="36" t="s">
+      <c r="C35" s="2" t="s">
         <v>278</v>
       </c>
+      <c r="D35" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="36" t="s">
         <v>41</v>
       </c>
       <c r="B36" s="36" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C36" s="36" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D36" s="36" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="36" t="s">
-        <v>109</v>
+        <v>41</v>
       </c>
       <c r="B37" s="36" t="s">
-        <v>282</v>
+        <v>218</v>
       </c>
       <c r="C37" s="36" t="s">
         <v>283</v>
@@ -5623,9 +5646,9 @@
         <v>284</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="36" t="s">
-        <v>109</v>
+        <v>41</v>
       </c>
       <c r="B38" s="36" t="s">
         <v>285</v>
@@ -5639,7 +5662,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="36" t="s">
-        <v>83</v>
+        <v>109</v>
       </c>
       <c r="B39" s="36" t="s">
         <v>288</v>
@@ -5653,7 +5676,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="36" t="s">
-        <v>83</v>
+        <v>109</v>
       </c>
       <c r="B40" s="36" t="s">
         <v>291</v>
@@ -5683,39 +5706,37 @@
       <c r="A42" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="G42" s="42" t="s">
-        <v>215</v>
+      <c r="B42" s="36" t="s">
+        <v>297</v>
+      </c>
+      <c r="C42" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="D42" s="36" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="36" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B43" s="36" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C43" s="36" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="D43" s="36" t="s">
-        <v>299</v>
-      </c>
-      <c r="H43" s="34"/>
+        <v>302</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="B44" s="36" t="s">
-        <v>300</v>
-      </c>
-      <c r="C44" s="36" t="s">
-        <v>301</v>
-      </c>
-      <c r="D44" s="36" t="s">
-        <v>302</v>
-      </c>
-      <c r="H44" s="34"/>
+        <v>83</v>
+      </c>
+      <c r="G44" s="42" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="36" t="s">
@@ -5747,8 +5768,36 @@
       </c>
       <c r="H46" s="34"/>
     </row>
-    <row r="1048398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" s="36" t="s">
+        <v>309</v>
+      </c>
+      <c r="C47" s="36" t="s">
+        <v>310</v>
+      </c>
+      <c r="D47" s="36" t="s">
+        <v>311</v>
+      </c>
+      <c r="H47" s="34"/>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" s="36" t="s">
+        <v>312</v>
+      </c>
+      <c r="C48" s="36" t="s">
+        <v>313</v>
+      </c>
+      <c r="D48" s="36" t="s">
+        <v>314</v>
+      </c>
+      <c r="H48" s="34"/>
+    </row>
     <row r="1048400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5964,63 +6013,63 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="54" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="B1" s="54" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="C1" s="54" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="D1" s="54" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="E1" s="54" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="F1" s="54" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="G1" s="54" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="H1" s="54" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="I1" s="54" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="J1" s="54" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="K1" s="54" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="L1" s="55" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="20" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="H2" s="20" t="n">
         <v>-10</v>
@@ -6029,36 +6078,36 @@
         <v>100</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="K2" s="20" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="L2" s="20" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="D3" s="56" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="E3" s="56" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="F3" s="56" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="H3" s="20" t="n">
         <v>-10</v>
@@ -6067,36 +6116,36 @@
         <v>100</v>
       </c>
       <c r="J3" s="20" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="K3" s="20" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="L3" s="20" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="20" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="H4" s="20" t="n">
         <v>-10</v>
@@ -6105,36 +6154,36 @@
         <v>100</v>
       </c>
       <c r="J4" s="20" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="K4" s="20" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="L4" s="20" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="20" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="H5" s="20" t="n">
         <v>-10</v>
@@ -6143,13 +6192,13 @@
         <v>100</v>
       </c>
       <c r="J5" s="20" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="L5" s="20" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
     </row>
     <row r="1048465" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -6282,8 +6331,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B44" activeCellId="0" sqref="B44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6320,13 +6369,13 @@
         <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6334,13 +6383,13 @@
         <v>47</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6348,13 +6397,13 @@
         <v>69</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6362,13 +6411,13 @@
         <v>69</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6376,13 +6425,13 @@
         <v>69</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6390,13 +6439,13 @@
         <v>148</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6404,13 +6453,13 @@
         <v>148</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6418,13 +6467,13 @@
         <v>165</v>
       </c>
       <c r="B9" s="57" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6432,13 +6481,13 @@
         <v>165</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6446,13 +6495,13 @@
         <v>165</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6460,13 +6509,13 @@
         <v>165</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6474,13 +6523,13 @@
         <v>165</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6488,13 +6537,13 @@
         <v>165</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6502,13 +6551,13 @@
         <v>165</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6516,13 +6565,13 @@
         <v>165</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6530,13 +6579,13 @@
         <v>165</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6544,13 +6593,13 @@
         <v>165</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>394</v>
+        <v>400</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6558,13 +6607,13 @@
         <v>165</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6572,13 +6621,13 @@
         <v>165</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6586,13 +6635,13 @@
         <v>165</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>401</v>
+        <v>407</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>402</v>
+        <v>408</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>403</v>
+        <v>409</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6600,13 +6649,13 @@
         <v>165</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>405</v>
+        <v>411</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>406</v>
+        <v>412</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6614,13 +6663,13 @@
         <v>165</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>407</v>
+        <v>413</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6628,13 +6677,13 @@
         <v>165</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>410</v>
+        <v>416</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>411</v>
+        <v>417</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>412</v>
+        <v>418</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6642,13 +6691,13 @@
         <v>165</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>414</v>
+        <v>420</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>414</v>
+        <v>420</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6656,13 +6705,13 @@
         <v>165</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>416</v>
+        <v>422</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>417</v>
+        <v>423</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6670,19 +6719,19 @@
         <v>165</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>418</v>
+        <v>424</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>198</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>419</v>
+        <v>425</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>420</v>
+        <v>426</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>421</v>
+        <v>427</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6690,13 +6739,13 @@
         <v>165</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>422</v>
+        <v>428</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>423</v>
+        <v>429</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>424</v>
+        <v>430</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6704,13 +6753,13 @@
         <v>165</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6718,13 +6767,13 @@
         <v>165</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>427</v>
+        <v>433</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>428</v>
+        <v>434</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>429</v>
+        <v>435</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6732,13 +6781,13 @@
         <v>165</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>430</v>
+        <v>436</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>431</v>
+        <v>437</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>432</v>
+        <v>438</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6746,13 +6795,13 @@
         <v>165</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>433</v>
+        <v>439</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>434</v>
+        <v>440</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6760,13 +6809,13 @@
         <v>165</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>436</v>
+        <v>442</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6774,13 +6823,13 @@
         <v>165</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>439</v>
+        <v>445</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>440</v>
+        <v>446</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6788,13 +6837,13 @@
         <v>165</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>442</v>
+        <v>448</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6802,13 +6851,13 @@
         <v>165</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>444</v>
+        <v>450</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>445</v>
+        <v>451</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6816,13 +6865,13 @@
         <v>165</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>446</v>
+        <v>452</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>447</v>
+        <v>453</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>448</v>
+        <v>454</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6830,13 +6879,13 @@
         <v>165</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>449</v>
+        <v>455</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>450</v>
+        <v>456</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>451</v>
+        <v>457</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6844,13 +6893,13 @@
         <v>165</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>452</v>
+        <v>458</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>453</v>
+        <v>459</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>454</v>
+        <v>460</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6858,13 +6907,13 @@
         <v>165</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>455</v>
+        <v>461</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>456</v>
+        <v>462</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>456</v>
+        <v>462</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6872,13 +6921,13 @@
         <v>165</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>457</v>
+        <v>463</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>458</v>
+        <v>464</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>458</v>
+        <v>464</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6886,13 +6935,13 @@
         <v>165</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>459</v>
+        <v>465</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>460</v>
+        <v>466</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>460</v>
+        <v>466</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6900,13 +6949,13 @@
         <v>165</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>461</v>
+        <v>467</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>462</v>
+        <v>468</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>463</v>
+        <v>469</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6914,13 +6963,13 @@
         <v>165</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>464</v>
+        <v>470</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>465</v>
+        <v>471</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6928,13 +6977,13 @@
         <v>165</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
     </row>
     <row r="1048377" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Label: Add descriptions for location comparison
Fix: #109
- Updated styles to accommodate address name elements in the participant app.
- Modified the results template to display the new descriptions alongside address names.
</commit_message>
<xml_diff>
--- a/localisation/references/questionnaireLocalisation.xlsx
+++ b/localisation/references/questionnaireLocalisation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="482">
   <si>
     <t xml:space="preserve">questionName</t>
   </si>
@@ -1208,6 +1208,24 @@
   </si>
   <si>
     <t xml:space="preserve">Costs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locationComparison.descriptionTop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nous avons estimé le coût moyen du transport et le nombre de véhicules selon l’emplacement, la taille, le revenu et le nombre de permis du ménage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We estimated the average transportation cost and the number of vehicles based on household location, size, income, and number of driver’s licenses.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locationComparison.descriptionBottom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le nombre de véhicules estimé peut différer de la situation actuelle.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The estimated number of vehicles may differ from the current situation.</t>
   </si>
   <si>
     <t xml:space="preserve">locationComparison.costsMonthly</t>
@@ -1487,7 +1505,7 @@
     <numFmt numFmtId="166" formatCode="General"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1622,6 +1640,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1713,7 +1737,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1944,6 +1968,14 @@
     </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -4157,7 +4189,7 @@
       <c r="XFA33" s="1"/>
       <c r="XFB33" s="1"/>
       <c r="XFC33" s="1"/>
-      <c r="XFD33" s="0"/>
+      <c r="XFD33" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
@@ -4264,7 +4296,7 @@
       <c r="XFA35" s="1"/>
       <c r="XFB35" s="1"/>
       <c r="XFC35" s="1"/>
-      <c r="XFD35" s="0"/>
+      <c r="XFD35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
@@ -5029,7 +5061,7 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
@@ -6331,8 +6363,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6542,7 +6574,7 @@
       <c r="C14" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="58" t="s">
         <v>389</v>
       </c>
     </row>
@@ -6556,7 +6588,7 @@
       <c r="C15" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="58" t="s">
         <v>392</v>
       </c>
     </row>
@@ -6564,21 +6596,21 @@
       <c r="A16" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="1" t="s">
         <v>393</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="59" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>396</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -6588,11 +6620,11 @@
         <v>398</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+    <row r="18" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="34" t="s">
         <v>399</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -6613,7 +6645,7 @@
         <v>403</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6621,13 +6653,13 @@
         <v>165</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="D20" s="2" t="s">
         <v>406</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6635,12 +6667,12 @@
         <v>165</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="D21" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>409</v>
       </c>
     </row>
@@ -6693,11 +6725,11 @@
       <c r="B25" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>420</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6705,47 +6737,41 @@
         <v>165</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="C26" s="2" t="s">
         <v>422</v>
       </c>
+      <c r="C26" s="1" t="s">
+        <v>423</v>
+      </c>
       <c r="D26" s="2" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="B27" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>427</v>
+      <c r="D27" s="2" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="2" t="s">
         <v>429</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6753,13 +6779,19 @@
         <v>165</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>432</v>
+      <c r="F29" s="2" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6767,13 +6799,13 @@
         <v>165</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="D30" s="2" t="s">
         <v>435</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6781,12 +6813,12 @@
         <v>165</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="C31" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="C31" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>438</v>
       </c>
     </row>
@@ -6798,10 +6830,10 @@
         <v>439</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>295</v>
+        <v>440</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6809,13 +6841,13 @@
         <v>165</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6823,12 +6855,12 @@
         <v>165</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="D34" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>446</v>
       </c>
     </row>
@@ -6840,10 +6872,10 @@
         <v>447</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="D35" s="1" t="s">
         <v>448</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6851,13 +6883,13 @@
         <v>165</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6865,10 +6897,10 @@
         <v>165</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>453</v>
+        <v>403</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>454</v>
@@ -6913,7 +6945,7 @@
         <v>462</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6921,13 +6953,13 @@
         <v>165</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6935,13 +6967,13 @@
         <v>165</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6949,13 +6981,13 @@
         <v>165</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6963,10 +6995,10 @@
         <v>165</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>472</v>
@@ -6986,8 +7018,34 @@
         <v>475</v>
       </c>
     </row>
-    <row r="1048377" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048378" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
     <row r="1048379" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048380" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048381" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
template: show the number of predicted vehicles for each home
</commit_message>
<xml_diff>
--- a/localisation/references/questionnaireLocalisation.xlsx
+++ b/localisation/references/questionnaireLocalisation.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="485">
   <si>
     <t xml:space="preserve">questionName</t>
   </si>
@@ -1304,6 +1304,15 @@
   </si>
   <si>
     <t xml:space="preserve">Our model estimates that households in this situation have {{numberOfCars}} cars.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locationComparison.predictedVehicles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le nombre de véhicules estimé pour ce domicile est de {{predictedCarNumber}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The estimated number of vehicles for this home is {{predictedCarNumber}}</t>
   </si>
   <si>
     <t xml:space="preserve">locationComparison.environmentTitle</t>
@@ -1499,13 +1508,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;VRAI&quot;;&quot;VRAI&quot;;&quot;FAUX&quot;"/>
-    <numFmt numFmtId="166" formatCode="General"/>
-    <numFmt numFmtId="167" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1640,12 +1648,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1737,7 +1739,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="54">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1790,10 +1792,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1803,10 +1801,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1826,15 +1820,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1867,10 +1857,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1914,7 +1900,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1922,11 +1908,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1938,7 +1924,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1968,14 +1954,6 @@
     </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2287,7 +2265,7 @@
       <selection pane="bottomRight" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.29"/>
@@ -2377,7 +2355,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" s="14" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="13" customFormat="true" ht="64.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
@@ -2412,7 +2390,7 @@
       <c r="Q2" s="9"/>
       <c r="R2" s="9"/>
       <c r="S2" s="9"/>
-      <c r="T2" s="13" t="b">
+      <c r="T2" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2420,176 +2398,176 @@
       <c r="V2" s="9"/>
       <c r="W2" s="9"/>
       <c r="X2" s="9"/>
-      <c r="XEE2" s="15"/>
-      <c r="XEF2" s="15"/>
-      <c r="XEG2" s="15"/>
-      <c r="XEH2" s="15"/>
-      <c r="XEI2" s="15"/>
-      <c r="XEJ2" s="15"/>
-      <c r="XEK2" s="15"/>
-      <c r="XEL2" s="15"/>
-      <c r="XEM2" s="15"/>
-      <c r="XEN2" s="15"/>
-      <c r="XEO2" s="15"/>
-      <c r="XEP2" s="15"/>
-      <c r="XEQ2" s="15"/>
-      <c r="XER2" s="15"/>
-      <c r="XES2" s="15"/>
-      <c r="XET2" s="15"/>
-      <c r="XEU2" s="15"/>
-      <c r="XEV2" s="15"/>
-      <c r="XEW2" s="15"/>
-      <c r="XEX2" s="15"/>
-      <c r="XEY2" s="15"/>
-      <c r="XEZ2" s="15"/>
-      <c r="XFA2" s="15"/>
-      <c r="XFB2" s="15"/>
-      <c r="XFC2" s="15"/>
-      <c r="XFD2" s="15"/>
-    </row>
-    <row r="3" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="16" t="s">
+      <c r="XEE2" s="14"/>
+      <c r="XEF2" s="14"/>
+      <c r="XEG2" s="14"/>
+      <c r="XEH2" s="14"/>
+      <c r="XEI2" s="14"/>
+      <c r="XEJ2" s="14"/>
+      <c r="XEK2" s="14"/>
+      <c r="XEL2" s="14"/>
+      <c r="XEM2" s="14"/>
+      <c r="XEN2" s="14"/>
+      <c r="XEO2" s="14"/>
+      <c r="XEP2" s="14"/>
+      <c r="XEQ2" s="14"/>
+      <c r="XER2" s="14"/>
+      <c r="XES2" s="14"/>
+      <c r="XET2" s="14"/>
+      <c r="XEU2" s="14"/>
+      <c r="XEV2" s="14"/>
+      <c r="XEW2" s="14"/>
+      <c r="XEX2" s="14"/>
+      <c r="XEY2" s="14"/>
+      <c r="XEZ2" s="14"/>
+      <c r="XFA2" s="14"/>
+      <c r="XFB2" s="14"/>
+      <c r="XFC2" s="14"/>
+      <c r="XFD2" s="14"/>
+    </row>
+    <row r="3" customFormat="false" ht="89.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="17" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D3" s="16" t="s">
+      <c r="C3" s="15" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16" t="str">
+      <c r="E3" s="15"/>
+      <c r="F3" s="15" t="str">
         <f aca="false">REPLACE(A3, FIND("_", A3), 1, ".")</f>
         <v>household.size</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16" t="s">
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16" t="s">
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="17" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U3" s="16"/>
-      <c r="V3" s="16"/>
-      <c r="W3" s="16"/>
-      <c r="X3" s="16"/>
-      <c r="Y3" s="18"/>
-      <c r="XFD3" s="19"/>
-    </row>
-    <row r="4" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="16" t="s">
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="15"/>
+      <c r="Y3" s="16"/>
+      <c r="XFD3" s="17"/>
+    </row>
+    <row r="4" customFormat="false" ht="140.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="17" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D4" s="16" t="s">
+      <c r="C4" s="15" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16" t="s">
+      <c r="E4" s="15"/>
+      <c r="F4" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="20" t="s">
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="17" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16"/>
-      <c r="W4" s="16"/>
-      <c r="X4" s="16"/>
-      <c r="Y4" s="18"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="15"/>
+      <c r="Y4" s="16"/>
       <c r="XFD4" s="1"/>
     </row>
-    <row r="5" s="25" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="21" t="s">
+    <row r="5" s="22" customFormat="true" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="22" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D5" s="21" t="s">
+      <c r="C5" s="19" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D5" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="24" t="str">
+      <c r="E5" s="20"/>
+      <c r="F5" s="21" t="str">
         <f aca="false">REPLACE(A5, FIND("_", A5), 1, ".")</f>
         <v>home.save</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="22" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U5" s="23"/>
-      <c r="V5" s="23"/>
-      <c r="W5" s="23"/>
-      <c r="X5" s="23"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="19" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U5" s="20"/>
+      <c r="V5" s="20"/>
+      <c r="W5" s="20"/>
+      <c r="X5" s="20"/>
       <c r="XEE5" s="1"/>
       <c r="XEF5" s="1"/>
       <c r="XEG5" s="1"/>
@@ -2615,9 +2593,9 @@
       <c r="XFA5" s="1"/>
       <c r="XFB5" s="1"/>
       <c r="XFC5" s="1"/>
-      <c r="XFD5" s="15"/>
-    </row>
-    <row r="6" s="14" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="XFD5" s="14"/>
+    </row>
+    <row r="6" s="13" customFormat="true" ht="64.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
         <v>46</v>
       </c>
@@ -2652,7 +2630,7 @@
       <c r="Q6" s="9"/>
       <c r="R6" s="9"/>
       <c r="S6" s="9"/>
-      <c r="T6" s="13" t="b">
+      <c r="T6" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2660,70 +2638,70 @@
       <c r="V6" s="9"/>
       <c r="W6" s="9"/>
       <c r="X6" s="9"/>
-      <c r="XEE6" s="15"/>
-      <c r="XEF6" s="15"/>
-      <c r="XEG6" s="15"/>
-      <c r="XEH6" s="15"/>
-      <c r="XEI6" s="15"/>
-      <c r="XEJ6" s="15"/>
-      <c r="XEK6" s="15"/>
-      <c r="XEL6" s="15"/>
-      <c r="XEM6" s="15"/>
-      <c r="XEN6" s="15"/>
-      <c r="XEO6" s="15"/>
-      <c r="XEP6" s="15"/>
-      <c r="XEQ6" s="15"/>
-      <c r="XER6" s="15"/>
-      <c r="XES6" s="15"/>
-      <c r="XET6" s="15"/>
-      <c r="XEU6" s="15"/>
-      <c r="XEV6" s="15"/>
-      <c r="XEW6" s="15"/>
-      <c r="XEX6" s="15"/>
-      <c r="XEY6" s="15"/>
-      <c r="XEZ6" s="15"/>
-      <c r="XFA6" s="15"/>
-      <c r="XFB6" s="15"/>
-      <c r="XFC6" s="15"/>
-      <c r="XFD6" s="26"/>
-    </row>
-    <row r="7" s="18" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27" t="s">
+      <c r="XEE6" s="14"/>
+      <c r="XEF6" s="14"/>
+      <c r="XEG6" s="14"/>
+      <c r="XEH6" s="14"/>
+      <c r="XEI6" s="14"/>
+      <c r="XEJ6" s="14"/>
+      <c r="XEK6" s="14"/>
+      <c r="XEL6" s="14"/>
+      <c r="XEM6" s="14"/>
+      <c r="XEN6" s="14"/>
+      <c r="XEO6" s="14"/>
+      <c r="XEP6" s="14"/>
+      <c r="XEQ6" s="14"/>
+      <c r="XER6" s="14"/>
+      <c r="XES6" s="14"/>
+      <c r="XET6" s="14"/>
+      <c r="XEU6" s="14"/>
+      <c r="XEV6" s="14"/>
+      <c r="XEW6" s="14"/>
+      <c r="XEX6" s="14"/>
+      <c r="XEY6" s="14"/>
+      <c r="XEZ6" s="14"/>
+      <c r="XFA6" s="14"/>
+      <c r="XFB6" s="14"/>
+      <c r="XFC6" s="14"/>
+      <c r="XFD6" s="23"/>
+    </row>
+    <row r="7" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="17" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D7" s="29" t="s">
+      <c r="C7" s="15" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="30"/>
-      <c r="S7" s="30"/>
-      <c r="T7" s="31" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U7" s="30"/>
-      <c r="V7" s="30"/>
-      <c r="W7" s="30"/>
-      <c r="X7" s="30"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="27"/>
+      <c r="T7" s="28" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U7" s="27"/>
+      <c r="V7" s="27"/>
+      <c r="W7" s="27"/>
+      <c r="X7" s="27"/>
       <c r="XEE7" s="1"/>
       <c r="XEF7" s="1"/>
       <c r="XEG7" s="1"/>
@@ -2751,57 +2729,57 @@
       <c r="XFC7" s="1"/>
       <c r="XFD7" s="1"/>
     </row>
-    <row r="8" s="18" customFormat="true" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="29" t="s">
+    <row r="8" s="16" customFormat="true" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="17" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D8" s="29" t="s">
+      <c r="C8" s="15" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D8" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="G8" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="29" t="s">
+      <c r="H8" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="I8" s="29" t="s">
+      <c r="I8" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="J8" s="29" t="s">
+      <c r="J8" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="K8" s="29"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32" t="s">
+      <c r="K8" s="26"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="O8" s="32"/>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="32"/>
-      <c r="R8" s="32"/>
-      <c r="S8" s="32"/>
-      <c r="T8" s="31" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U8" s="32"/>
-      <c r="V8" s="32"/>
-      <c r="W8" s="32"/>
-      <c r="X8" s="32"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="29"/>
+      <c r="T8" s="28" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U8" s="29"/>
+      <c r="V8" s="29"/>
+      <c r="W8" s="29"/>
+      <c r="X8" s="29"/>
       <c r="XEE8" s="1"/>
       <c r="XEF8" s="1"/>
       <c r="XEG8" s="1"/>
@@ -2829,55 +2807,55 @@
       <c r="XFC8" s="1"/>
       <c r="XFD8" s="1"/>
     </row>
-    <row r="9" s="18" customFormat="true" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="29" t="s">
+    <row r="9" s="16" customFormat="true" ht="98.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="17" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D9" s="29" t="s">
+      <c r="C9" s="15" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D9" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="H9" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32" t="s">
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32" t="s">
+      <c r="N9" s="29"/>
+      <c r="O9" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="P9" s="32"/>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="32"/>
-      <c r="S9" s="32"/>
-      <c r="T9" s="31" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U9" s="32"/>
-      <c r="V9" s="32"/>
-      <c r="W9" s="32"/>
-      <c r="X9" s="32"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="28" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U9" s="29"/>
+      <c r="V9" s="29"/>
+      <c r="W9" s="29"/>
+      <c r="X9" s="29"/>
       <c r="XEE9" s="1"/>
       <c r="XEF9" s="1"/>
       <c r="XEG9" s="1"/>
@@ -2905,50 +2883,50 @@
       <c r="XFC9" s="1"/>
       <c r="XFD9" s="1"/>
     </row>
-    <row r="10" s="25" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="21" t="s">
+    <row r="10" s="22" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="17" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D10" s="29" t="s">
+      <c r="C10" s="15" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="24" t="str">
+      <c r="E10" s="20"/>
+      <c r="F10" s="21" t="str">
         <f aca="false">REPLACE(A10, FIND("_", A10), 1, ".")</f>
         <v>household.save</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="H10" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="21" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U10" s="23"/>
-      <c r="V10" s="23"/>
-      <c r="W10" s="23"/>
-      <c r="X10" s="23"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="19" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U10" s="20"/>
+      <c r="V10" s="20"/>
+      <c r="W10" s="20"/>
+      <c r="X10" s="20"/>
       <c r="XEE10" s="1"/>
       <c r="XEF10" s="1"/>
       <c r="XEG10" s="1"/>
@@ -2976,7 +2954,7 @@
       <c r="XFC10" s="1"/>
       <c r="XFD10" s="1"/>
     </row>
-    <row r="11" s="14" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" s="13" customFormat="true" ht="64.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
         <v>68</v>
       </c>
@@ -3011,7 +2989,7 @@
       <c r="Q11" s="9"/>
       <c r="R11" s="9"/>
       <c r="S11" s="9"/>
-      <c r="T11" s="13" t="b">
+      <c r="T11" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3019,70 +2997,70 @@
       <c r="V11" s="9"/>
       <c r="W11" s="9"/>
       <c r="X11" s="9"/>
-      <c r="XEE11" s="15"/>
-      <c r="XEF11" s="15"/>
-      <c r="XEG11" s="15"/>
-      <c r="XEH11" s="15"/>
-      <c r="XEI11" s="15"/>
-      <c r="XEJ11" s="15"/>
-      <c r="XEK11" s="15"/>
-      <c r="XEL11" s="15"/>
-      <c r="XEM11" s="15"/>
-      <c r="XEN11" s="15"/>
-      <c r="XEO11" s="15"/>
-      <c r="XEP11" s="15"/>
-      <c r="XEQ11" s="15"/>
-      <c r="XER11" s="15"/>
-      <c r="XES11" s="15"/>
-      <c r="XET11" s="15"/>
-      <c r="XEU11" s="15"/>
-      <c r="XEV11" s="15"/>
-      <c r="XEW11" s="15"/>
-      <c r="XEX11" s="15"/>
-      <c r="XEY11" s="15"/>
-      <c r="XEZ11" s="15"/>
-      <c r="XFA11" s="15"/>
-      <c r="XFB11" s="15"/>
-      <c r="XFC11" s="15"/>
+      <c r="XEE11" s="14"/>
+      <c r="XEF11" s="14"/>
+      <c r="XEG11" s="14"/>
+      <c r="XEH11" s="14"/>
+      <c r="XEI11" s="14"/>
+      <c r="XEJ11" s="14"/>
+      <c r="XEK11" s="14"/>
+      <c r="XEL11" s="14"/>
+      <c r="XEM11" s="14"/>
+      <c r="XEN11" s="14"/>
+      <c r="XEO11" s="14"/>
+      <c r="XEP11" s="14"/>
+      <c r="XEQ11" s="14"/>
+      <c r="XER11" s="14"/>
+      <c r="XES11" s="14"/>
+      <c r="XET11" s="14"/>
+      <c r="XEU11" s="14"/>
+      <c r="XEV11" s="14"/>
+      <c r="XEW11" s="14"/>
+      <c r="XEX11" s="14"/>
+      <c r="XEY11" s="14"/>
+      <c r="XEZ11" s="14"/>
+      <c r="XFA11" s="14"/>
+      <c r="XFB11" s="14"/>
+      <c r="XFC11" s="14"/>
       <c r="XFD11" s="1"/>
     </row>
-    <row r="12" s="18" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="27" t="s">
+    <row r="12" s="16" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="33" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D12" s="27" t="s">
+      <c r="C12" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D12" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="30"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="30"/>
-      <c r="R12" s="30"/>
-      <c r="S12" s="30"/>
-      <c r="T12" s="31" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U12" s="30"/>
-      <c r="V12" s="30"/>
-      <c r="W12" s="30"/>
-      <c r="X12" s="30"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27"/>
+      <c r="Q12" s="27"/>
+      <c r="R12" s="27"/>
+      <c r="S12" s="27"/>
+      <c r="T12" s="28" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U12" s="27"/>
+      <c r="V12" s="27"/>
+      <c r="W12" s="27"/>
+      <c r="X12" s="27"/>
       <c r="XEE12" s="1"/>
       <c r="XEF12" s="1"/>
       <c r="XEG12" s="1"/>
@@ -3110,53 +3088,53 @@
       <c r="XFC12" s="1"/>
       <c r="XFD12" s="1"/>
     </row>
-    <row r="13" s="18" customFormat="true" ht="137.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="27" t="s">
+    <row r="13" s="16" customFormat="true" ht="142.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="33" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D13" s="27" t="s">
+      <c r="C13" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D13" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="29" t="s">
+      <c r="E13" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="F13" s="30" t="s">
+      <c r="F13" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="G13" s="29" t="s">
+      <c r="G13" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="H13" s="29" t="s">
+      <c r="H13" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="35" t="s">
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="O13" s="30"/>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="30"/>
-      <c r="R13" s="30"/>
-      <c r="S13" s="30"/>
-      <c r="T13" s="31" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U13" s="30"/>
-      <c r="V13" s="30"/>
-      <c r="W13" s="30"/>
-      <c r="X13" s="30"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="27"/>
+      <c r="Q13" s="27"/>
+      <c r="R13" s="27"/>
+      <c r="S13" s="27"/>
+      <c r="T13" s="28" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U13" s="27"/>
+      <c r="V13" s="27"/>
+      <c r="W13" s="27"/>
+      <c r="X13" s="27"/>
       <c r="XEE13" s="1"/>
       <c r="XEF13" s="1"/>
       <c r="XEG13" s="1"/>
@@ -3184,53 +3162,53 @@
       <c r="XFC13" s="1"/>
       <c r="XFD13" s="1"/>
     </row>
-    <row r="14" s="18" customFormat="true" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="29" t="s">
+    <row r="14" s="16" customFormat="true" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="33" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D14" s="29" t="s">
+      <c r="C14" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D14" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="E14" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="F14" s="32" t="s">
+      <c r="F14" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="G14" s="29" t="s">
+      <c r="G14" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="H14" s="29" t="s">
+      <c r="H14" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="32"/>
-      <c r="N14" s="32"/>
-      <c r="O14" s="20" t="s">
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="32"/>
-      <c r="S14" s="32"/>
-      <c r="T14" s="31" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U14" s="32"/>
-      <c r="V14" s="32"/>
-      <c r="W14" s="32"/>
-      <c r="X14" s="32"/>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="29"/>
+      <c r="R14" s="29"/>
+      <c r="S14" s="29"/>
+      <c r="T14" s="28" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U14" s="29"/>
+      <c r="V14" s="29"/>
+      <c r="W14" s="29"/>
+      <c r="X14" s="29"/>
       <c r="XEE14" s="1"/>
       <c r="XEF14" s="1"/>
       <c r="XEG14" s="1"/>
@@ -3262,70 +3240,70 @@
       <c r="A15" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="33" t="b">
+      <c r="C15" s="26" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="29" t="s">
+      <c r="E15" s="26" t="s">
         <v>72</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G15" s="29" t="s">
+      <c r="G15" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="H15" s="29" t="s">
+      <c r="H15" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="M15" s="34"/>
-      <c r="O15" s="36" t="s">
+      <c r="M15" s="30"/>
+      <c r="O15" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="T15" s="31" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T15" s="28" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="33" t="b">
+      <c r="C16" s="26" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E16" s="29"/>
+      <c r="E16" s="26"/>
       <c r="F16" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G16" s="21" t="s">
+      <c r="G16" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="H16" s="21" t="s">
+      <c r="H16" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="M16" s="34"/>
-      <c r="O16" s="36"/>
-      <c r="T16" s="31" t="n">
+      <c r="M16" s="30"/>
+      <c r="O16" s="32"/>
+      <c r="T16" s="28" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="XFD16" s="1"/>
     </row>
-    <row r="17" s="14" customFormat="true" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" s="13" customFormat="true" ht="140.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
         <v>91</v>
       </c>
@@ -3360,7 +3338,7 @@
       <c r="Q17" s="9"/>
       <c r="R17" s="9"/>
       <c r="S17" s="9"/>
-      <c r="T17" s="13" t="b">
+      <c r="T17" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3368,105 +3346,105 @@
       <c r="V17" s="9"/>
       <c r="W17" s="9"/>
       <c r="X17" s="9"/>
-      <c r="XEE17" s="15"/>
-      <c r="XEF17" s="15"/>
-      <c r="XEG17" s="15"/>
-      <c r="XEH17" s="15"/>
-      <c r="XEI17" s="15"/>
-      <c r="XEJ17" s="15"/>
-      <c r="XEK17" s="15"/>
-      <c r="XEL17" s="15"/>
-      <c r="XEM17" s="15"/>
-      <c r="XEN17" s="15"/>
-      <c r="XEO17" s="15"/>
-      <c r="XEP17" s="15"/>
-      <c r="XEQ17" s="15"/>
-      <c r="XER17" s="15"/>
-      <c r="XES17" s="15"/>
-      <c r="XET17" s="15"/>
-      <c r="XEU17" s="15"/>
-      <c r="XEV17" s="15"/>
-      <c r="XEW17" s="15"/>
-      <c r="XEX17" s="15"/>
-      <c r="XEY17" s="15"/>
-      <c r="XEZ17" s="15"/>
-      <c r="XFA17" s="15"/>
-      <c r="XFB17" s="15"/>
-      <c r="XFC17" s="15"/>
+      <c r="XEE17" s="14"/>
+      <c r="XEF17" s="14"/>
+      <c r="XEG17" s="14"/>
+      <c r="XEH17" s="14"/>
+      <c r="XEI17" s="14"/>
+      <c r="XEJ17" s="14"/>
+      <c r="XEK17" s="14"/>
+      <c r="XEL17" s="14"/>
+      <c r="XEM17" s="14"/>
+      <c r="XEN17" s="14"/>
+      <c r="XEO17" s="14"/>
+      <c r="XEP17" s="14"/>
+      <c r="XEQ17" s="14"/>
+      <c r="XER17" s="14"/>
+      <c r="XES17" s="14"/>
+      <c r="XET17" s="14"/>
+      <c r="XEU17" s="14"/>
+      <c r="XEV17" s="14"/>
+      <c r="XEW17" s="14"/>
+      <c r="XEX17" s="14"/>
+      <c r="XEY17" s="14"/>
+      <c r="XEZ17" s="14"/>
+      <c r="XFA17" s="14"/>
+      <c r="XFB17" s="14"/>
+      <c r="XFC17" s="14"/>
       <c r="XFD17" s="1"/>
     </row>
-    <row r="18" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="37" t="s">
+    <row r="18" s="23" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="38" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D18" s="37" t="s">
+      <c r="C18" s="34" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D18" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="M18" s="37"/>
-      <c r="O18" s="37"/>
-      <c r="T18" s="38" t="n">
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="M18" s="33"/>
+      <c r="O18" s="33"/>
+      <c r="T18" s="34" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="XFD18" s="1"/>
     </row>
-    <row r="19" s="18" customFormat="true" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="34" t="s">
+    <row r="19" s="16" customFormat="true" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="40" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D19" s="16" t="s">
+      <c r="C19" s="36" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D19" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="F19" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="H19" s="16" t="s">
+      <c r="H19" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="35"/>
-      <c r="N19" s="35" t="s">
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="O19" s="35"/>
-      <c r="P19" s="35"/>
-      <c r="Q19" s="35"/>
-      <c r="R19" s="35"/>
-      <c r="S19" s="35"/>
-      <c r="T19" s="16" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U19" s="35"/>
-      <c r="V19" s="35"/>
-      <c r="W19" s="35"/>
-      <c r="X19" s="35"/>
+      <c r="O19" s="31"/>
+      <c r="P19" s="31"/>
+      <c r="Q19" s="31"/>
+      <c r="R19" s="31"/>
+      <c r="S19" s="31"/>
+      <c r="T19" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U19" s="31"/>
+      <c r="V19" s="31"/>
+      <c r="W19" s="31"/>
+      <c r="X19" s="31"/>
       <c r="XEE19" s="1"/>
       <c r="XEF19" s="1"/>
       <c r="XEG19" s="1"/>
@@ -3494,52 +3472,52 @@
       <c r="XFC19" s="1"/>
       <c r="XFD19" s="1"/>
     </row>
-    <row r="20" s="18" customFormat="true" ht="96.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="34" t="s">
+    <row r="20" s="16" customFormat="true" ht="96.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="40" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D20" s="16" t="s">
+      <c r="C20" s="36" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D20" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="F20" s="34" t="s">
+      <c r="F20" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="G20" s="34" t="s">
+      <c r="G20" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="H20" s="34" t="s">
+      <c r="H20" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="35"/>
-      <c r="M20" s="35"/>
-      <c r="N20" s="35"/>
-      <c r="O20" s="35"/>
-      <c r="P20" s="35"/>
-      <c r="Q20" s="35"/>
-      <c r="R20" s="35"/>
-      <c r="S20" s="35"/>
-      <c r="T20" s="16" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U20" s="35"/>
-      <c r="V20" s="35"/>
-      <c r="W20" s="35"/>
-      <c r="X20" s="35"/>
-      <c r="Y20" s="18" t="s">
+      <c r="I20" s="35"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="31"/>
+      <c r="P20" s="31"/>
+      <c r="Q20" s="31"/>
+      <c r="R20" s="31"/>
+      <c r="S20" s="31"/>
+      <c r="T20" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U20" s="31"/>
+      <c r="V20" s="31"/>
+      <c r="W20" s="31"/>
+      <c r="X20" s="31"/>
+      <c r="Y20" s="16" t="s">
         <v>104</v>
       </c>
       <c r="XEE20" s="1"/>
@@ -3569,196 +3547,196 @@
       <c r="XFC20" s="1"/>
       <c r="XFD20" s="1"/>
     </row>
-    <row r="21" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="16" t="s">
+    <row r="21" customFormat="false" ht="51.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="17" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D21" s="16" t="s">
+      <c r="C21" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D21" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="G21" s="16" t="s">
+      <c r="G21" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="H21" s="16" t="s">
+      <c r="H21" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="20" t="s">
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="16"/>
-      <c r="S21" s="16"/>
-      <c r="T21" s="16" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U21" s="16"/>
-      <c r="V21" s="16"/>
-      <c r="W21" s="16"/>
-      <c r="X21" s="16"/>
-      <c r="Y21" s="18"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
+      <c r="T21" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U21" s="15"/>
+      <c r="V21" s="15"/>
+      <c r="W21" s="15"/>
+      <c r="X21" s="15"/>
+      <c r="Y21" s="16"/>
     </row>
     <row r="22" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="17" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D22" s="16" t="s">
+      <c r="C22" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D22" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="F22" s="16" t="s">
+      <c r="F22" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="G22" s="29" t="s">
+      <c r="G22" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="H22" s="29" t="s">
+      <c r="H22" s="26" t="s">
         <v>113</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="O22" s="41"/>
-      <c r="T22" s="31" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="41" t="s">
+      <c r="O22" s="37"/>
+      <c r="T22" s="28" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="17" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D23" s="16" t="s">
+      <c r="C23" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D23" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="E23" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="F23" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="G23" s="29" t="s">
+      <c r="G23" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="H23" s="29" t="s">
+      <c r="H23" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="M23" s="34" t="s">
+      <c r="M23" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="O23" s="42" t="s">
+      <c r="O23" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="T23" s="31" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="41" t="s">
+      <c r="T23" s="28" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="37" t="s">
         <v>120</v>
       </c>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="17" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D24" s="16" t="s">
+      <c r="C24" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D24" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E24" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="F24" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="G24" s="29" t="s">
+      <c r="G24" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="H24" s="29" t="s">
+      <c r="H24" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="M24" s="34" t="s">
+      <c r="M24" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="O24" s="42"/>
-      <c r="T24" s="31" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="41" t="s">
+      <c r="O24" s="38"/>
+      <c r="T24" s="28" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="39.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="17" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D25" s="16" t="s">
+      <c r="C25" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D25" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="F25" s="16" t="s">
+      <c r="F25" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="G25" s="29" t="s">
+      <c r="G25" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="H25" s="29" t="s">
+      <c r="H25" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="M25" s="34" t="s">
+      <c r="M25" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="N25" s="16" t="s">
+      <c r="N25" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="O25" s="42"/>
-      <c r="T25" s="31" t="n">
+      <c r="O25" s="38"/>
+      <c r="T25" s="28" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3766,40 +3744,40 @@
         <v>130</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="41" t="s">
+    <row r="26" customFormat="false" ht="33.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="17" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D26" s="16" t="s">
+      <c r="C26" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D26" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="E26" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="F26" s="16" t="s">
+      <c r="F26" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="G26" s="29" t="s">
+      <c r="G26" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="H26" s="29" t="s">
+      <c r="H26" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="K26" s="16"/>
-      <c r="M26" s="34" t="s">
+      <c r="K26" s="15"/>
+      <c r="M26" s="30" t="s">
         <v>124</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="T26" s="31" t="n">
+      <c r="T26" s="28" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3810,121 +3788,121 @@
         <v>136</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="41" t="s">
+    <row r="27" customFormat="false" ht="33.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="17" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D27" s="16" t="s">
+      <c r="C27" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D27" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="G27" s="29" t="s">
+      <c r="G27" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="H27" s="29" t="s">
+      <c r="H27" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="K27" s="16"/>
-      <c r="M27" s="34" t="s">
+      <c r="K27" s="15"/>
+      <c r="M27" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="T27" s="31" t="n">
+      <c r="T27" s="28" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="XFD27" s="1"/>
     </row>
-    <row r="28" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="33.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="17" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D28" s="16" t="s">
+      <c r="C28" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D28" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E28" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="F28" s="16" t="s">
+      <c r="F28" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="G28" s="29" t="s">
+      <c r="G28" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="H28" s="29" t="s">
+      <c r="H28" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="M28" s="34" t="s">
+      <c r="M28" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="T28" s="31" t="n">
+      <c r="T28" s="28" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="XFD28" s="1"/>
     </row>
-    <row r="29" s="25" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="21" t="s">
+    <row r="29" s="22" customFormat="true" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="22" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D29" s="21" t="s">
+      <c r="C29" s="19" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D29" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E29" s="23"/>
-      <c r="F29" s="24" t="str">
+      <c r="E29" s="20"/>
+      <c r="F29" s="21" t="str">
         <f aca="false">REPLACE(A29, FIND("_", A29), 1, ".")</f>
         <v>addresses.save</v>
       </c>
-      <c r="G29" s="21" t="s">
+      <c r="G29" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="H29" s="21" t="s">
+      <c r="H29" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="21"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="23"/>
-      <c r="Q29" s="23"/>
-      <c r="R29" s="23"/>
-      <c r="S29" s="23"/>
-      <c r="T29" s="21" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U29" s="23"/>
-      <c r="V29" s="23"/>
-      <c r="W29" s="23"/>
-      <c r="X29" s="23"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="20"/>
+      <c r="P29" s="20"/>
+      <c r="Q29" s="20"/>
+      <c r="R29" s="20"/>
+      <c r="S29" s="20"/>
+      <c r="T29" s="19" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U29" s="20"/>
+      <c r="V29" s="20"/>
+      <c r="W29" s="20"/>
+      <c r="X29" s="20"/>
       <c r="XEE29" s="1"/>
       <c r="XEF29" s="1"/>
       <c r="XEG29" s="1"/>
@@ -3952,14 +3930,14 @@
       <c r="XFC29" s="1"/>
       <c r="XFD29" s="1"/>
     </row>
-    <row r="30" s="14" customFormat="true" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" s="13" customFormat="true" ht="178.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="40" t="n">
+      <c r="C30" s="36" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3987,7 +3965,7 @@
       <c r="Q30" s="9"/>
       <c r="R30" s="9"/>
       <c r="S30" s="9"/>
-      <c r="T30" s="13" t="b">
+      <c r="T30" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3995,100 +3973,100 @@
       <c r="V30" s="9"/>
       <c r="W30" s="9"/>
       <c r="X30" s="9"/>
-      <c r="XEE30" s="15"/>
-      <c r="XEF30" s="15"/>
-      <c r="XEG30" s="15"/>
-      <c r="XEH30" s="15"/>
-      <c r="XEI30" s="15"/>
-      <c r="XEJ30" s="15"/>
-      <c r="XEK30" s="15"/>
-      <c r="XEL30" s="15"/>
-      <c r="XEM30" s="15"/>
-      <c r="XEN30" s="15"/>
-      <c r="XEO30" s="15"/>
-      <c r="XEP30" s="15"/>
-      <c r="XEQ30" s="15"/>
-      <c r="XER30" s="15"/>
-      <c r="XES30" s="15"/>
-      <c r="XET30" s="15"/>
-      <c r="XEU30" s="15"/>
-      <c r="XEV30" s="15"/>
-      <c r="XEW30" s="15"/>
-      <c r="XEX30" s="15"/>
-      <c r="XEY30" s="15"/>
-      <c r="XEZ30" s="15"/>
-      <c r="XFA30" s="15"/>
-      <c r="XFB30" s="15"/>
-      <c r="XFC30" s="15"/>
+      <c r="XEE30" s="14"/>
+      <c r="XEF30" s="14"/>
+      <c r="XEG30" s="14"/>
+      <c r="XEH30" s="14"/>
+      <c r="XEI30" s="14"/>
+      <c r="XEJ30" s="14"/>
+      <c r="XEK30" s="14"/>
+      <c r="XEL30" s="14"/>
+      <c r="XEM30" s="14"/>
+      <c r="XEN30" s="14"/>
+      <c r="XEO30" s="14"/>
+      <c r="XEP30" s="14"/>
+      <c r="XEQ30" s="14"/>
+      <c r="XER30" s="14"/>
+      <c r="XES30" s="14"/>
+      <c r="XET30" s="14"/>
+      <c r="XEU30" s="14"/>
+      <c r="XEV30" s="14"/>
+      <c r="XEW30" s="14"/>
+      <c r="XEX30" s="14"/>
+      <c r="XEY30" s="14"/>
+      <c r="XEZ30" s="14"/>
+      <c r="XFA30" s="14"/>
+      <c r="XFB30" s="14"/>
+      <c r="XFC30" s="14"/>
       <c r="XFD30" s="1"/>
     </row>
-    <row r="31" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="17" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D31" s="34" t="s">
+      <c r="C31" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D31" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="T31" s="16" t="n">
+      <c r="T31" s="15" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="XFD31" s="1"/>
     </row>
-    <row r="32" s="18" customFormat="true" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="34" t="s">
+    <row r="32" s="16" customFormat="true" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="30" t="s">
         <v>152</v>
       </c>
-      <c r="B32" s="39" t="s">
+      <c r="B32" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="C32" s="40" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D32" s="16" t="s">
+      <c r="C32" s="36" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D32" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="E32" s="16" t="s">
+      <c r="E32" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="F32" s="16" t="s">
+      <c r="F32" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="G32" s="16" t="s">
+      <c r="G32" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="H32" s="16" t="s">
+      <c r="H32" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="I32" s="39"/>
-      <c r="J32" s="39"/>
-      <c r="K32" s="39"/>
-      <c r="L32" s="35"/>
-      <c r="M32" s="35"/>
-      <c r="N32" s="35" t="s">
+      <c r="I32" s="35"/>
+      <c r="J32" s="35"/>
+      <c r="K32" s="35"/>
+      <c r="L32" s="31"/>
+      <c r="M32" s="31"/>
+      <c r="N32" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="O32" s="35"/>
-      <c r="P32" s="35"/>
-      <c r="Q32" s="35"/>
-      <c r="R32" s="35"/>
-      <c r="S32" s="35"/>
-      <c r="T32" s="16" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U32" s="35"/>
-      <c r="V32" s="35"/>
-      <c r="W32" s="35"/>
-      <c r="X32" s="35"/>
+      <c r="O32" s="31"/>
+      <c r="P32" s="31"/>
+      <c r="Q32" s="31"/>
+      <c r="R32" s="31"/>
+      <c r="S32" s="31"/>
+      <c r="T32" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U32" s="31"/>
+      <c r="V32" s="31"/>
+      <c r="W32" s="31"/>
+      <c r="X32" s="31"/>
       <c r="XEE32" s="1"/>
       <c r="XEF32" s="1"/>
       <c r="XEG32" s="1"/>
@@ -4116,52 +4094,52 @@
       <c r="XFC32" s="1"/>
       <c r="XFD32" s="1"/>
     </row>
-    <row r="33" s="18" customFormat="true" ht="96.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="34" t="s">
+    <row r="33" s="16" customFormat="true" ht="96.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="B33" s="39" t="s">
+      <c r="B33" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="40" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D33" s="16" t="s">
+      <c r="C33" s="36" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D33" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="E33" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="F33" s="34" t="s">
+      <c r="F33" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="G33" s="34" t="s">
+      <c r="G33" s="30" t="s">
         <v>156</v>
       </c>
-      <c r="H33" s="34" t="s">
+      <c r="H33" s="30" t="s">
         <v>157</v>
       </c>
-      <c r="I33" s="39"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="39"/>
-      <c r="L33" s="35"/>
-      <c r="M33" s="35"/>
-      <c r="N33" s="35"/>
-      <c r="O33" s="35"/>
-      <c r="P33" s="32"/>
-      <c r="Q33" s="32"/>
-      <c r="R33" s="32"/>
-      <c r="S33" s="32"/>
-      <c r="T33" s="16" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U33" s="32"/>
-      <c r="V33" s="32"/>
-      <c r="W33" s="32"/>
-      <c r="X33" s="32"/>
-      <c r="Y33" s="18" t="s">
+      <c r="I33" s="35"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="35"/>
+      <c r="L33" s="31"/>
+      <c r="M33" s="31"/>
+      <c r="N33" s="31"/>
+      <c r="O33" s="31"/>
+      <c r="P33" s="29"/>
+      <c r="Q33" s="29"/>
+      <c r="R33" s="29"/>
+      <c r="S33" s="29"/>
+      <c r="T33" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U33" s="29"/>
+      <c r="V33" s="29"/>
+      <c r="W33" s="29"/>
+      <c r="X33" s="29"/>
+      <c r="Y33" s="16" t="s">
         <v>104</v>
       </c>
       <c r="XEE33" s="1"/>
@@ -4191,86 +4169,86 @@
       <c r="XFC33" s="1"/>
       <c r="XFD33" s="1"/>
     </row>
-    <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="39.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B34" s="29" t="s">
+      <c r="B34" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="43" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D34" s="16" t="s">
+      <c r="C34" s="39" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D34" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="E34" s="16" t="s">
+      <c r="E34" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="F34" s="16" t="s">
+      <c r="F34" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="G34" s="29" t="s">
+      <c r="G34" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="H34" s="29" t="s">
+      <c r="H34" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="K34" s="16" t="s">
+      <c r="K34" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="M34" s="34"/>
-      <c r="T34" s="16" t="n">
+      <c r="M34" s="30"/>
+      <c r="T34" s="15" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="XFD34" s="1"/>
     </row>
-    <row r="35" s="25" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="21" t="s">
+    <row r="35" s="22" customFormat="true" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="22" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D35" s="16" t="s">
+      <c r="C35" s="19" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D35" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="24" t="str">
+      <c r="E35" s="20"/>
+      <c r="F35" s="21" t="str">
         <f aca="false">REPLACE(A35, FIND("_", A35), 1, ".")</f>
         <v>destinations.save</v>
       </c>
-      <c r="G35" s="21" t="s">
+      <c r="G35" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="H35" s="21" t="s">
+      <c r="H35" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="21"/>
-      <c r="L35" s="23"/>
-      <c r="M35" s="23"/>
-      <c r="N35" s="23"/>
-      <c r="O35" s="23"/>
-      <c r="P35" s="23"/>
-      <c r="Q35" s="23"/>
-      <c r="R35" s="23"/>
-      <c r="S35" s="23"/>
-      <c r="T35" s="21" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U35" s="23"/>
-      <c r="V35" s="23"/>
-      <c r="W35" s="23"/>
-      <c r="X35" s="23"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="20"/>
+      <c r="M35" s="20"/>
+      <c r="N35" s="20"/>
+      <c r="O35" s="20"/>
+      <c r="P35" s="20"/>
+      <c r="Q35" s="20"/>
+      <c r="R35" s="20"/>
+      <c r="S35" s="20"/>
+      <c r="T35" s="19" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U35" s="20"/>
+      <c r="V35" s="20"/>
+      <c r="W35" s="20"/>
+      <c r="X35" s="20"/>
       <c r="XEE35" s="1"/>
       <c r="XEF35" s="1"/>
       <c r="XEG35" s="1"/>
@@ -4298,21 +4276,21 @@
       <c r="XFC35" s="1"/>
       <c r="XFD35" s="1"/>
     </row>
-    <row r="36" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="40" t="n">
+      <c r="C36" s="36" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="F36" s="16" t="s">
+      <c r="F36" s="15" t="s">
         <v>164</v>
       </c>
       <c r="G36" s="2" t="s">
@@ -4321,19 +4299,19 @@
       <c r="H36" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="T36" s="16" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T36" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
         <v>168</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="40" t="n">
+      <c r="C37" s="36" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4398,48 +4376,48 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="34" width="38.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="34" width="15.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="34" width="31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="44" width="20.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="34" width="19.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="34" width="12.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="34" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="38.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="15.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="30" width="31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="40" width="20.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="30" width="19.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="30" width="12.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="30" width="8.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="41" t="s">
         <v>171</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="41" t="s">
         <v>172</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="42" t="s">
         <v>173</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="41" t="s">
         <v>174</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="41" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="34" t="s">
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="30" t="s">
         <v>176</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="43" t="s">
         <v>177</v>
       </c>
-      <c r="E2" s="34" t="n">
+      <c r="E2" s="30" t="n">
         <v>16</v>
       </c>
     </row>
@@ -4680,196 +4658,196 @@
       <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="34" width="10.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="34" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="34" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="34" width="12.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="34" width="10.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="34" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="34" width="15.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="34" width="10.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="10.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="30" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="30" width="12.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="30" width="10.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="30" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="30" width="15.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="30" width="10.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="45" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="44" t="s">
         <v>180</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="44" t="s">
         <v>181</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="44" t="s">
         <v>182</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="44" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="34" t="s">
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="30" t="s">
         <v>186</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="30" t="s">
         <v>187</v>
       </c>
-      <c r="E2" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F2" s="50" t="b">
+      <c r="E2" s="46" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="46" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G2" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="34" t="s">
+      <c r="G2" s="46" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="30" t="s">
         <v>189</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="30" t="s">
         <v>190</v>
       </c>
-      <c r="E3" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F3" s="50" t="b">
+      <c r="E3" s="46" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="46" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G3" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="34" t="s">
+      <c r="G3" s="46" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="30" t="s">
         <v>191</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="30" t="s">
         <v>192</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="30" t="s">
         <v>193</v>
       </c>
-      <c r="E4" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F4" s="50" t="b">
+      <c r="E4" s="46" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="46" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G4" s="50" t="b">
+      <c r="G4" s="46" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="30" t="s">
         <v>194</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="30" t="s">
         <v>195</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="30" t="s">
         <v>196</v>
       </c>
-      <c r="E5" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F5" s="50" t="b">
+      <c r="E5" s="46" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="46" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G5" s="50" t="b">
+      <c r="G5" s="46" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="30" t="s">
         <v>197</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="30" t="s">
         <v>198</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="30" t="s">
         <v>199</v>
       </c>
-      <c r="E6" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F6" s="50" t="b">
+      <c r="E6" s="46" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="46" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G6" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="34" t="s">
+      <c r="G6" s="46" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="30" t="s">
         <v>201</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="30" t="s">
         <v>202</v>
       </c>
-      <c r="E7" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F7" s="50" t="b">
+      <c r="E7" s="46" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="46" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G7" s="50" t="b">
+      <c r="G7" s="46" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5065,385 +5043,385 @@
       <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="36" width="29.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="36" width="19.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="36" width="30.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="36" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="36" width="24.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="36" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="29.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="32" width="19.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="32" width="30.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="32" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="32" width="24.29"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="32" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="47" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="47" t="s">
         <v>174</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="G1" s="47" t="s">
         <v>204</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="H1" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="32" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="38" t="s">
         <v>207</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="38" t="s">
         <v>209</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="38" t="s">
         <v>209</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="38" t="s">
         <v>211</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="38" t="s">
         <v>212</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="38" t="s">
         <v>212</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="38" t="s">
         <v>214</v>
       </c>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="38" t="s">
         <v>212</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="38" t="s">
         <v>217</v>
       </c>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="38" t="s">
         <v>218</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="38" t="s">
         <v>218</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="38" t="s">
         <v>219</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="38" t="s">
         <v>220</v>
       </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="38" t="s">
         <v>221</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="38" t="s">
         <v>221</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="38" t="s">
         <v>223</v>
       </c>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42" t="s">
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="H8" s="42"/>
+      <c r="H8" s="38"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42" t="s">
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38" t="s">
         <v>209</v>
       </c>
-      <c r="H9" s="42"/>
+      <c r="H9" s="38"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42" t="s">
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="H10" s="42"/>
+      <c r="H10" s="38"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42" t="s">
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38" t="s">
         <v>218</v>
       </c>
-      <c r="H11" s="42"/>
+      <c r="H11" s="38"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="38" t="s">
         <v>224</v>
       </c>
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42" t="s">
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="H12" s="42"/>
+      <c r="H12" s="38"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="38" t="s">
         <v>224</v>
       </c>
-      <c r="B13" s="42"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42" t="s">
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38" t="s">
         <v>209</v>
       </c>
-      <c r="H13" s="42"/>
+      <c r="H13" s="38"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="38" t="s">
         <v>224</v>
       </c>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42" t="s">
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38" t="s">
         <v>221</v>
       </c>
-      <c r="H14" s="42"/>
+      <c r="H14" s="38"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="53" t="s">
+      <c r="A15" s="49" t="s">
         <v>225</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="38" t="s">
         <v>226</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="38" t="s">
         <v>227</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="53" t="s">
+      <c r="A16" s="49" t="s">
         <v>225</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="38" t="s">
         <v>229</v>
       </c>
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="53" t="s">
+      <c r="A17" s="49" t="s">
         <v>225</v>
       </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42" t="s">
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38" t="s">
         <v>221</v>
       </c>
-      <c r="H17" s="42"/>
+      <c r="H17" s="38"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="53" t="s">
+      <c r="A18" s="49" t="s">
         <v>232</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="38" t="s">
         <v>226</v>
       </c>
-      <c r="C18" s="42" t="s">
+      <c r="C18" s="38" t="s">
         <v>227</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="38" t="s">
         <v>233</v>
       </c>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="53" t="s">
+      <c r="A19" s="49" t="s">
         <v>232</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="38" t="s">
         <v>229</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="D19" s="42" t="s">
+      <c r="D19" s="38" t="s">
         <v>234</v>
       </c>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="53" t="s">
+      <c r="A20" s="49" t="s">
         <v>232</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="38" t="s">
         <v>235</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="38" t="s">
         <v>236</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="53" t="s">
+      <c r="A21" s="49" t="s">
         <v>232</v>
       </c>
-      <c r="B21" s="42"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42" t="s">
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38" t="s">
         <v>221</v>
       </c>
-      <c r="H21" s="42"/>
+      <c r="H21" s="38"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="32" t="s">
         <v>238</v>
       </c>
-      <c r="C22" s="36" t="s">
+      <c r="C22" s="32" t="s">
         <v>239</v>
       </c>
-      <c r="D22" s="36" t="s">
+      <c r="D22" s="32" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="32" t="s">
         <v>41</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -5459,7 +5437,7 @@
       <c r="F23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="36" t="s">
+      <c r="A24" s="32" t="s">
         <v>41</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -5475,7 +5453,7 @@
       <c r="F24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="32" t="s">
         <v>41</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -5491,7 +5469,7 @@
       <c r="F25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="36" t="s">
+      <c r="A26" s="32" t="s">
         <v>41</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -5507,7 +5485,7 @@
       <c r="F26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="32" t="s">
         <v>41</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -5523,7 +5501,7 @@
       <c r="F27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="32" t="s">
         <v>41</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -5539,7 +5517,7 @@
       <c r="F28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="36" t="s">
+      <c r="A29" s="32" t="s">
         <v>41</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -5555,7 +5533,7 @@
       <c r="F29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="36" t="s">
+      <c r="A30" s="32" t="s">
         <v>41</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -5571,7 +5549,7 @@
       <c r="F30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="36" t="s">
+      <c r="A31" s="32" t="s">
         <v>41</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -5587,7 +5565,7 @@
       <c r="F31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="32" t="s">
         <v>41</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -5603,7 +5581,7 @@
       <c r="F32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="36" t="s">
+      <c r="A33" s="32" t="s">
         <v>41</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -5619,7 +5597,7 @@
       <c r="F33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="36" t="s">
+      <c r="A34" s="32" t="s">
         <v>41</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -5635,7 +5613,7 @@
       <c r="F34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="36" t="s">
+      <c r="A35" s="32" t="s">
         <v>41</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -5651,184 +5629,184 @@
       <c r="F35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="36" t="s">
+      <c r="B36" s="32" t="s">
         <v>280</v>
       </c>
-      <c r="C36" s="36" t="s">
+      <c r="C36" s="32" t="s">
         <v>281</v>
       </c>
-      <c r="D36" s="36" t="s">
+      <c r="D36" s="32" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="36" t="s">
+      <c r="A37" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="36" t="s">
+      <c r="B37" s="32" t="s">
         <v>218</v>
       </c>
-      <c r="C37" s="36" t="s">
+      <c r="C37" s="32" t="s">
         <v>283</v>
       </c>
-      <c r="D37" s="36" t="s">
+      <c r="D37" s="32" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="36" t="s">
+      <c r="A38" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="36" t="s">
+      <c r="B38" s="32" t="s">
         <v>285</v>
       </c>
-      <c r="C38" s="36" t="s">
+      <c r="C38" s="32" t="s">
         <v>286</v>
       </c>
-      <c r="D38" s="36" t="s">
+      <c r="D38" s="32" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="36" t="s">
+      <c r="A39" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="B39" s="36" t="s">
+      <c r="B39" s="32" t="s">
         <v>288</v>
       </c>
-      <c r="C39" s="36" t="s">
+      <c r="C39" s="32" t="s">
         <v>289</v>
       </c>
-      <c r="D39" s="36" t="s">
+      <c r="D39" s="32" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="36" t="s">
+      <c r="A40" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="B40" s="36" t="s">
+      <c r="B40" s="32" t="s">
         <v>291</v>
       </c>
-      <c r="C40" s="36" t="s">
+      <c r="C40" s="32" t="s">
         <v>292</v>
       </c>
-      <c r="D40" s="36" t="s">
+      <c r="D40" s="32" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="36" t="s">
+      <c r="A41" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="B41" s="36" t="s">
+      <c r="B41" s="32" t="s">
         <v>294</v>
       </c>
-      <c r="C41" s="36" t="s">
+      <c r="C41" s="32" t="s">
         <v>295</v>
       </c>
-      <c r="D41" s="36" t="s">
+      <c r="D41" s="32" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="36" t="s">
+      <c r="A42" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="B42" s="36" t="s">
+      <c r="B42" s="32" t="s">
         <v>297</v>
       </c>
-      <c r="C42" s="36" t="s">
+      <c r="C42" s="32" t="s">
         <v>298</v>
       </c>
-      <c r="D42" s="36" t="s">
+      <c r="D42" s="32" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="36" t="s">
+      <c r="A43" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="36" t="s">
+      <c r="B43" s="32" t="s">
         <v>300</v>
       </c>
-      <c r="C43" s="36" t="s">
+      <c r="C43" s="32" t="s">
         <v>301</v>
       </c>
-      <c r="D43" s="36" t="s">
+      <c r="D43" s="32" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="36" t="s">
+      <c r="A44" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="G44" s="42" t="s">
+      <c r="G44" s="38" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="36" t="s">
+      <c r="A45" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="36" t="s">
+      <c r="B45" s="32" t="s">
         <v>303</v>
       </c>
-      <c r="C45" s="36" t="s">
+      <c r="C45" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="D45" s="36" t="s">
+      <c r="D45" s="32" t="s">
         <v>305</v>
       </c>
-      <c r="H45" s="34"/>
+      <c r="H45" s="30"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="36" t="s">
+      <c r="A46" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="B46" s="36" t="s">
+      <c r="B46" s="32" t="s">
         <v>306</v>
       </c>
-      <c r="C46" s="36" t="s">
+      <c r="C46" s="32" t="s">
         <v>307</v>
       </c>
-      <c r="D46" s="36" t="s">
+      <c r="D46" s="32" t="s">
         <v>308</v>
       </c>
-      <c r="H46" s="34"/>
+      <c r="H46" s="30"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="36" t="s">
+      <c r="A47" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="B47" s="36" t="s">
+      <c r="B47" s="32" t="s">
         <v>309</v>
       </c>
-      <c r="C47" s="36" t="s">
+      <c r="C47" s="32" t="s">
         <v>310</v>
       </c>
-      <c r="D47" s="36" t="s">
+      <c r="D47" s="32" t="s">
         <v>311</v>
       </c>
-      <c r="H47" s="34"/>
+      <c r="H47" s="30"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="36" t="s">
+      <c r="A48" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="B48" s="36" t="s">
+      <c r="B48" s="32" t="s">
         <v>312</v>
       </c>
-      <c r="C48" s="36" t="s">
+      <c r="C48" s="32" t="s">
         <v>313</v>
       </c>
-      <c r="D48" s="36" t="s">
+      <c r="D48" s="32" t="s">
         <v>314</v>
       </c>
-      <c r="H48" s="34"/>
+      <c r="H48" s="30"/>
     </row>
     <row r="1048400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -6029,7 +6007,7 @@
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.71"/>
@@ -6044,192 +6022,192 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="50" t="s">
         <v>315</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="50" t="s">
         <v>316</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="50" t="s">
         <v>317</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="50" t="s">
         <v>318</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="50" t="s">
         <v>319</v>
       </c>
-      <c r="F1" s="54" t="s">
+      <c r="F1" s="50" t="s">
         <v>320</v>
       </c>
-      <c r="G1" s="54" t="s">
+      <c r="G1" s="50" t="s">
         <v>321</v>
       </c>
-      <c r="H1" s="54" t="s">
+      <c r="H1" s="50" t="s">
         <v>322</v>
       </c>
-      <c r="I1" s="54" t="s">
+      <c r="I1" s="50" t="s">
         <v>323</v>
       </c>
-      <c r="J1" s="54" t="s">
+      <c r="J1" s="50" t="s">
         <v>324</v>
       </c>
-      <c r="K1" s="54" t="s">
+      <c r="K1" s="50" t="s">
         <v>325</v>
       </c>
-      <c r="L1" s="55" t="s">
+      <c r="L1" s="51" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="18" t="s">
         <v>327</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="18" t="s">
         <v>328</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="18" t="s">
         <v>329</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="18" t="s">
         <v>330</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="18" t="s">
         <v>331</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="18" t="s">
         <v>332</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="18" t="s">
         <v>333</v>
       </c>
-      <c r="H2" s="20" t="n">
+      <c r="H2" s="18" t="n">
         <v>-10</v>
       </c>
-      <c r="I2" s="20" t="n">
+      <c r="I2" s="18" t="n">
         <v>100</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="18" t="s">
         <v>334</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="18" t="s">
         <v>334</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="18" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="18" t="s">
         <v>336</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="18" t="s">
         <v>337</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="18" t="s">
         <v>338</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="52" t="s">
         <v>339</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="52" t="s">
         <v>340</v>
       </c>
-      <c r="F3" s="56" t="s">
+      <c r="F3" s="52" t="s">
         <v>341</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="18" t="s">
         <v>342</v>
       </c>
-      <c r="H3" s="20" t="n">
+      <c r="H3" s="18" t="n">
         <v>-10</v>
       </c>
-      <c r="I3" s="20" t="n">
+      <c r="I3" s="18" t="n">
         <v>100</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="18" t="s">
         <v>334</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="18" t="s">
         <v>334</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="18" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="18" t="s">
         <v>344</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="18" t="s">
         <v>345</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="18" t="s">
         <v>346</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="18" t="s">
         <v>347</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="18" t="s">
         <v>348</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="18" t="s">
         <v>349</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="18" t="s">
         <v>350</v>
       </c>
-      <c r="H4" s="20" t="n">
+      <c r="H4" s="18" t="n">
         <v>-10</v>
       </c>
-      <c r="I4" s="20" t="n">
+      <c r="I4" s="18" t="n">
         <v>100</v>
       </c>
-      <c r="J4" s="20" t="s">
+      <c r="J4" s="18" t="s">
         <v>334</v>
       </c>
-      <c r="K4" s="20" t="s">
+      <c r="K4" s="18" t="s">
         <v>334</v>
       </c>
-      <c r="L4" s="20" t="s">
+      <c r="L4" s="18" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>351</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="18" t="s">
         <v>337</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="18" t="s">
         <v>352</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="18" t="s">
         <v>353</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="18" t="s">
         <v>340</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="18" t="s">
         <v>354</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="18" t="s">
         <v>355</v>
       </c>
-      <c r="H5" s="20" t="n">
+      <c r="H5" s="18" t="n">
         <v>-10</v>
       </c>
-      <c r="I5" s="20" t="n">
+      <c r="I5" s="18" t="n">
         <v>100</v>
       </c>
-      <c r="J5" s="20" t="s">
+      <c r="J5" s="18" t="s">
         <v>334</v>
       </c>
-      <c r="K5" s="20" t="s">
+      <c r="K5" s="18" t="s">
         <v>334</v>
       </c>
-      <c r="L5" s="20" t="s">
+      <c r="L5" s="18" t="s">
         <v>335</v>
       </c>
     </row>
@@ -6363,11 +6341,11 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="33.83"/>
@@ -6410,17 +6388,17 @@
         <v>358</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="30" t="s">
         <v>360</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="30" t="s">
         <v>361</v>
       </c>
     </row>
@@ -6438,31 +6416,31 @@
         <v>363</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="30" t="s">
         <v>364</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="30" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="30" t="s">
         <v>367</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="30" t="s">
         <v>368</v>
       </c>
     </row>
@@ -6480,31 +6458,31 @@
         <v>370</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>148</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="30" t="s">
         <v>371</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="30" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="53" t="s">
         <v>373</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="30" t="s">
         <v>374</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D9" s="30" t="s">
         <v>374</v>
       </c>
     </row>
@@ -6536,11 +6514,11 @@
         <v>380</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="30" t="s">
         <v>381</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -6574,7 +6552,7 @@
       <c r="C14" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="D14" s="58" t="s">
+      <c r="D14" s="2" t="s">
         <v>389</v>
       </c>
     </row>
@@ -6588,11 +6566,11 @@
       <c r="C15" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="D15" s="58" t="s">
+      <c r="D15" s="2" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
         <v>165</v>
       </c>
@@ -6602,7 +6580,7 @@
       <c r="C16" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="D16" s="59" t="s">
+      <c r="D16" s="30" t="s">
         <v>395</v>
       </c>
     </row>
@@ -6620,11 +6598,11 @@
         <v>398</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="30" t="s">
         <v>399</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -6753,11 +6731,11 @@
       <c r="B27" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>426</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6765,10 +6743,10 @@
         <v>165</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>429</v>
@@ -6778,20 +6756,14 @@
       <c r="A29" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D29" s="1" t="s">
+      <c r="C29" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>432</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6799,12 +6771,18 @@
         <v>165</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="E30" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="F30" s="2" t="s">
         <v>436</v>
       </c>
     </row>
@@ -6815,11 +6793,11 @@
       <c r="B31" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="1" t="s">
         <v>438</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6827,12 +6805,12 @@
         <v>165</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="C32" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="C32" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>441</v>
       </c>
     </row>
@@ -6858,10 +6836,10 @@
         <v>445</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>295</v>
+        <v>446</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6869,10 +6847,10 @@
         <v>165</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>448</v>
+        <v>295</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>449</v>
@@ -6888,7 +6866,7 @@
       <c r="C36" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="2" t="s">
         <v>452</v>
       </c>
     </row>
@@ -6900,10 +6878,10 @@
         <v>453</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>403</v>
+        <v>454</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6911,10 +6889,10 @@
         <v>165</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>456</v>
+        <v>403</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>457</v>
@@ -6973,7 +6951,7 @@
         <v>468</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6981,13 +6959,13 @@
         <v>165</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6995,13 +6973,13 @@
         <v>165</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7009,10 +6987,10 @@
         <v>165</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>475</v>
@@ -7046,7 +7024,20 @@
         <v>481</v>
       </c>
     </row>
-    <row r="1048379" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>484</v>
+      </c>
+    </row>
     <row r="1048380" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048381" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048382" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>